<commit_message>
Clean & Load Data of Customer_List Table
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E126B0-3504-499A-8880-D702B74E8C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01E805A-0F41-4750-8CE2-5D9DFA5D0841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="3" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
   <sheets>
     <sheet name="Data &amp; Purpose" sheetId="1" r:id="rId1"/>
     <sheet name="Plan BI Pages" sheetId="4" r:id="rId2"/>
     <sheet name="Before &amp; After Column" sheetId="2" r:id="rId3"/>
-    <sheet name="Data Transformation" sheetId="3" r:id="rId4"/>
+    <sheet name="Data Cleaning" sheetId="3" r:id="rId4"/>
+    <sheet name="Data-Transformation-Wrangling" sheetId="5" r:id="rId5"/>
+    <sheet name="Story Telling" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="83">
   <si>
     <t>Load Order</t>
   </si>
@@ -175,13 +177,124 @@
   </si>
   <si>
     <t>Map-based analysis of orders, customers, sellers</t>
+  </si>
+  <si>
+    <t>Sr. No</t>
+  </si>
+  <si>
+    <t>Column Name</t>
+  </si>
+  <si>
+    <t>Column Description</t>
+  </si>
+  <si>
+    <t>Customer_Trx_ID</t>
+  </si>
+  <si>
+    <t>Unique customer transaction</t>
+  </si>
+  <si>
+    <t>Subscriber_ID</t>
+  </si>
+  <si>
+    <t>Unique subscriber ID</t>
+  </si>
+  <si>
+    <t>Subscribe_Date</t>
+  </si>
+  <si>
+    <t>Customer subscription date</t>
+  </si>
+  <si>
+    <t>First_Order_Date</t>
+  </si>
+  <si>
+    <t>Date of first order</t>
+  </si>
+  <si>
+    <t>Customer_Postal_Code</t>
+  </si>
+  <si>
+    <t>Postal code of customer</t>
+  </si>
+  <si>
+    <t>Customer_City</t>
+  </si>
+  <si>
+    <t>Customer city</t>
+  </si>
+  <si>
+    <t>Customer_Country</t>
+  </si>
+  <si>
+    <t>Customer country</t>
+  </si>
+  <si>
+    <t>Customer_Country_Code</t>
+  </si>
+  <si>
+    <t>Country ISO code</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Customer age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Customer gender</t>
+  </si>
+  <si>
+    <t>Sr. No.</t>
+  </si>
+  <si>
+    <t>Applied Steps</t>
+  </si>
+  <si>
+    <t>Rows Before</t>
+  </si>
+  <si>
+    <t>Rows After</t>
+  </si>
+  <si>
+    <t>Effect (Rows)</t>
+  </si>
+  <si>
+    <t>Col Before</t>
+  </si>
+  <si>
+    <t>Col After</t>
+  </si>
+  <si>
+    <t>Effect (Columns)</t>
+  </si>
+  <si>
+    <t>Load CSV File</t>
+  </si>
+  <si>
+    <t>Customer_List</t>
+  </si>
+  <si>
+    <t>Remove Errors</t>
+  </si>
+  <si>
+    <t>Remove Blank Rows</t>
+  </si>
+  <si>
+    <t>Remove Duplicates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remvoe Duplicates </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,8 +325,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,6 +362,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -286,6 +437,30 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -763,7 +938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D5AE18-0AB2-4473-9365-BAFCC77B8CAC}">
   <dimension ref="B4:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -880,11 +1055,444 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035EC863-7662-4F46-A1E6-DDC33702C1E8}">
+  <dimension ref="C4:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="28.109375" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="51" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C7" s="5">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C8" s="5">
+        <v>4</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C9" s="5">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C10" s="5">
+        <v>6</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C11" s="5">
+        <v>7</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C12" s="5">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C13" s="5">
+        <v>9</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C14" s="5">
+        <v>10</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05F3B95-CD15-4EA0-ACD4-4067EC5DC14D}">
+  <dimension ref="B2:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" customWidth="1"/>
+    <col min="8" max="8" width="24.109375" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="11" max="11" width="33.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="C2" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="13">
+        <v>0</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>102727</v>
+      </c>
+      <c r="G5">
+        <v>102727</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="13">
+        <v>1</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f>G5</f>
+        <v>102727</v>
+      </c>
+      <c r="G6">
+        <v>102727</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="13">
+        <v>2</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <f>G6</f>
+        <v>102727</v>
+      </c>
+      <c r="G7">
+        <v>102727</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="13">
+        <v>3</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <f>G7</f>
+        <v>102727</v>
+      </c>
+      <c r="G8">
+        <v>102727</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="13">
+        <v>4</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <f>G8</f>
+        <v>102727</v>
+      </c>
+      <c r="G9">
+        <v>99442</v>
+      </c>
+      <c r="H9">
+        <f>F9-G9</f>
+        <v>3285</v>
+      </c>
+      <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="13">
+        <v>5</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <f>G9</f>
+        <v>99442</v>
+      </c>
+      <c r="G10">
+        <v>99441</v>
+      </c>
+      <c r="H10">
+        <f>F10-G10</f>
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="13">
+        <v>6</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <f>G10</f>
+        <v>99441</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="13">
+        <v>7</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="E12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="13">
+        <v>8</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="E13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="13">
+        <v>9</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="E14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="13">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7DB601-2E61-4816-8642-3B30D49A003A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -892,13 +1500,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05F3B95-CD15-4EA0-ACD4-4067EC5DC14D}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD85EE9-7333-4E1C-BE00-8EC167B0E968}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>

<commit_message>
Add 2 more table 1.Geolocations & 2.Order_Items
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01E805A-0F41-4750-8CE2-5D9DFA5D0841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E1DC09-A743-4962-8665-57A02AC2EB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="3" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="109">
   <si>
     <t>Load Order</t>
   </si>
@@ -288,6 +288,84 @@
   </si>
   <si>
     <t xml:space="preserve">Remvoe Duplicates </t>
+  </si>
+  <si>
+    <t>Remove Top Row</t>
+  </si>
+  <si>
+    <t>Use / Description</t>
+  </si>
+  <si>
+    <t>Geo_Postal_Code</t>
+  </si>
+  <si>
+    <t>Represents the postal or ZIP code of the location (e.g., NL-5211). Useful for mapping or grouping areas.</t>
+  </si>
+  <si>
+    <t>Geo_Lat</t>
+  </si>
+  <si>
+    <t>Latitude coordinate of the location. Used for geographic visualization or map plotting.</t>
+  </si>
+  <si>
+    <t>Geo_Lon</t>
+  </si>
+  <si>
+    <t>Longitude coordinate of the location. Used along with latitude for exact location plotting on maps.</t>
+  </si>
+  <si>
+    <t>Geolocation_City</t>
+  </si>
+  <si>
+    <t>Name of the city corresponding to the postal code. Useful for regional-level analysis.</t>
+  </si>
+  <si>
+    <t>Geo_Country</t>
+  </si>
+  <si>
+    <t>Name of the country. Helps in country-wise comparison and filtering.</t>
+  </si>
+  <si>
+    <t>Order_ID</t>
+  </si>
+  <si>
+    <t>Unique identifier for each customer order. Helps in tracking and linking order details across tables.</t>
+  </si>
+  <si>
+    <t>Order_Item_ID</t>
+  </si>
+  <si>
+    <t>Indicates the item number within a specific order (useful when an order has multiple products).</t>
+  </si>
+  <si>
+    <t>Product_ID</t>
+  </si>
+  <si>
+    <t>Unique identifier for the product being sold. Used to link with the Product details table.</t>
+  </si>
+  <si>
+    <t>Seller_ID</t>
+  </si>
+  <si>
+    <t>Unique identifier for the seller or vendor fulfilling the order. Useful for seller-level performance analysis.</t>
+  </si>
+  <si>
+    <t>Shipping_Limit_Date</t>
+  </si>
+  <si>
+    <t>The latest date and time by which the seller must ship the product. Useful for logistics and SLA tracking.</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>The selling price of the product (excluding shipping). Used to calculate revenue and profitability.</t>
+  </si>
+  <si>
+    <t>Freight_Value</t>
+  </si>
+  <si>
+    <t>Shipping or delivery cost charged for the order. Used to analyze logistics costs and profit margins.</t>
   </si>
 </sst>
 </file>
@@ -334,7 +412,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,12 +440,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -441,26 +513,28 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1055,151 +1129,327 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035EC863-7662-4F46-A1E6-DDC33702C1E8}">
-  <dimension ref="C4:E14"/>
+  <dimension ref="B3:E43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.109375" customWidth="1"/>
     <col min="4" max="4" width="26.6640625" customWidth="1"/>
     <col min="5" max="5" width="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C4" s="6" t="s">
+    <row r="3" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B3" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="16" t="s">
         <v>49</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="16" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C7" s="5">
         <v>3</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="16" t="s">
         <v>53</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="5">
         <v>4</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="16" t="s">
         <v>55</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C9" s="5">
         <v>5</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="16" t="s">
         <v>57</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C10" s="5">
         <v>6</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="16" t="s">
         <v>59</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C11" s="5">
         <v>7</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="16" t="s">
         <v>61</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C12" s="5">
         <v>8</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="16" t="s">
         <v>63</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C13" s="5">
         <v>9</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="16" t="s">
         <v>65</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C14" s="5">
         <v>10</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="16" t="s">
         <v>67</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>68</v>
       </c>
     </row>
+    <row r="19" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B19" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C21" s="5">
+        <v>1</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C22" s="5">
+        <v>2</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C23" s="5">
+        <v>3</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C24" s="5">
+        <v>4</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C25" s="5">
+        <v>5</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B30" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C32" s="5">
+        <v>1</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C33" s="5">
+        <v>2</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C34" s="5">
+        <v>3</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C35" s="5">
+        <v>4</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C36" s="5">
+        <v>5</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C37" s="5">
+        <v>6</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C38" s="5">
+        <v>7</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B43" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05F3B95-CD15-4EA0-ACD4-4067EC5DC14D}">
-  <dimension ref="B2:K15"/>
+  <dimension ref="B2:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1217,271 +1467,640 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="13">
-        <v>0</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="11">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="E5" s="14">
+        <v>0</v>
+      </c>
+      <c r="F5" s="14">
         <v>102727</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="14">
         <v>102727</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
+      <c r="H5" s="14">
+        <v>0</v>
+      </c>
+      <c r="I5" s="14">
         <v>10</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="14">
         <v>10</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="13">
+      <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="14">
         <v>1</v>
       </c>
-      <c r="F6">
-        <f>G5</f>
+      <c r="F6" s="14">
+        <f t="shared" ref="F6:F11" si="0">G5</f>
         <v>102727</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="14">
         <v>102727</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
+      <c r="H6" s="14">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14">
         <v>10</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="14">
         <v>10</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="13">
+      <c r="B7" s="11">
         <v>2</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="14">
         <v>2</v>
       </c>
-      <c r="F7">
-        <f>G6</f>
+      <c r="F7" s="14">
+        <f t="shared" si="0"/>
         <v>102727</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="14">
         <v>102727</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
+      <c r="H7" s="14">
+        <v>0</v>
+      </c>
+      <c r="I7" s="14">
         <v>10</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="14">
         <v>10</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="13">
+      <c r="B8" s="11">
         <v>3</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="14">
         <v>3</v>
       </c>
-      <c r="F8">
-        <f>G7</f>
+      <c r="F8" s="14">
+        <f t="shared" si="0"/>
         <v>102727</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="14">
         <v>102727</v>
       </c>
-      <c r="I8">
+      <c r="H8" s="14"/>
+      <c r="I8" s="14">
         <v>10</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="14">
         <v>10</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="13">
+      <c r="B9" s="11">
         <v>4</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>82</v>
       </c>
       <c r="D9" t="s">
         <v>49</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="14">
         <v>4</v>
       </c>
-      <c r="F9">
-        <f>G8</f>
+      <c r="F9" s="14">
+        <f t="shared" si="0"/>
         <v>102727</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="14">
         <v>99442</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="14">
         <f>F9-G9</f>
         <v>3285</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="14">
         <v>10</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="14">
         <v>10</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="13">
+      <c r="B10" s="11">
         <v>5</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>80</v>
       </c>
       <c r="D10" t="s">
         <v>49</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="14">
         <v>5</v>
       </c>
-      <c r="F10">
-        <f>G9</f>
+      <c r="F10" s="14">
+        <f t="shared" si="0"/>
         <v>99442</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="14">
         <v>99441</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="14">
         <f>F10-G10</f>
         <v>1</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="14">
         <v>10</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="14">
         <v>10</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="13">
-        <v>6</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="E11">
-        <v>6</v>
-      </c>
-      <c r="F11">
-        <f>G10</f>
-        <v>99441</v>
-      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
     </row>
     <row r="12" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="13">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="12"/>
+    </row>
+    <row r="16" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="11">
+        <v>0</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="14">
+        <v>0</v>
+      </c>
+      <c r="F17" s="14">
+        <v>1000163</v>
+      </c>
+      <c r="G17" s="14">
+        <v>1000163</v>
+      </c>
+      <c r="H17" s="14">
+        <v>0</v>
+      </c>
+      <c r="I17" s="14">
+        <v>5</v>
+      </c>
+      <c r="J17" s="14">
+        <v>5</v>
+      </c>
+      <c r="K17" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B18" s="11">
+        <v>1</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="14">
+        <v>1</v>
+      </c>
+      <c r="F18" s="14">
+        <f>G17</f>
+        <v>1000163</v>
+      </c>
+      <c r="G18" s="14">
+        <v>1000163</v>
+      </c>
+      <c r="H18" s="14">
+        <v>0</v>
+      </c>
+      <c r="I18" s="14">
+        <v>5</v>
+      </c>
+      <c r="J18" s="14">
+        <v>5</v>
+      </c>
+      <c r="K18" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B19" s="11">
+        <v>2</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="14">
+        <v>2</v>
+      </c>
+      <c r="F19" s="14">
+        <f>G18</f>
+        <v>1000163</v>
+      </c>
+      <c r="G19" s="14">
+        <v>1000163</v>
+      </c>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14">
+        <v>5</v>
+      </c>
+      <c r="J19" s="14">
+        <v>5</v>
+      </c>
+      <c r="K19" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B20" s="11">
+        <v>3</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="14">
+        <v>3</v>
+      </c>
+      <c r="F20" s="14">
+        <f>G19</f>
+        <v>1000163</v>
+      </c>
+      <c r="G20" s="14">
+        <v>1686</v>
+      </c>
+      <c r="H20" s="14">
+        <f>F20-G20</f>
+        <v>998477</v>
+      </c>
+      <c r="I20" s="14">
+        <v>5</v>
+      </c>
+      <c r="J20" s="14">
+        <v>5</v>
+      </c>
+      <c r="K20" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="15">
+        <v>4</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="14">
+        <v>4</v>
+      </c>
+      <c r="F21" s="14">
+        <f>G20</f>
+        <v>1686</v>
+      </c>
+      <c r="G21" s="14">
+        <v>1685</v>
+      </c>
+      <c r="H21" s="14">
+        <v>1</v>
+      </c>
+      <c r="I21" s="14">
+        <v>5</v>
+      </c>
+      <c r="J21" s="14">
+        <v>5</v>
+      </c>
+      <c r="K21" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E22" s="14">
+        <v>5</v>
+      </c>
+      <c r="F22" s="14">
+        <f>G21</f>
+        <v>1685</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+    </row>
+    <row r="26" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="C26" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B28" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B29" s="11">
+        <v>0</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="14">
+        <v>0</v>
+      </c>
+      <c r="F29" s="14">
+        <v>112650</v>
+      </c>
+      <c r="G29" s="14">
+        <v>112650</v>
+      </c>
+      <c r="H29" s="14">
+        <v>0</v>
+      </c>
+      <c r="I29" s="14">
         <v>7</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="E12">
+      <c r="J29" s="14">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="13">
-        <v>8</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="E13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="13">
-        <v>9</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="E14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="13">
-        <v>10</v>
-      </c>
-      <c r="E15">
-        <v>10</v>
-      </c>
+      <c r="K29" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B30" s="11">
+        <v>1</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="14">
+        <v>1</v>
+      </c>
+      <c r="F30" s="14">
+        <f>G29</f>
+        <v>112650</v>
+      </c>
+      <c r="G30" s="14">
+        <v>112650</v>
+      </c>
+      <c r="H30" s="14">
+        <f>F30-G30</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="14">
+        <v>7</v>
+      </c>
+      <c r="J30" s="14">
+        <v>7</v>
+      </c>
+      <c r="K30" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B31" s="11">
+        <v>2</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" s="14">
+        <v>2</v>
+      </c>
+      <c r="F31" s="14">
+        <f>G30</f>
+        <v>112650</v>
+      </c>
+      <c r="G31" s="14">
+        <v>112650</v>
+      </c>
+      <c r="H31" s="14">
+        <v>0</v>
+      </c>
+      <c r="I31" s="14">
+        <v>7</v>
+      </c>
+      <c r="J31" s="14">
+        <v>7</v>
+      </c>
+      <c r="K31" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B32" s="11">
+        <v>3</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" s="14">
+        <v>3</v>
+      </c>
+      <c r="F32" s="14">
+        <f>G31</f>
+        <v>112650</v>
+      </c>
+      <c r="G32" s="14">
+        <v>112650</v>
+      </c>
+      <c r="H32" s="14">
+        <v>0</v>
+      </c>
+      <c r="I32" s="14">
+        <v>7</v>
+      </c>
+      <c r="J32" s="14">
+        <v>7</v>
+      </c>
+      <c r="K32" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B33" s="15">
+        <v>4</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="14">
+        <v>4</v>
+      </c>
+      <c r="F33" s="14">
+        <f>G32</f>
+        <v>112650</v>
+      </c>
+      <c r="G33" s="14">
+        <v>98666</v>
+      </c>
+      <c r="H33" s="14">
+        <f>F33-G33</f>
+        <v>13984</v>
+      </c>
+      <c r="I33" s="14">
+        <v>7</v>
+      </c>
+      <c r="J33" s="14">
+        <v>7</v>
+      </c>
+      <c r="K33" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E34" s="14">
+        <v>5</v>
+      </c>
+      <c r="F34" s="14">
+        <f>G33</f>
+        <v>98666</v>
+      </c>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Order_Payment, Order_Reviews, Orders those tables in Power BI after transformation & Add Steps in Excel Report
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E1DC09-A743-4962-8665-57A02AC2EB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342534C8-3B04-4D85-A125-2D110C73A8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="3" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="150">
   <si>
     <t>Load Order</t>
   </si>
@@ -182,9 +182,6 @@
     <t>Sr. No</t>
   </si>
   <si>
-    <t>Column Name</t>
-  </si>
-  <si>
     <t>Column Description</t>
   </si>
   <si>
@@ -366,6 +363,132 @@
   </si>
   <si>
     <t>Shipping or delivery cost charged for the order. Used to analyze logistics costs and profit margins.</t>
+  </si>
+  <si>
+    <t>Description / Use</t>
+  </si>
+  <si>
+    <t>Unique identifier of the order. Helps link payment records to order details.</t>
+  </si>
+  <si>
+    <t>Payment_Sequential</t>
+  </si>
+  <si>
+    <t>Payment attempt number for the same order (1 = first attempt).</t>
+  </si>
+  <si>
+    <t>Payment_Type</t>
+  </si>
+  <si>
+    <t>Method of payment (credit card, debit card, voucher, etc.).</t>
+  </si>
+  <si>
+    <t>Payment_Installments</t>
+  </si>
+  <si>
+    <t>Number of installments chosen by customer. Useful for financial analysis.</t>
+  </si>
+  <si>
+    <t>Payment_Value</t>
+  </si>
+  <si>
+    <t>Total payment amount made for the order. Used for revenue calculations.</t>
+  </si>
+  <si>
+    <t>Review_ID</t>
+  </si>
+  <si>
+    <t>Unique identifier for each customer review. Used for identification and linking.</t>
+  </si>
+  <si>
+    <t>The order associated with the review. Helps join with orders table for analysis.</t>
+  </si>
+  <si>
+    <t>Review_Score</t>
+  </si>
+  <si>
+    <t>Rating given by customer (1 to 5). Used for sentiment and performance analysis.</t>
+  </si>
+  <si>
+    <t>Review_Comment_Title_En</t>
+  </si>
+  <si>
+    <t>Short title/headline of the review (in English).</t>
+  </si>
+  <si>
+    <t>Review_Comment_Message_En</t>
+  </si>
+  <si>
+    <t>Full review message written by customer (in English). Used for text analysis.</t>
+  </si>
+  <si>
+    <t>Review_Creation_Date</t>
+  </si>
+  <si>
+    <t>Date when customer submitted the review. Helps track review trends over time.</t>
+  </si>
+  <si>
+    <t>Review_Answer_Timestamp</t>
+  </si>
+  <si>
+    <t>Timestamp when seller responded to the review. Helps measure response time and service quality.</t>
+  </si>
+  <si>
+    <t>Remove Empty String</t>
+  </si>
+  <si>
+    <t>After Column Name</t>
+  </si>
+  <si>
+    <t>Review_Title</t>
+  </si>
+  <si>
+    <t>Review_Message</t>
+  </si>
+  <si>
+    <t>Before Column Name</t>
+  </si>
+  <si>
+    <t>Unique ID of each order placed by a customer. Used as the primary key to link with other tables.</t>
+  </si>
+  <si>
+    <t>Unique identifier of the customer who placed the order. Helps track customer-level activity.</t>
+  </si>
+  <si>
+    <t>Order_Status</t>
+  </si>
+  <si>
+    <t>Current state of the order (delivered, shipped, invoiced, canceled, etc.). Used in order lifecycle analysis.</t>
+  </si>
+  <si>
+    <t>Order_Purchase_Timestamp</t>
+  </si>
+  <si>
+    <t>Exact date &amp; time when the order was placed. Helps calculate lead time and order trend analysis.</t>
+  </si>
+  <si>
+    <t>Order_Approved_At</t>
+  </si>
+  <si>
+    <t>Date &amp; time when payment was approved. May be blank if order is pending.</t>
+  </si>
+  <si>
+    <t>Order_Delivered_Carrier_Date</t>
+  </si>
+  <si>
+    <t>Date &amp; time when the seller/carrier dispatched the order. Null means shipment not yet done.</t>
+  </si>
+  <si>
+    <t>Order_Delivered_Customer_Date</t>
+  </si>
+  <si>
+    <t>Date &amp; time when the customer actually received the product. Used to calculate delivery time.</t>
+  </si>
+  <si>
+    <t>Order_Estimated_Delivery_Date</t>
+  </si>
+  <si>
+    <t>Expected delivery date provided at the time of purchase. Used to measure delays or early deliveries.</t>
   </si>
 </sst>
 </file>
@@ -530,11 +653,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1129,314 +1252,625 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035EC863-7662-4F46-A1E6-DDC33702C1E8}">
-  <dimension ref="B3:E43"/>
+  <dimension ref="B3:F76"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.109375" customWidth="1"/>
     <col min="4" max="4" width="26.6640625" customWidth="1"/>
     <col min="5" max="5" width="51" customWidth="1"/>
+    <col min="6" max="6" width="34.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B3" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F4" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C7" s="5">
         <v>3</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="5">
         <v>4</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="5" t="s">
+    </row>
+    <row r="9" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C9" s="5">
+        <v>5</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C9" s="5">
-        <v>5</v>
-      </c>
-      <c r="D9" s="16" t="s">
+      <c r="E9" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C10" s="5">
         <v>6</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C11" s="5">
         <v>7</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C12" s="5">
         <v>8</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C13" s="5">
         <v>9</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C14" s="5">
         <v>10</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B19" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>47</v>
+        <v>135</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="46.8" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C21" s="5">
         <v>1</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C22" s="5">
         <v>2</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C23" s="5">
         <v>3</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C24" s="5">
         <v>4</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E24" s="5" t="s">
+    </row>
+    <row r="25" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C25" s="5">
+        <v>5</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="C25" s="5">
-        <v>5</v>
-      </c>
-      <c r="D25" s="16" t="s">
+      <c r="E25" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B30" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C31" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>47</v>
+        <v>135</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C32" s="5">
         <v>1</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C33" s="5">
         <v>2</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C34" s="5">
         <v>3</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="46.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C35" s="5">
         <v>4</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E35" s="5" t="s">
+    </row>
+    <row r="36" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C36" s="5">
+        <v>5</v>
+      </c>
+      <c r="D36" s="14" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="C36" s="5">
-        <v>5</v>
-      </c>
-      <c r="D36" s="16" t="s">
+      <c r="E36" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C37" s="5">
         <v>6</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C38" s="5">
         <v>7</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E38" s="5" t="s">
+    </row>
+    <row r="43" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B43" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="43" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B43" s="13" t="s">
-        <v>17</v>
-      </c>
+      <c r="F44" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C45" s="5">
+        <v>1</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C46" s="5">
+        <v>2</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C47" s="5">
+        <v>3</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C48" s="5">
+        <v>4</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C49" s="5">
+        <v>5</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B54" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C55" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C56" s="5">
+        <v>1</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C57" s="5">
+        <v>2</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F57" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C58" s="5">
+        <v>3</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C59" s="5">
+        <v>4</v>
+      </c>
+      <c r="D59" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C60" s="5">
+        <v>5</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F60" s="14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C61" s="5">
+        <v>6</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="C62" s="5">
+        <v>7</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B67" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C68" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C69" s="14">
+        <v>1</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F69" s="11"/>
+    </row>
+    <row r="70" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C70" s="14">
+        <v>2</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F70" s="11"/>
+    </row>
+    <row r="71" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C71" s="14">
+        <v>3</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F71" s="11"/>
+    </row>
+    <row r="72" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C72" s="14">
+        <v>4</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F72" s="11"/>
+    </row>
+    <row r="73" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C73" s="14">
+        <v>5</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F73" s="11"/>
+    </row>
+    <row r="74" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C74" s="14">
+        <v>6</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F74" s="11"/>
+    </row>
+    <row r="75" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C75" s="14">
+        <v>7</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F75" s="11"/>
+    </row>
+    <row r="76" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C76" s="14">
+        <v>8</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F76" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1446,17 +1880,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05F3B95-CD15-4EA0-ACD4-4067EC5DC14D}">
-  <dimension ref="B2:K34"/>
+  <dimension ref="B2:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.6640625" customWidth="1"/>
     <col min="7" max="7" width="26.33203125" customWidth="1"/>
@@ -1468,37 +1902,37 @@
   <sheetData>
     <row r="2" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="C2" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>70</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -1506,27 +1940,27 @@
         <v>0</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="14">
-        <v>0</v>
-      </c>
-      <c r="F5" s="14">
+        <v>76</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0</v>
+      </c>
+      <c r="F5" s="11">
         <v>102727</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="11">
         <v>102727</v>
       </c>
-      <c r="H5" s="14">
-        <v>0</v>
-      </c>
-      <c r="I5" s="14">
+      <c r="H5" s="11">
+        <v>0</v>
+      </c>
+      <c r="I5" s="11">
         <v>10</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="11">
         <v>10</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="11">
         <v>0</v>
       </c>
     </row>
@@ -1535,28 +1969,28 @@
         <v>1</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="14">
+        <v>78</v>
+      </c>
+      <c r="E6" s="11">
         <v>1</v>
       </c>
-      <c r="F6" s="14">
-        <f t="shared" ref="F6:F11" si="0">G5</f>
+      <c r="F6" s="11">
+        <f t="shared" ref="F6:F10" si="0">G5</f>
         <v>102727</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="11">
         <v>102727</v>
       </c>
-      <c r="H6" s="14">
-        <v>0</v>
-      </c>
-      <c r="I6" s="14">
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6" s="11">
         <v>10</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="11">
         <v>10</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="11">
         <v>0</v>
       </c>
     </row>
@@ -1565,28 +1999,28 @@
         <v>2</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E7" s="14">
+        <v>79</v>
+      </c>
+      <c r="E7" s="11">
         <v>2</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="11">
         <f t="shared" si="0"/>
         <v>102727</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="11">
         <v>102727</v>
       </c>
-      <c r="H7" s="14">
-        <v>0</v>
-      </c>
-      <c r="I7" s="14">
+      <c r="H7" s="11">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11">
         <v>10</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="11">
         <v>10</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="11">
         <v>0</v>
       </c>
     </row>
@@ -1595,26 +2029,26 @@
         <v>3</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="14">
+        <v>80</v>
+      </c>
+      <c r="E8" s="11">
         <v>3</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="11">
         <f t="shared" si="0"/>
         <v>102727</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="11">
         <v>102727</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14">
+      <c r="H8" s="11"/>
+      <c r="I8" s="11">
         <v>10</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="11">
         <v>10</v>
       </c>
-      <c r="K8" s="14">
+      <c r="K8" s="11">
         <v>0</v>
       </c>
     </row>
@@ -1623,32 +2057,32 @@
         <v>4</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="14">
+        <v>48</v>
+      </c>
+      <c r="E9" s="11">
         <v>4</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="11">
         <f t="shared" si="0"/>
         <v>102727</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="11">
         <v>99442</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="11">
         <f>F9-G9</f>
         <v>3285</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9" s="11">
         <v>10</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="11">
         <v>10</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="11">
         <v>0</v>
       </c>
     </row>
@@ -1657,32 +2091,32 @@
         <v>5</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="14">
-        <v>5</v>
-      </c>
-      <c r="F10" s="14">
+        <v>48</v>
+      </c>
+      <c r="E10" s="11">
+        <v>5</v>
+      </c>
+      <c r="F10" s="11">
         <f t="shared" si="0"/>
         <v>99442</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="11">
         <v>99441</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="11">
         <f>F10-G10</f>
         <v>1</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="11">
         <v>10</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="11">
         <v>10</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="11">
         <v>0</v>
       </c>
     </row>
@@ -1709,32 +2143,32 @@
     </row>
     <row r="16" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>70</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F16" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="H16" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="I16" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="J16" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="K16" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="17" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -1742,27 +2176,27 @@
         <v>0</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="14">
-        <v>0</v>
-      </c>
-      <c r="F17" s="14">
+        <v>76</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0</v>
+      </c>
+      <c r="F17" s="11">
         <v>1000163</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="11">
         <v>1000163</v>
       </c>
-      <c r="H17" s="14">
-        <v>0</v>
-      </c>
-      <c r="I17" s="14">
-        <v>5</v>
-      </c>
-      <c r="J17" s="14">
-        <v>5</v>
-      </c>
-      <c r="K17" s="14">
+      <c r="H17" s="11">
+        <v>0</v>
+      </c>
+      <c r="I17" s="11">
+        <v>5</v>
+      </c>
+      <c r="J17" s="11">
+        <v>5</v>
+      </c>
+      <c r="K17" s="11">
         <v>0</v>
       </c>
     </row>
@@ -1771,28 +2205,28 @@
         <v>1</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="14">
+        <v>78</v>
+      </c>
+      <c r="E18" s="11">
         <v>1</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="11">
         <f>G17</f>
         <v>1000163</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="11">
         <v>1000163</v>
       </c>
-      <c r="H18" s="14">
-        <v>0</v>
-      </c>
-      <c r="I18" s="14">
-        <v>5</v>
-      </c>
-      <c r="J18" s="14">
-        <v>5</v>
-      </c>
-      <c r="K18" s="14">
+      <c r="H18" s="11">
+        <v>0</v>
+      </c>
+      <c r="I18" s="11">
+        <v>5</v>
+      </c>
+      <c r="J18" s="11">
+        <v>5</v>
+      </c>
+      <c r="K18" s="11">
         <v>0</v>
       </c>
     </row>
@@ -1801,26 +2235,26 @@
         <v>2</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="14">
+        <v>79</v>
+      </c>
+      <c r="E19" s="11">
         <v>2</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="11">
         <f>G18</f>
         <v>1000163</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="11">
         <v>1000163</v>
       </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14">
-        <v>5</v>
-      </c>
-      <c r="J19" s="14">
-        <v>5</v>
-      </c>
-      <c r="K19" s="14">
+      <c r="H19" s="11"/>
+      <c r="I19" s="11">
+        <v>5</v>
+      </c>
+      <c r="J19" s="11">
+        <v>5</v>
+      </c>
+      <c r="K19" s="11">
         <v>0</v>
       </c>
     </row>
@@ -1829,75 +2263,75 @@
         <v>3</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="14">
+        <v>80</v>
+      </c>
+      <c r="E20" s="11">
         <v>3</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="11">
         <f>G19</f>
         <v>1000163</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="11">
         <v>1686</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="11">
         <f>F20-G20</f>
         <v>998477</v>
       </c>
-      <c r="I20" s="14">
-        <v>5</v>
-      </c>
-      <c r="J20" s="14">
-        <v>5</v>
-      </c>
-      <c r="K20" s="14">
+      <c r="I20" s="11">
+        <v>5</v>
+      </c>
+      <c r="J20" s="11">
+        <v>5</v>
+      </c>
+      <c r="K20" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B21" s="15">
+      <c r="B21" s="11">
         <v>4</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="14">
+      <c r="C21" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="11">
         <v>4</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="11">
         <f>G20</f>
         <v>1686</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="11">
         <v>1685</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="11">
         <v>1</v>
       </c>
-      <c r="I21" s="14">
-        <v>5</v>
-      </c>
-      <c r="J21" s="14">
-        <v>5</v>
-      </c>
-      <c r="K21" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E22" s="14">
-        <v>5</v>
-      </c>
-      <c r="F22" s="14">
+      <c r="I21" s="11">
+        <v>5</v>
+      </c>
+      <c r="J21" s="11">
+        <v>5</v>
+      </c>
+      <c r="K21" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E22" s="11">
+        <v>5</v>
+      </c>
+      <c r="F22" s="11">
         <f>G21</f>
         <v>1685</v>
       </c>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
     </row>
     <row r="26" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="C26" s="13" t="s">
@@ -1906,32 +2340,32 @@
     </row>
     <row r="28" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>70</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F28" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="H28" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="I28" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="I28" s="10" t="s">
+      <c r="J28" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="J28" s="10" t="s">
+      <c r="K28" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="K28" s="10" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="29" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -1939,27 +2373,27 @@
         <v>0</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" s="14">
-        <v>0</v>
-      </c>
-      <c r="F29" s="14">
+        <v>76</v>
+      </c>
+      <c r="E29" s="11">
+        <v>0</v>
+      </c>
+      <c r="F29" s="11">
         <v>112650</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="11">
         <v>112650</v>
       </c>
-      <c r="H29" s="14">
-        <v>0</v>
-      </c>
-      <c r="I29" s="14">
+      <c r="H29" s="11">
+        <v>0</v>
+      </c>
+      <c r="I29" s="11">
         <v>7</v>
       </c>
-      <c r="J29" s="14">
+      <c r="J29" s="11">
         <v>7</v>
       </c>
-      <c r="K29" s="14">
+      <c r="K29" s="11">
         <v>0</v>
       </c>
     </row>
@@ -1968,29 +2402,29 @@
         <v>1</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="14">
+        <v>78</v>
+      </c>
+      <c r="E30" s="11">
         <v>1</v>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="11">
         <f>G29</f>
         <v>112650</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="11">
         <v>112650</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="11">
         <f>F30-G30</f>
         <v>0</v>
       </c>
-      <c r="I30" s="14">
+      <c r="I30" s="11">
         <v>7</v>
       </c>
-      <c r="J30" s="14">
+      <c r="J30" s="11">
         <v>7</v>
       </c>
-      <c r="K30" s="14">
+      <c r="K30" s="11">
         <v>0</v>
       </c>
     </row>
@@ -1999,28 +2433,28 @@
         <v>2</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" s="14">
+        <v>79</v>
+      </c>
+      <c r="E31" s="11">
         <v>2</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="11">
         <f>G30</f>
         <v>112650</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="11">
         <v>112650</v>
       </c>
-      <c r="H31" s="14">
-        <v>0</v>
-      </c>
-      <c r="I31" s="14">
+      <c r="H31" s="11">
+        <v>0</v>
+      </c>
+      <c r="I31" s="11">
         <v>7</v>
       </c>
-      <c r="J31" s="14">
+      <c r="J31" s="11">
         <v>7</v>
       </c>
-      <c r="K31" s="14">
+      <c r="K31" s="11">
         <v>0</v>
       </c>
     </row>
@@ -2029,78 +2463,650 @@
         <v>3</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="E32" s="14">
+        <v>80</v>
+      </c>
+      <c r="E32" s="11">
         <v>3</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="11">
         <f>G31</f>
         <v>112650</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="11">
         <v>112650</v>
       </c>
-      <c r="H32" s="14">
-        <v>0</v>
-      </c>
-      <c r="I32" s="14">
+      <c r="H32" s="11">
+        <v>0</v>
+      </c>
+      <c r="I32" s="11">
         <v>7</v>
       </c>
-      <c r="J32" s="14">
+      <c r="J32" s="11">
         <v>7</v>
       </c>
-      <c r="K32" s="14">
+      <c r="K32" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B33" s="15">
+      <c r="B33" s="11">
         <v>4</v>
       </c>
-      <c r="C33" s="15" t="s">
-        <v>81</v>
+      <c r="C33" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="D33" t="s">
-        <v>95</v>
-      </c>
-      <c r="E33" s="14">
+        <v>94</v>
+      </c>
+      <c r="E33" s="11">
         <v>4</v>
       </c>
-      <c r="F33" s="14">
+      <c r="F33" s="11">
         <f>G32</f>
         <v>112650</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="11">
         <v>98666</v>
       </c>
-      <c r="H33" s="14">
+      <c r="H33" s="11">
         <f>F33-G33</f>
         <v>13984</v>
       </c>
-      <c r="I33" s="14">
+      <c r="I33" s="11">
         <v>7</v>
       </c>
-      <c r="J33" s="14">
+      <c r="J33" s="11">
         <v>7</v>
       </c>
-      <c r="K33" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E34" s="14">
-        <v>5</v>
-      </c>
-      <c r="F34" s="14">
+      <c r="K33" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E34" s="11">
+        <v>5</v>
+      </c>
+      <c r="F34" s="11">
         <f>G33</f>
         <v>98666</v>
       </c>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+    </row>
+    <row r="38" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="C38" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B39" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I39" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J39" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B40" s="11">
+        <v>0</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E40" s="11">
+        <v>0</v>
+      </c>
+      <c r="F40" s="11">
+        <v>103886</v>
+      </c>
+      <c r="G40" s="11">
+        <v>103886</v>
+      </c>
+      <c r="H40" s="11">
+        <v>0</v>
+      </c>
+      <c r="I40" s="11">
+        <v>5</v>
+      </c>
+      <c r="J40" s="11">
+        <v>5</v>
+      </c>
+      <c r="K40" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B41" s="11">
+        <v>1</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" s="11">
+        <v>1</v>
+      </c>
+      <c r="F41" s="11">
+        <f>G40</f>
+        <v>103886</v>
+      </c>
+      <c r="G41" s="11">
+        <v>103886</v>
+      </c>
+      <c r="H41" s="11">
+        <v>0</v>
+      </c>
+      <c r="I41" s="11">
+        <v>5</v>
+      </c>
+      <c r="J41" s="11">
+        <v>5</v>
+      </c>
+      <c r="K41" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B42" s="11">
+        <v>2</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E42" s="11">
+        <v>2</v>
+      </c>
+      <c r="F42" s="11">
+        <f>G41</f>
+        <v>103886</v>
+      </c>
+      <c r="G42" s="11">
+        <v>103886</v>
+      </c>
+      <c r="H42" s="11">
+        <v>0</v>
+      </c>
+      <c r="I42" s="11">
+        <v>5</v>
+      </c>
+      <c r="J42" s="11">
+        <v>5</v>
+      </c>
+      <c r="K42" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B43" s="11">
+        <v>3</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" s="11">
+        <v>3</v>
+      </c>
+      <c r="F43" s="11">
+        <f>G42</f>
+        <v>103886</v>
+      </c>
+      <c r="G43" s="11">
+        <v>103886</v>
+      </c>
+      <c r="H43" s="11">
+        <v>0</v>
+      </c>
+      <c r="I43" s="11">
+        <v>5</v>
+      </c>
+      <c r="J43" s="11">
+        <v>5</v>
+      </c>
+      <c r="K43" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E44" s="11">
+        <v>4</v>
+      </c>
+      <c r="F44" s="11">
+        <f>G43</f>
+        <v>103886</v>
+      </c>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+    </row>
+    <row r="48" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="C48" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B49" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I49" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J49" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="K49" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B50" s="11">
+        <v>0</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E50" s="11">
+        <v>0</v>
+      </c>
+      <c r="F50" s="11">
+        <v>99329</v>
+      </c>
+      <c r="G50" s="11">
+        <v>99329</v>
+      </c>
+      <c r="H50" s="11">
+        <v>0</v>
+      </c>
+      <c r="I50" s="11">
+        <v>7</v>
+      </c>
+      <c r="J50" s="11">
+        <v>7</v>
+      </c>
+      <c r="K50" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B51" s="11">
+        <v>1</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" s="11">
+        <v>1</v>
+      </c>
+      <c r="F51" s="11">
+        <f>G50</f>
+        <v>99329</v>
+      </c>
+      <c r="G51" s="11">
+        <v>99327</v>
+      </c>
+      <c r="H51" s="11">
+        <f>F51-G51</f>
+        <v>2</v>
+      </c>
+      <c r="I51" s="11">
+        <v>7</v>
+      </c>
+      <c r="J51" s="11">
+        <v>7</v>
+      </c>
+      <c r="K51" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B52" s="11">
+        <v>2</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E52" s="11">
+        <v>2</v>
+      </c>
+      <c r="F52" s="11">
+        <f>G51</f>
+        <v>99327</v>
+      </c>
+      <c r="G52" s="11">
+        <v>99268</v>
+      </c>
+      <c r="H52" s="11">
+        <f>F52-G52</f>
+        <v>59</v>
+      </c>
+      <c r="I52" s="11">
+        <v>7</v>
+      </c>
+      <c r="J52" s="11">
+        <v>7</v>
+      </c>
+      <c r="K52" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B53" s="11">
+        <v>3</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E53" s="11">
+        <v>3</v>
+      </c>
+      <c r="F53" s="11">
+        <f>G52</f>
+        <v>99268</v>
+      </c>
+      <c r="G53" s="11">
+        <v>99268</v>
+      </c>
+      <c r="H53" s="11">
+        <f>F53-G53</f>
+        <v>0</v>
+      </c>
+      <c r="I53" s="11">
+        <v>7</v>
+      </c>
+      <c r="J53" s="11">
+        <v>7</v>
+      </c>
+      <c r="K53" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B54" s="15">
+        <v>4</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" t="s">
+        <v>94</v>
+      </c>
+      <c r="E54" s="11">
+        <v>4</v>
+      </c>
+      <c r="F54" s="11">
+        <f>G53</f>
+        <v>99268</v>
+      </c>
+      <c r="G54" s="11">
+        <v>99223</v>
+      </c>
+      <c r="H54" s="11">
+        <f>F54-G54</f>
+        <v>45</v>
+      </c>
+      <c r="I54" s="11">
+        <v>7</v>
+      </c>
+      <c r="J54" s="11">
+        <v>7</v>
+      </c>
+      <c r="K54" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B55" s="15">
+        <v>5</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D55" t="s">
+        <v>127</v>
+      </c>
+      <c r="E55" s="11">
+        <v>5</v>
+      </c>
+      <c r="F55" s="11">
+        <f>G54</f>
+        <v>99223</v>
+      </c>
+      <c r="G55" s="11">
+        <v>99221</v>
+      </c>
+      <c r="H55" s="11">
+        <f>F55-G55</f>
+        <v>2</v>
+      </c>
+      <c r="I55" s="11">
+        <v>7</v>
+      </c>
+      <c r="J55" s="11">
+        <v>7</v>
+      </c>
+      <c r="K55" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E56" s="11">
+        <v>6</v>
+      </c>
+      <c r="F56" s="11">
+        <f>G55</f>
+        <v>99221</v>
+      </c>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+    </row>
+    <row r="61" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="C61" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B62" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I62" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J62" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="K62" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B63" s="11">
+        <v>0</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E63" s="16">
+        <v>0</v>
+      </c>
+      <c r="F63" s="16">
+        <v>99441</v>
+      </c>
+      <c r="G63" s="16">
+        <v>99441</v>
+      </c>
+      <c r="H63" s="16">
+        <v>0</v>
+      </c>
+      <c r="I63" s="16">
+        <v>8</v>
+      </c>
+      <c r="J63" s="16">
+        <v>8</v>
+      </c>
+      <c r="K63" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B64" s="11">
+        <v>1</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E64" s="16">
+        <v>1</v>
+      </c>
+      <c r="F64" s="16">
+        <f>G63</f>
+        <v>99441</v>
+      </c>
+      <c r="G64" s="16">
+        <v>99441</v>
+      </c>
+      <c r="H64" s="16">
+        <v>0</v>
+      </c>
+      <c r="I64" s="16">
+        <v>8</v>
+      </c>
+      <c r="J64" s="16">
+        <v>8</v>
+      </c>
+      <c r="K64" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B65" s="11">
+        <v>2</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E65" s="16">
+        <v>2</v>
+      </c>
+      <c r="F65" s="16">
+        <f>G64</f>
+        <v>99441</v>
+      </c>
+      <c r="G65" s="16">
+        <v>99441</v>
+      </c>
+      <c r="H65" s="16">
+        <v>0</v>
+      </c>
+      <c r="I65" s="16">
+        <v>8</v>
+      </c>
+      <c r="J65" s="16">
+        <v>8</v>
+      </c>
+      <c r="K65" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B66" s="11">
+        <v>3</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E66" s="16">
+        <v>3</v>
+      </c>
+      <c r="F66" s="16">
+        <f>G65</f>
+        <v>99441</v>
+      </c>
+      <c r="G66" s="16">
+        <v>99441</v>
+      </c>
+      <c r="H66" s="16">
+        <v>0</v>
+      </c>
+      <c r="I66" s="16">
+        <v>8</v>
+      </c>
+      <c r="J66" s="16">
+        <v>8</v>
+      </c>
+      <c r="K66" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E67" s="16">
+        <v>4</v>
+      </c>
+      <c r="F67" s="16">
+        <f>G66</f>
+        <v>99441</v>
+      </c>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="16"/>
+      <c r="K67" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Product Table in Power BI After Transformation & Also add Steps in Excel Sheet
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342534C8-3B04-4D85-A125-2D110C73A8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6412223-1588-4357-AB18-0F6D3F8E99E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="3" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="163">
   <si>
     <t>Load Order</t>
   </si>
@@ -489,6 +489,45 @@
   </si>
   <si>
     <t>Expected delivery date provided at the time of purchase. Used to measure delays or early deliveries.</t>
+  </si>
+  <si>
+    <t>Column Name</t>
+  </si>
+  <si>
+    <t>Unique identifier for each product. Used to link product details with orders and order items.</t>
+  </si>
+  <si>
+    <t>Product_Category_Name</t>
+  </si>
+  <si>
+    <t>Category/group of the product (e.g., Baby, Sports, Perfumery). Helpful for category-wise analysis and segmentation.</t>
+  </si>
+  <si>
+    <t>Product_Weight_Gr</t>
+  </si>
+  <si>
+    <t>Weight of the product in grams. Useful for logistics cost calculation and freight analysis.</t>
+  </si>
+  <si>
+    <t>Product_Length_Cm</t>
+  </si>
+  <si>
+    <t>Length of the product package in centimeters. Used to estimate package volume.</t>
+  </si>
+  <si>
+    <t>Product_Height_Cm</t>
+  </si>
+  <si>
+    <t>Height of the product package in centimeters. Contributes to volume and shipping dimension calculations.</t>
+  </si>
+  <si>
+    <t>Product_Width_Cm</t>
+  </si>
+  <si>
+    <t>Width of the product package in centimeters. Helps calculate cubic volume for delivery estimation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove Row Top 4 of Zero </t>
   </si>
 </sst>
 </file>
@@ -656,8 +695,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1252,10 +1291,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035EC863-7662-4F46-A1E6-DDC33702C1E8}">
-  <dimension ref="B3:F76"/>
+  <dimension ref="B3:F97"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView topLeftCell="B72" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1729,7 +1768,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="61" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C61" s="5">
         <v>6</v>
       </c>
@@ -1743,7 +1782,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="2:6" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C62" s="5">
         <v>7</v>
       </c>
@@ -1871,6 +1910,116 @@
         <v>149</v>
       </c>
       <c r="F76" s="11"/>
+    </row>
+    <row r="82" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B82" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C83" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C84" s="14">
+        <v>1</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F84" s="15"/>
+    </row>
+    <row r="85" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C85" s="14">
+        <v>2</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F85" s="15"/>
+    </row>
+    <row r="86" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C86" s="14">
+        <v>3</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F86" s="15"/>
+    </row>
+    <row r="87" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C87" s="14">
+        <v>4</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F87" s="15"/>
+    </row>
+    <row r="88" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C88" s="14">
+        <v>5</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F88" s="15"/>
+    </row>
+    <row r="89" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C89" s="14">
+        <v>6</v>
+      </c>
+      <c r="D89" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F89" s="15"/>
+    </row>
+    <row r="96" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B96" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C97" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1880,16 +2029,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05F3B95-CD15-4EA0-ACD4-4067EC5DC14D}">
-  <dimension ref="B2:K67"/>
+  <dimension ref="B2:K79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I71" sqref="I71"/>
+    <sheetView tabSelected="1" topLeftCell="D61" workbookViewId="0">
+      <selection activeCell="H79" sqref="H79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.6640625" customWidth="1"/>
@@ -2777,7 +2926,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="11">
-        <f>G50</f>
+        <f t="shared" ref="F51:F56" si="1">G50</f>
         <v>99329</v>
       </c>
       <c r="G51" s="11">
@@ -2808,7 +2957,7 @@
         <v>2</v>
       </c>
       <c r="F52" s="11">
-        <f>G51</f>
+        <f t="shared" si="1"/>
         <v>99327</v>
       </c>
       <c r="G52" s="11">
@@ -2839,7 +2988,7 @@
         <v>3</v>
       </c>
       <c r="F53" s="11">
-        <f>G52</f>
+        <f t="shared" si="1"/>
         <v>99268</v>
       </c>
       <c r="G53" s="11">
@@ -2860,7 +3009,7 @@
       </c>
     </row>
     <row r="54" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B54" s="15">
+      <c r="B54" s="11">
         <v>4</v>
       </c>
       <c r="C54" s="11" t="s">
@@ -2873,7 +3022,7 @@
         <v>4</v>
       </c>
       <c r="F54" s="11">
-        <f>G53</f>
+        <f t="shared" si="1"/>
         <v>99268</v>
       </c>
       <c r="G54" s="11">
@@ -2894,7 +3043,7 @@
       </c>
     </row>
     <row r="55" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B55" s="15">
+      <c r="B55" s="11">
         <v>5</v>
       </c>
       <c r="C55" s="11" t="s">
@@ -2907,7 +3056,7 @@
         <v>5</v>
       </c>
       <c r="F55" s="11">
-        <f>G54</f>
+        <f t="shared" si="1"/>
         <v>99223</v>
       </c>
       <c r="G55" s="11">
@@ -2932,7 +3081,7 @@
         <v>6</v>
       </c>
       <c r="F56" s="11">
-        <f>G55</f>
+        <f t="shared" si="1"/>
         <v>99221</v>
       </c>
       <c r="G56" s="11"/>
@@ -2982,25 +3131,25 @@
       <c r="C63" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E63" s="16">
-        <v>0</v>
-      </c>
-      <c r="F63" s="16">
+      <c r="E63" s="15">
+        <v>0</v>
+      </c>
+      <c r="F63" s="15">
         <v>99441</v>
       </c>
-      <c r="G63" s="16">
+      <c r="G63" s="15">
         <v>99441</v>
       </c>
-      <c r="H63" s="16">
-        <v>0</v>
-      </c>
-      <c r="I63" s="16">
+      <c r="H63" s="15">
+        <v>0</v>
+      </c>
+      <c r="I63" s="15">
         <v>8</v>
       </c>
-      <c r="J63" s="16">
+      <c r="J63" s="15">
         <v>8</v>
       </c>
-      <c r="K63" s="16">
+      <c r="K63" s="15">
         <v>0</v>
       </c>
     </row>
@@ -3011,26 +3160,26 @@
       <c r="C64" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E64" s="16">
+      <c r="E64" s="15">
         <v>1</v>
       </c>
-      <c r="F64" s="16">
+      <c r="F64" s="15">
         <f>G63</f>
         <v>99441</v>
       </c>
-      <c r="G64" s="16">
+      <c r="G64" s="15">
         <v>99441</v>
       </c>
-      <c r="H64" s="16">
-        <v>0</v>
-      </c>
-      <c r="I64" s="16">
+      <c r="H64" s="15">
+        <v>0</v>
+      </c>
+      <c r="I64" s="15">
         <v>8</v>
       </c>
-      <c r="J64" s="16">
+      <c r="J64" s="15">
         <v>8</v>
       </c>
-      <c r="K64" s="16">
+      <c r="K64" s="15">
         <v>0</v>
       </c>
     </row>
@@ -3041,26 +3190,26 @@
       <c r="C65" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E65" s="16">
+      <c r="E65" s="15">
         <v>2</v>
       </c>
-      <c r="F65" s="16">
+      <c r="F65" s="15">
         <f>G64</f>
         <v>99441</v>
       </c>
-      <c r="G65" s="16">
+      <c r="G65" s="15">
         <v>99441</v>
       </c>
-      <c r="H65" s="16">
-        <v>0</v>
-      </c>
-      <c r="I65" s="16">
+      <c r="H65" s="15">
+        <v>0</v>
+      </c>
+      <c r="I65" s="15">
         <v>8</v>
       </c>
-      <c r="J65" s="16">
+      <c r="J65" s="15">
         <v>8</v>
       </c>
-      <c r="K65" s="16">
+      <c r="K65" s="15">
         <v>0</v>
       </c>
     </row>
@@ -3071,42 +3220,277 @@
       <c r="C66" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E66" s="16">
+      <c r="E66" s="15">
         <v>3</v>
       </c>
-      <c r="F66" s="16">
+      <c r="F66" s="15">
         <f>G65</f>
         <v>99441</v>
       </c>
-      <c r="G66" s="16">
+      <c r="G66" s="15">
         <v>99441</v>
       </c>
-      <c r="H66" s="16">
-        <v>0</v>
-      </c>
-      <c r="I66" s="16">
+      <c r="H66" s="15">
+        <v>0</v>
+      </c>
+      <c r="I66" s="15">
         <v>8</v>
       </c>
-      <c r="J66" s="16">
+      <c r="J66" s="15">
         <v>8</v>
       </c>
-      <c r="K66" s="16">
+      <c r="K66" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E67" s="16">
+      <c r="E67" s="15">
         <v>4</v>
       </c>
-      <c r="F67" s="16">
+      <c r="F67" s="15">
         <f>G66</f>
         <v>99441</v>
       </c>
-      <c r="G67" s="16"/>
-      <c r="H67" s="16"/>
-      <c r="I67" s="16"/>
-      <c r="J67" s="16"/>
-      <c r="K67" s="16"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="15"/>
+      <c r="K67" s="15"/>
+    </row>
+    <row r="71" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="C71" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B72" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H72" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I72" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J72" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="K72" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B73" s="11">
+        <v>0</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E73" s="11">
+        <v>0</v>
+      </c>
+      <c r="F73" s="11">
+        <v>32951</v>
+      </c>
+      <c r="G73" s="11">
+        <v>32951</v>
+      </c>
+      <c r="H73" s="11">
+        <v>0</v>
+      </c>
+      <c r="I73" s="11">
+        <v>6</v>
+      </c>
+      <c r="J73" s="11">
+        <v>6</v>
+      </c>
+      <c r="K73" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B74" s="11">
+        <v>1</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E74" s="11">
+        <v>1</v>
+      </c>
+      <c r="F74" s="11">
+        <f>G73</f>
+        <v>32951</v>
+      </c>
+      <c r="G74" s="11">
+        <v>32951</v>
+      </c>
+      <c r="H74" s="11">
+        <v>0</v>
+      </c>
+      <c r="I74" s="11">
+        <v>6</v>
+      </c>
+      <c r="J74" s="11">
+        <v>6</v>
+      </c>
+      <c r="K74" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B75" s="11">
+        <v>2</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E75" s="11">
+        <v>2</v>
+      </c>
+      <c r="F75" s="11">
+        <f>G74</f>
+        <v>32951</v>
+      </c>
+      <c r="G75" s="11">
+        <v>32951</v>
+      </c>
+      <c r="H75" s="11">
+        <v>0</v>
+      </c>
+      <c r="I75" s="11">
+        <v>6</v>
+      </c>
+      <c r="J75" s="11">
+        <v>6</v>
+      </c>
+      <c r="K75" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B76" s="11">
+        <v>3</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E76" s="11">
+        <v>3</v>
+      </c>
+      <c r="F76" s="11">
+        <f>G75</f>
+        <v>32951</v>
+      </c>
+      <c r="G76" s="11">
+        <v>32951</v>
+      </c>
+      <c r="H76" s="11">
+        <v>0</v>
+      </c>
+      <c r="I76" s="11">
+        <v>6</v>
+      </c>
+      <c r="J76" s="11">
+        <v>6</v>
+      </c>
+      <c r="K76" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B77" s="16">
+        <v>4</v>
+      </c>
+      <c r="C77" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D77" t="s">
+        <v>154</v>
+      </c>
+      <c r="E77" s="11">
+        <v>4</v>
+      </c>
+      <c r="F77" s="11">
+        <f>G76</f>
+        <v>32951</v>
+      </c>
+      <c r="G77" s="11">
+        <v>32949</v>
+      </c>
+      <c r="H77" s="11">
+        <f>F77-G77</f>
+        <v>2</v>
+      </c>
+      <c r="I77" s="11">
+        <v>6</v>
+      </c>
+      <c r="J77" s="11">
+        <v>6</v>
+      </c>
+      <c r="K77" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B78" s="16">
+        <v>5</v>
+      </c>
+      <c r="C78" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D78" t="s">
+        <v>154</v>
+      </c>
+      <c r="E78" s="11">
+        <v>5</v>
+      </c>
+      <c r="F78" s="11">
+        <f>G77</f>
+        <v>32949</v>
+      </c>
+      <c r="G78" s="11">
+        <v>32945</v>
+      </c>
+      <c r="H78" s="11">
+        <f>F78-G78</f>
+        <v>4</v>
+      </c>
+      <c r="I78" s="11">
+        <v>6</v>
+      </c>
+      <c r="J78" s="11">
+        <v>6</v>
+      </c>
+      <c r="K78" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E79" s="11">
+        <v>6</v>
+      </c>
+      <c r="F79" s="11">
+        <f>G78</f>
+        <v>32945</v>
+      </c>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="11"/>
+      <c r="J79" s="11"/>
+      <c r="K79" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Load All Data Tables in Power BI After Transformation
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6412223-1588-4357-AB18-0F6D3F8E99E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA037218-847A-4F1A-8E72-363E889D32B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="3" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="4" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
   <sheets>
     <sheet name="Data &amp; Purpose" sheetId="1" r:id="rId1"/>
@@ -39,10 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="163">
-  <si>
-    <t>Load Order</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="173">
   <si>
     <t>Table Name</t>
   </si>
@@ -528,6 +525,39 @@
   </si>
   <si>
     <t xml:space="preserve">Remove Row Top 4 of Zero </t>
+  </si>
+  <si>
+    <t>Unique identifier for each seller. Used as primary key to link with orders and products.</t>
+  </si>
+  <si>
+    <t>Seller_Name</t>
+  </si>
+  <si>
+    <t>Name of the seller or company. Useful for reporting, dashboards, and seller analysis.</t>
+  </si>
+  <si>
+    <t>Seller_Postal_Code</t>
+  </si>
+  <si>
+    <t>Postal code of the seller’s location. Helps in geographical analysis and logistics planning.</t>
+  </si>
+  <si>
+    <t>Seller_City</t>
+  </si>
+  <si>
+    <t>City where the seller is located. Useful for city-level reporting and mapping.</t>
+  </si>
+  <si>
+    <t>Country_Code</t>
+  </si>
+  <si>
+    <t>ISO code of the seller’s country (e.g., DE, ES). Useful for country-level aggregation.</t>
+  </si>
+  <si>
+    <t>Seller_Country</t>
+  </si>
+  <si>
+    <t>Full name of the country of the seller. Helps in dashboards, maps, and regional analysis.</t>
   </si>
 </sst>
 </file>
@@ -1013,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86A2538-5635-4BDC-9780-4AA41F00BE4C}">
   <dimension ref="B4:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1027,16 +1057,16 @@
   <sheetData>
     <row r="4" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1044,13 +1074,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1058,13 +1088,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1072,13 +1102,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1086,13 +1116,13 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1100,13 +1130,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="31.2" x14ac:dyDescent="0.3">
@@ -1114,13 +1144,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1128,13 +1158,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1142,13 +1172,13 @@
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1156,13 +1186,13 @@
         <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1175,7 +1205,7 @@
   <dimension ref="B4:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1187,13 +1217,13 @@
   <sheetData>
     <row r="4" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1201,10 +1231,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1212,10 +1242,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
@@ -1223,10 +1253,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1234,10 +1264,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1245,10 +1275,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1256,10 +1286,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1267,10 +1297,10 @@
         <v>7</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1278,10 +1308,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1291,10 +1321,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035EC863-7662-4F46-A1E6-DDC33702C1E8}">
-  <dimension ref="B3:F97"/>
+  <dimension ref="B3:F103"/>
   <sheetViews>
-    <sheetView topLeftCell="B72" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1308,21 +1338,21 @@
   <sheetData>
     <row r="3" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B3" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1330,10 +1360,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1341,10 +1371,10 @@
         <v>2</v>
       </c>
       <c r="D6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1352,10 +1382,10 @@
         <v>3</v>
       </c>
       <c r="D7" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1363,10 +1393,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1374,10 +1404,10 @@
         <v>5</v>
       </c>
       <c r="D9" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1385,10 +1415,10 @@
         <v>6</v>
       </c>
       <c r="D10" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1396,10 +1426,10 @@
         <v>7</v>
       </c>
       <c r="D11" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1407,10 +1437,10 @@
         <v>8</v>
       </c>
       <c r="D12" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1418,10 +1448,10 @@
         <v>9</v>
       </c>
       <c r="D13" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1429,29 +1459,29 @@
         <v>10</v>
       </c>
       <c r="D14" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B19" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
@@ -1459,10 +1489,10 @@
         <v>1</v>
       </c>
       <c r="D21" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1470,10 +1500,10 @@
         <v>2</v>
       </c>
       <c r="D22" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1481,10 +1511,10 @@
         <v>3</v>
       </c>
       <c r="D23" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1492,10 +1522,10 @@
         <v>4</v>
       </c>
       <c r="D24" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1503,29 +1533,29 @@
         <v>5</v>
       </c>
       <c r="D25" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B30" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1533,10 +1563,10 @@
         <v>1</v>
       </c>
       <c r="D32" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1544,10 +1574,10 @@
         <v>2</v>
       </c>
       <c r="D33" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1555,10 +1585,10 @@
         <v>3</v>
       </c>
       <c r="D34" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="35" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
@@ -1566,10 +1596,10 @@
         <v>4</v>
       </c>
       <c r="D35" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="36" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
@@ -1577,10 +1607,10 @@
         <v>5</v>
       </c>
       <c r="D36" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1588,10 +1618,10 @@
         <v>6</v>
       </c>
       <c r="D37" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1599,29 +1629,29 @@
         <v>7</v>
       </c>
       <c r="D38" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B43" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C44" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1629,10 +1659,10 @@
         <v>1</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1640,10 +1670,10 @@
         <v>2</v>
       </c>
       <c r="D46" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="47" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1651,10 +1681,10 @@
         <v>3</v>
       </c>
       <c r="D47" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="48" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1662,10 +1692,10 @@
         <v>4</v>
       </c>
       <c r="D48" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="49" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1673,29 +1703,29 @@
         <v>5</v>
       </c>
       <c r="D49" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B54" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C55" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1703,13 +1733,13 @@
         <v>1</v>
       </c>
       <c r="D56" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E56" s="5" t="s">
-        <v>119</v>
-      </c>
       <c r="F56" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1717,13 +1747,13 @@
         <v>2</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1731,13 +1761,13 @@
         <v>3</v>
       </c>
       <c r="D58" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="E58" s="5" t="s">
-        <v>122</v>
-      </c>
       <c r="F58" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1745,13 +1775,13 @@
         <v>4</v>
       </c>
       <c r="D59" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="E59" s="5" t="s">
-        <v>124</v>
-      </c>
       <c r="F59" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="60" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1759,13 +1789,13 @@
         <v>5</v>
       </c>
       <c r="D60" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E60" s="5" t="s">
-        <v>126</v>
-      </c>
       <c r="F60" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="61" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1773,13 +1803,13 @@
         <v>6</v>
       </c>
       <c r="D61" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E61" s="5" t="s">
-        <v>128</v>
-      </c>
       <c r="F61" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1787,32 +1817,32 @@
         <v>7</v>
       </c>
       <c r="D62" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E62" s="5" t="s">
-        <v>130</v>
-      </c>
       <c r="F62" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="67" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B67" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C68" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1820,10 +1850,10 @@
         <v>1</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F69" s="11"/>
     </row>
@@ -1832,10 +1862,10 @@
         <v>2</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F70" s="11"/>
     </row>
@@ -1844,10 +1874,10 @@
         <v>3</v>
       </c>
       <c r="D71" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>139</v>
       </c>
       <c r="F71" s="11"/>
     </row>
@@ -1856,10 +1886,10 @@
         <v>4</v>
       </c>
       <c r="D72" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E72" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="F72" s="11"/>
     </row>
@@ -1868,10 +1898,10 @@
         <v>5</v>
       </c>
       <c r="D73" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="E73" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>143</v>
       </c>
       <c r="F73" s="11"/>
     </row>
@@ -1880,10 +1910,10 @@
         <v>6</v>
       </c>
       <c r="D74" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="E74" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>145</v>
       </c>
       <c r="F74" s="11"/>
     </row>
@@ -1892,10 +1922,10 @@
         <v>7</v>
       </c>
       <c r="D75" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E75" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>147</v>
       </c>
       <c r="F75" s="11"/>
     </row>
@@ -1904,30 +1934,30 @@
         <v>8</v>
       </c>
       <c r="D76" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E76" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="F76" s="11"/>
     </row>
     <row r="82" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B82" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C83" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="84" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -1935,10 +1965,10 @@
         <v>1</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F84" s="15"/>
     </row>
@@ -1947,10 +1977,10 @@
         <v>2</v>
       </c>
       <c r="D85" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="E85" s="5" t="s">
         <v>152</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>153</v>
       </c>
       <c r="F85" s="15"/>
     </row>
@@ -1959,10 +1989,10 @@
         <v>3</v>
       </c>
       <c r="D86" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="E86" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>155</v>
       </c>
       <c r="F86" s="15"/>
     </row>
@@ -1971,10 +2001,10 @@
         <v>4</v>
       </c>
       <c r="D87" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="E87" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>157</v>
       </c>
       <c r="F87" s="15"/>
     </row>
@@ -1983,10 +2013,10 @@
         <v>5</v>
       </c>
       <c r="D88" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="E88" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>159</v>
       </c>
       <c r="F88" s="15"/>
     </row>
@@ -1995,31 +2025,103 @@
         <v>6</v>
       </c>
       <c r="D89" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="E89" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>161</v>
       </c>
       <c r="F89" s="15"/>
     </row>
     <row r="96" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B96" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C97" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>132</v>
-      </c>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="98" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C98" s="14">
+        <v>1</v>
+      </c>
+      <c r="D98" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F98" s="11"/>
+    </row>
+    <row r="99" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C99" s="14">
+        <v>2</v>
+      </c>
+      <c r="D99" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F99" s="11"/>
+    </row>
+    <row r="100" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C100" s="14">
+        <v>3</v>
+      </c>
+      <c r="D100" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F100" s="11"/>
+    </row>
+    <row r="101" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C101" s="14">
+        <v>4</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="F101" s="11"/>
+    </row>
+    <row r="102" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C102" s="14">
+        <v>5</v>
+      </c>
+      <c r="D102" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F102" s="11"/>
+    </row>
+    <row r="103" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C103" s="14">
+        <v>6</v>
+      </c>
+      <c r="D103" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F103" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2029,10 +2131,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05F3B95-CD15-4EA0-ACD4-4067EC5DC14D}">
-  <dimension ref="B2:K79"/>
+  <dimension ref="B2:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D61" workbookViewId="0">
-      <selection activeCell="H79" sqref="H79"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2051,37 +2153,37 @@
   <sheetData>
     <row r="2" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="C2" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2089,7 +2191,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5" s="11">
         <v>0</v>
@@ -2118,7 +2220,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" s="11">
         <v>1</v>
@@ -2148,7 +2250,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="11">
         <v>2</v>
@@ -2178,7 +2280,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" s="11">
         <v>3</v>
@@ -2206,10 +2308,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="11">
         <v>4</v>
@@ -2240,10 +2342,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="11">
         <v>5</v>
@@ -2284,7 +2386,7 @@
     <row r="14" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B14" s="12"/>
       <c r="C14" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2292,32 +2394,32 @@
     </row>
     <row r="16" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F16" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="H16" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="I16" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="J16" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="K16" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="17" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2325,7 +2427,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E17" s="11">
         <v>0</v>
@@ -2354,7 +2456,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E18" s="11">
         <v>1</v>
@@ -2384,7 +2486,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E19" s="11">
         <v>2</v>
@@ -2412,7 +2514,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E20" s="11">
         <v>3</v>
@@ -2443,7 +2545,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E21" s="11">
         <v>4</v>
@@ -2484,37 +2586,37 @@
     </row>
     <row r="26" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="C26" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F28" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="H28" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="I28" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="I28" s="10" t="s">
+      <c r="J28" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J28" s="10" t="s">
+      <c r="K28" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="K28" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="29" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2522,7 +2624,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E29" s="11">
         <v>0</v>
@@ -2551,7 +2653,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E30" s="11">
         <v>1</v>
@@ -2582,7 +2684,7 @@
         <v>2</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E31" s="11">
         <v>2</v>
@@ -2612,7 +2714,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E32" s="11">
         <v>3</v>
@@ -2642,10 +2744,10 @@
         <v>4</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E33" s="11">
         <v>4</v>
@@ -2687,36 +2789,36 @@
     </row>
     <row r="38" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="C38" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B39" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="E39" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F39" s="9" t="s">
+      <c r="G39" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="H39" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="H39" s="9" t="s">
+      <c r="I39" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="I39" s="10" t="s">
+      <c r="J39" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J39" s="10" t="s">
+      <c r="K39" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="K39" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="40" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2724,7 +2826,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E40" s="11">
         <v>0</v>
@@ -2753,7 +2855,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E41" s="11">
         <v>1</v>
@@ -2783,7 +2885,7 @@
         <v>2</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E42" s="11">
         <v>2</v>
@@ -2813,7 +2915,7 @@
         <v>3</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E43" s="11">
         <v>3</v>
@@ -2854,36 +2956,36 @@
     </row>
     <row r="48" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="C48" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B49" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="E49" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F49" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E49" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F49" s="9" t="s">
+      <c r="G49" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="H49" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="H49" s="9" t="s">
+      <c r="I49" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="I49" s="10" t="s">
+      <c r="J49" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J49" s="10" t="s">
+      <c r="K49" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="K49" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="50" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -2891,7 +2993,7 @@
         <v>0</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E50" s="11">
         <v>0</v>
@@ -2920,7 +3022,7 @@
         <v>1</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E51" s="11">
         <v>1</v>
@@ -2951,7 +3053,7 @@
         <v>2</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E52" s="11">
         <v>2</v>
@@ -2982,7 +3084,7 @@
         <v>3</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E53" s="11">
         <v>3</v>
@@ -3013,10 +3115,10 @@
         <v>4</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E54" s="11">
         <v>4</v>
@@ -3047,10 +3149,10 @@
         <v>5</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D55" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E55" s="11">
         <v>5</v>
@@ -3092,36 +3194,36 @@
     </row>
     <row r="61" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="C61" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B62" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="E62" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F62" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E62" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F62" s="9" t="s">
+      <c r="G62" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G62" s="9" t="s">
+      <c r="H62" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="H62" s="9" t="s">
+      <c r="I62" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="I62" s="10" t="s">
+      <c r="J62" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J62" s="10" t="s">
+      <c r="K62" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="K62" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="63" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -3129,7 +3231,7 @@
         <v>0</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E63" s="15">
         <v>0</v>
@@ -3158,7 +3260,7 @@
         <v>1</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E64" s="15">
         <v>1</v>
@@ -3188,7 +3290,7 @@
         <v>2</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E65" s="15">
         <v>2</v>
@@ -3218,7 +3320,7 @@
         <v>3</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E66" s="15">
         <v>3</v>
@@ -3259,36 +3361,36 @@
     </row>
     <row r="71" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
       <c r="C71" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B72" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C72" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="E72" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F72" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E72" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F72" s="9" t="s">
+      <c r="G72" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G72" s="9" t="s">
+      <c r="H72" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="H72" s="9" t="s">
+      <c r="I72" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="I72" s="10" t="s">
+      <c r="J72" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J72" s="10" t="s">
+      <c r="K72" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="K72" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -3296,7 +3398,7 @@
         <v>0</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E73" s="11">
         <v>0</v>
@@ -3325,7 +3427,7 @@
         <v>1</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E74" s="11">
         <v>1</v>
@@ -3355,7 +3457,7 @@
         <v>2</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E75" s="11">
         <v>2</v>
@@ -3385,7 +3487,7 @@
         <v>3</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E76" s="11">
         <v>3</v>
@@ -3415,10 +3517,10 @@
         <v>4</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D77" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E77" s="11">
         <v>4</v>
@@ -3449,10 +3551,10 @@
         <v>5</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D78" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E78" s="11">
         <v>5</v>
@@ -3491,6 +3593,173 @@
       <c r="I79" s="11"/>
       <c r="J79" s="11"/>
       <c r="K79" s="11"/>
+    </row>
+    <row r="83" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="C83" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B84" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H84" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I84" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J84" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K84" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B85" s="11">
+        <v>0</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E85" s="11">
+        <v>0</v>
+      </c>
+      <c r="F85" s="11">
+        <v>3095</v>
+      </c>
+      <c r="G85" s="11">
+        <v>3095</v>
+      </c>
+      <c r="H85" s="11">
+        <v>0</v>
+      </c>
+      <c r="I85" s="11">
+        <v>6</v>
+      </c>
+      <c r="J85" s="11">
+        <v>6</v>
+      </c>
+      <c r="K85" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B86" s="11">
+        <v>1</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E86" s="11">
+        <v>1</v>
+      </c>
+      <c r="F86" s="11">
+        <f>G85</f>
+        <v>3095</v>
+      </c>
+      <c r="G86" s="11">
+        <v>3095</v>
+      </c>
+      <c r="H86" s="11">
+        <v>0</v>
+      </c>
+      <c r="I86" s="11">
+        <v>6</v>
+      </c>
+      <c r="J86" s="11">
+        <v>6</v>
+      </c>
+      <c r="K86" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B87" s="11">
+        <v>2</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E87" s="11">
+        <v>2</v>
+      </c>
+      <c r="F87" s="11">
+        <f>G86</f>
+        <v>3095</v>
+      </c>
+      <c r="G87" s="11">
+        <v>3095</v>
+      </c>
+      <c r="H87" s="11">
+        <v>0</v>
+      </c>
+      <c r="I87" s="11">
+        <v>6</v>
+      </c>
+      <c r="J87" s="11">
+        <v>6</v>
+      </c>
+      <c r="K87" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B88" s="11">
+        <v>3</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E88" s="11">
+        <v>3</v>
+      </c>
+      <c r="F88" s="11">
+        <f>G87</f>
+        <v>3095</v>
+      </c>
+      <c r="G88" s="11">
+        <v>3095</v>
+      </c>
+      <c r="H88" s="11">
+        <v>0</v>
+      </c>
+      <c r="I88" s="11">
+        <v>6</v>
+      </c>
+      <c r="J88" s="11">
+        <v>6</v>
+      </c>
+      <c r="K88" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E89" s="11">
+        <v>4</v>
+      </c>
+      <c r="F89" s="11">
+        <f>G88</f>
+        <v>3095</v>
+      </c>
+      <c r="G89" s="11"/>
+      <c r="H89" s="11"/>
+      <c r="I89" s="11"/>
+      <c r="J89" s="11"/>
+      <c r="K89" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3501,7 +3770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7DB601-2E61-4816-8642-3B30D49A003A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>

<commit_message>
Work on Excel Report & Rename Some Columns
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA037218-847A-4F1A-8E72-363E889D32B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463A294E-6CBC-4477-BE4E-62EF66EB4AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="4" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="2" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
   <sheets>
     <sheet name="Data &amp; Purpose" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="205">
   <si>
     <t>Table Name</t>
   </si>
@@ -437,12 +437,6 @@
     <t>After Column Name</t>
   </si>
   <si>
-    <t>Review_Title</t>
-  </si>
-  <si>
-    <t>Review_Message</t>
-  </si>
-  <si>
     <t>Before Column Name</t>
   </si>
   <si>
@@ -558,13 +552,115 @@
   </si>
   <si>
     <t>Full name of the country of the seller. Helps in dashboards, maps, and regional analysis.</t>
+  </si>
+  <si>
+    <t>Customer ID</t>
+  </si>
+  <si>
+    <t>Subscription Date</t>
+  </si>
+  <si>
+    <t>First Order Date</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Order ID</t>
+  </si>
+  <si>
+    <t>Product ID</t>
+  </si>
+  <si>
+    <t>Seller ID</t>
+  </si>
+  <si>
+    <t>Item Price</t>
+  </si>
+  <si>
+    <t>Shipping Cost</t>
+  </si>
+  <si>
+    <t>Shipping Deadline</t>
+  </si>
+  <si>
+    <t>Payment Method</t>
+  </si>
+  <si>
+    <t>Installments</t>
+  </si>
+  <si>
+    <t>Payment Amount</t>
+  </si>
+  <si>
+    <t>Review ID</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Review Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Order Date</t>
+  </si>
+  <si>
+    <t>Delivery Date</t>
+  </si>
+  <si>
+    <t>Estimated Delivery Date</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Weight (g)</t>
+  </si>
+  <si>
+    <t>Length (cm)</t>
+  </si>
+  <si>
+    <t>Height (cm)</t>
+  </si>
+  <si>
+    <t>Width (cm)</t>
+  </si>
+  <si>
+    <t>Seller Name</t>
+  </si>
+  <si>
+    <t>Remove Column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove Column </t>
+  </si>
+  <si>
+    <t>Perform Activity</t>
+  </si>
+  <si>
+    <t>Data Wrangling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -603,8 +699,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -659,6 +763,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -687,7 +809,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -725,8 +847,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1205,7 +1348,7 @@
   <dimension ref="B4:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C6" sqref="C6:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1321,10 +1464,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035EC863-7662-4F46-A1E6-DDC33702C1E8}">
-  <dimension ref="B3:F103"/>
+  <dimension ref="B3:H103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1334,28 +1477,33 @@
     <col min="4" max="4" width="26.6640625" customWidth="1"/>
     <col min="5" max="5" width="51" customWidth="1"/>
     <col min="6" max="6" width="34.21875" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B3" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C5" s="5">
         <v>1</v>
       </c>
@@ -1365,8 +1513,14 @@
       <c r="E5" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C6" s="5">
         <v>2</v>
       </c>
@@ -1376,8 +1530,14 @@
       <c r="E6" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G6" s="5">
+        <v>2</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C7" s="5">
         <v>3</v>
       </c>
@@ -1387,8 +1547,14 @@
       <c r="E7" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G7" s="5">
+        <v>3</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="5">
         <v>4</v>
       </c>
@@ -1398,8 +1564,14 @@
       <c r="E8" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G8" s="5">
+        <v>4</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C9" s="5">
         <v>5</v>
       </c>
@@ -1409,8 +1581,14 @@
       <c r="E9" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G9" s="5">
+        <v>5</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C10" s="5">
         <v>6</v>
       </c>
@@ -1420,8 +1598,14 @@
       <c r="E10" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G10" s="5">
+        <v>6</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C11" s="5">
         <v>7</v>
       </c>
@@ -1431,8 +1615,14 @@
       <c r="E11" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G11" s="5">
+        <v>7</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C12" s="5">
         <v>8</v>
       </c>
@@ -1442,8 +1632,14 @@
       <c r="E12" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G12" s="5">
+        <v>8</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C13" s="5">
         <v>9</v>
       </c>
@@ -1454,7 +1650,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C14" s="5">
         <v>10</v>
       </c>
@@ -1465,26 +1661,29 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B19" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
         <v>67</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C21" s="5">
         <v>1</v>
       </c>
@@ -1494,8 +1693,14 @@
       <c r="E21" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G21" s="17">
+        <v>1</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C22" s="5">
         <v>2</v>
       </c>
@@ -1505,8 +1710,14 @@
       <c r="E22" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G22" s="17">
+        <v>2</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C23" s="5">
         <v>3</v>
       </c>
@@ -1516,8 +1727,14 @@
       <c r="E23" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G23" s="17">
+        <v>3</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C24" s="5">
         <v>4</v>
       </c>
@@ -1527,8 +1744,14 @@
       <c r="E24" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G24" s="17">
+        <v>4</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C25" s="5">
         <v>5</v>
       </c>
@@ -1538,27 +1761,36 @@
       <c r="E25" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="G25" s="17">
+        <v>5</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B30" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C31" s="3" t="s">
         <v>67</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="G31" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H31" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C32" s="5">
         <v>1</v>
       </c>
@@ -1568,8 +1800,14 @@
       <c r="E32" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G32" s="17">
+        <v>1</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C33" s="5">
         <v>2</v>
       </c>
@@ -1579,8 +1817,14 @@
       <c r="E33" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G33" s="17">
+        <v>2</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C34" s="5">
         <v>3</v>
       </c>
@@ -1590,8 +1834,14 @@
       <c r="E34" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="G34" s="17">
+        <v>3</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C35" s="5">
         <v>4</v>
       </c>
@@ -1601,8 +1851,14 @@
       <c r="E35" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="G35" s="17">
+        <v>4</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C36" s="5">
         <v>5</v>
       </c>
@@ -1612,8 +1868,14 @@
       <c r="E36" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G36" s="17">
+        <v>5</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C37" s="5">
         <v>6</v>
       </c>
@@ -1623,8 +1885,14 @@
       <c r="E37" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G37" s="17">
+        <v>6</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C38" s="5">
         <v>7</v>
       </c>
@@ -1635,26 +1903,29 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B43" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C44" s="3" t="s">
         <v>67</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="G44" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H44" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C45" s="5">
         <v>1</v>
       </c>
@@ -1664,8 +1935,14 @@
       <c r="E45" s="5" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="46" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G45" s="17">
+        <v>1</v>
+      </c>
+      <c r="H45" s="18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C46" s="5">
         <v>2</v>
       </c>
@@ -1675,8 +1952,14 @@
       <c r="E46" s="5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="47" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G46" s="17">
+        <v>2</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C47" s="5">
         <v>3</v>
       </c>
@@ -1686,8 +1969,14 @@
       <c r="E47" s="5" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="48" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G47" s="17">
+        <v>3</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C48" s="5">
         <v>4</v>
       </c>
@@ -1697,8 +1986,14 @@
       <c r="E48" s="5" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="49" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G48" s="17">
+        <v>4</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C49" s="5">
         <v>5</v>
       </c>
@@ -1709,26 +2004,29 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B54" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C55" s="3" t="s">
         <v>67</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="G55" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H55" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="56" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C56" s="5">
         <v>1</v>
       </c>
@@ -1738,11 +2036,14 @@
       <c r="E56" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="F56" s="14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G56" s="17">
+        <v>1</v>
+      </c>
+      <c r="H56" s="18" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C57" s="5">
         <v>2</v>
       </c>
@@ -1752,11 +2053,14 @@
       <c r="E57" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F57" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G57" s="17">
+        <v>2</v>
+      </c>
+      <c r="H57" s="18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C58" s="5">
         <v>3</v>
       </c>
@@ -1766,11 +2070,14 @@
       <c r="E58" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="F58" s="14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G58" s="17">
+        <v>3</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C59" s="5">
         <v>4</v>
       </c>
@@ -1780,11 +2087,14 @@
       <c r="E59" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F59" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G59" s="17">
+        <v>4</v>
+      </c>
+      <c r="H59" s="18" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C60" s="5">
         <v>5</v>
       </c>
@@ -1794,11 +2104,8 @@
       <c r="E60" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="F60" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C61" s="5">
         <v>6</v>
       </c>
@@ -1808,11 +2115,8 @@
       <c r="E61" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="F61" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C62" s="5">
         <v>7</v>
       </c>
@@ -1822,30 +2126,30 @@
       <c r="E62" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="F62" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="67" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B67" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C68" s="3" t="s">
         <v>67</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F68" s="3" t="s">
+      <c r="G68" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H68" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C69" s="14">
         <v>1</v>
       </c>
@@ -1853,11 +2157,16 @@
         <v>93</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="F69" s="11"/>
-    </row>
-    <row r="70" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+      <c r="G69" s="17">
+        <v>1</v>
+      </c>
+      <c r="H69" s="18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C70" s="14">
         <v>2</v>
       </c>
@@ -1865,102 +2174,128 @@
         <v>47</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="F70" s="11"/>
-    </row>
-    <row r="71" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+      <c r="G70" s="17">
+        <v>2</v>
+      </c>
+      <c r="H70" s="18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C71" s="14">
         <v>3</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F71" s="11"/>
-    </row>
-    <row r="72" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+      <c r="G71" s="17">
+        <v>3</v>
+      </c>
+      <c r="H71" s="18" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C72" s="14">
         <v>4</v>
       </c>
       <c r="D72" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G72" s="17">
+        <v>4</v>
+      </c>
+      <c r="H72" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C73" s="14">
+        <v>5</v>
+      </c>
+      <c r="D73" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="E72" s="5" t="s">
+      <c r="E73" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="F72" s="11"/>
-    </row>
-    <row r="73" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="C73" s="14">
-        <v>5</v>
-      </c>
-      <c r="D73" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="F73" s="11"/>
-    </row>
-    <row r="74" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G73" s="17">
+        <v>5</v>
+      </c>
+      <c r="H73" s="18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C74" s="14">
         <v>6</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="F74" s="11"/>
-    </row>
-    <row r="75" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+      <c r="G74" s="17">
+        <v>6</v>
+      </c>
+      <c r="H74" s="18" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C75" s="14">
         <v>7</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="F75" s="11"/>
-    </row>
-    <row r="76" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C76" s="14">
         <v>8</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="F76" s="11"/>
-    </row>
-    <row r="82" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B82" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C83" s="3" t="s">
         <v>67</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F83" s="3" t="s">
+      <c r="G83" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H83" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="84" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C84" s="14">
         <v>1</v>
       </c>
@@ -1968,90 +2303,123 @@
         <v>97</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F84" s="15"/>
-    </row>
-    <row r="85" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+      <c r="G84" s="17">
+        <v>1</v>
+      </c>
+      <c r="H84" s="18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C85" s="14">
         <v>2</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="F85" s="15"/>
-    </row>
-    <row r="86" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+      <c r="G85" s="17">
+        <v>2</v>
+      </c>
+      <c r="H85" s="18" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C86" s="14">
         <v>3</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F86" s="15"/>
-    </row>
-    <row r="87" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+      <c r="G86" s="17">
+        <v>3</v>
+      </c>
+      <c r="H86" s="18" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C87" s="14">
         <v>4</v>
       </c>
       <c r="D87" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G87" s="17">
+        <v>4</v>
+      </c>
+      <c r="H87" s="18" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C88" s="14">
+        <v>5</v>
+      </c>
+      <c r="D88" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="E87" s="5" t="s">
+      <c r="E88" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="F87" s="15"/>
-    </row>
-    <row r="88" spans="2:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="C88" s="14">
-        <v>5</v>
-      </c>
-      <c r="D88" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F88" s="15"/>
-    </row>
-    <row r="89" spans="2:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G88" s="17">
+        <v>5</v>
+      </c>
+      <c r="H88" s="18" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C89" s="14">
         <v>6</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="F89" s="15"/>
-    </row>
-    <row r="96" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
+        <v>158</v>
+      </c>
+      <c r="G89" s="17">
+        <v>6</v>
+      </c>
+      <c r="H89" s="18" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B96" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C97" s="3" t="s">
         <v>67</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F97" s="3" t="s">
+      <c r="G97" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H97" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="98" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="98" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C98" s="14">
         <v>1</v>
       </c>
@@ -2059,69 +2427,93 @@
         <v>99</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="F98" s="11"/>
-    </row>
-    <row r="99" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+      <c r="G98" s="11">
+        <v>1</v>
+      </c>
+      <c r="H98" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="99" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C99" s="14">
         <v>2</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="F99" s="11"/>
-    </row>
-    <row r="100" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+      <c r="G99" s="11">
+        <v>2</v>
+      </c>
+      <c r="H99" s="16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="100" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C100" s="14">
         <v>3</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="F100" s="11"/>
-    </row>
-    <row r="101" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+      <c r="G100" s="11">
+        <v>3</v>
+      </c>
+      <c r="H100" s="16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="101" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C101" s="14">
         <v>4</v>
       </c>
       <c r="D101" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G101" s="11">
+        <v>4</v>
+      </c>
+      <c r="H101" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="102" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C102" s="14">
+        <v>5</v>
+      </c>
+      <c r="D102" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="E101" s="5" t="s">
+      <c r="E102" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="F101" s="11"/>
-    </row>
-    <row r="102" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="C102" s="14">
-        <v>5</v>
-      </c>
-      <c r="D102" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="E102" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F102" s="11"/>
-    </row>
-    <row r="103" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G102" s="11">
+        <v>5</v>
+      </c>
+      <c r="H102" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="103" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C103" s="14">
         <v>6</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="F103" s="11"/>
+        <v>170</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2131,17 +2523,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05F3B95-CD15-4EA0-ACD4-4067EC5DC14D}">
-  <dimension ref="B2:K89"/>
+  <dimension ref="A2:M98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="Q89" sqref="Q89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.6640625" customWidth="1"/>
     <col min="7" max="7" width="26.33203125" customWidth="1"/>
@@ -2151,12 +2543,12 @@
     <col min="11" max="11" width="33.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="C2" s="13" t="s">
+    <row r="2" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="C2" s="23" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>67</v>
       </c>
@@ -2186,7 +2578,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="11">
         <v>0</v>
       </c>
@@ -2215,7 +2607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="11">
         <v>1</v>
       </c>
@@ -2245,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="11">
         <v>2</v>
       </c>
@@ -2275,7 +2667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="11">
         <v>3</v>
       </c>
@@ -2303,7 +2695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="11">
         <v>4</v>
       </c>
@@ -2337,7 +2729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="11">
         <v>5</v>
       </c>
@@ -2371,134 +2763,160 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-    </row>
-    <row r="12" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-    </row>
-    <row r="13" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-    </row>
-    <row r="14" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B14" s="12"/>
-      <c r="C14" s="13" t="s">
+    <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="11">
+        <v>6</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="19">
+        <v>6</v>
+      </c>
+      <c r="F11" s="19">
+        <f>G10</f>
+        <v>99441</v>
+      </c>
+      <c r="G11" s="19">
+        <v>99441</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="19">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J11" s="19">
+        <v>9</v>
+      </c>
+      <c r="K11" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="11">
+        <v>7</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="19">
+        <v>7</v>
+      </c>
+      <c r="F12" s="19">
+        <f>G11</f>
+        <v>99441</v>
+      </c>
+      <c r="G12" s="19">
+        <v>99441</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0</v>
+      </c>
+      <c r="I12" s="19">
+        <v>9</v>
+      </c>
+      <c r="J12" s="19">
+        <v>8</v>
+      </c>
+      <c r="K12" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+    </row>
+    <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="12"/>
-    </row>
-    <row r="16" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="6" t="s">
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B16" s="12"/>
+      <c r="C16" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="12"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B18" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8" t="s">
+      <c r="D18" s="7"/>
+      <c r="E18" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F18" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G18" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H18" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I18" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J18" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="K16" s="10" t="s">
+      <c r="K18" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="11">
-        <v>0</v>
-      </c>
-      <c r="C17" s="11" t="s">
+    <row r="19" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B19" s="11">
+        <v>0</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="11">
-        <v>0</v>
-      </c>
-      <c r="F17" s="11">
-        <v>1000163</v>
-      </c>
-      <c r="G17" s="11">
-        <v>1000163</v>
-      </c>
-      <c r="H17" s="11">
-        <v>0</v>
-      </c>
-      <c r="I17" s="11">
-        <v>5</v>
-      </c>
-      <c r="J17" s="11">
-        <v>5</v>
-      </c>
-      <c r="K17" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B18" s="11">
-        <v>1</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="11">
-        <v>1</v>
-      </c>
-      <c r="F18" s="11">
-        <f>G17</f>
-        <v>1000163</v>
-      </c>
-      <c r="G18" s="11">
-        <v>1000163</v>
-      </c>
-      <c r="H18" s="11">
-        <v>0</v>
-      </c>
-      <c r="I18" s="11">
-        <v>5</v>
-      </c>
-      <c r="J18" s="11">
-        <v>5</v>
-      </c>
-      <c r="K18" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="11">
-        <v>2</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>78</v>
-      </c>
       <c r="E19" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F19" s="11">
-        <f>G18</f>
         <v>1000163</v>
       </c>
       <c r="G19" s="11">
         <v>1000163</v>
       </c>
-      <c r="H19" s="11"/>
+      <c r="H19" s="11">
+        <v>0</v>
+      </c>
       <c r="I19" s="11">
         <v>5</v>
       </c>
@@ -2509,26 +2927,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E20" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F20" s="11">
         <f>G19</f>
         <v>1000163</v>
       </c>
       <c r="G20" s="11">
-        <v>1686</v>
+        <v>1000163</v>
       </c>
       <c r="H20" s="11">
-        <f>F20-G20</f>
-        <v>998477</v>
+        <v>0</v>
       </c>
       <c r="I20" s="11">
         <v>5</v>
@@ -2540,26 +2957,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E21" s="11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F21" s="11">
         <f>G20</f>
-        <v>1686</v>
+        <v>1000163</v>
       </c>
       <c r="G21" s="11">
-        <v>1685</v>
-      </c>
-      <c r="H21" s="11">
-        <v>1</v>
-      </c>
+        <v>1000163</v>
+      </c>
+      <c r="H21" s="11"/>
       <c r="I21" s="11">
         <v>5</v>
       </c>
@@ -2570,103 +2985,134 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B22" s="11">
+        <v>3</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>79</v>
+      </c>
       <c r="E22" s="11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F22" s="11">
         <f>G21</f>
+        <v>1000163</v>
+      </c>
+      <c r="G22" s="11">
+        <v>1686</v>
+      </c>
+      <c r="H22" s="11">
+        <f>F22-G22</f>
+        <v>998477</v>
+      </c>
+      <c r="I22" s="11">
+        <v>5</v>
+      </c>
+      <c r="J22" s="11">
+        <v>5</v>
+      </c>
+      <c r="K22" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="11">
+        <v>4</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="11">
+        <v>4</v>
+      </c>
+      <c r="F23" s="11">
+        <f>G22</f>
+        <v>1686</v>
+      </c>
+      <c r="G23" s="11">
         <v>1685</v>
       </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-    </row>
-    <row r="26" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="C26" s="13" t="s">
+      <c r="H23" s="11">
+        <v>1</v>
+      </c>
+      <c r="I23" s="11">
+        <v>5</v>
+      </c>
+      <c r="J23" s="11">
+        <v>5</v>
+      </c>
+      <c r="K23" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+    </row>
+    <row r="27" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="C27" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B28" s="6" t="s">
+    <row r="29" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B29" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="8" t="s">
+      <c r="D29" s="7"/>
+      <c r="E29" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F29" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G29" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="H29" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I28" s="10" t="s">
+      <c r="I29" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="J28" s="10" t="s">
+      <c r="J29" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="K28" s="10" t="s">
+      <c r="K29" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B29" s="11">
-        <v>0</v>
-      </c>
-      <c r="C29" s="11" t="s">
+    <row r="30" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B30" s="11">
+        <v>0</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E29" s="11">
-        <v>0</v>
-      </c>
-      <c r="F29" s="11">
-        <v>112650</v>
-      </c>
-      <c r="G29" s="11">
-        <v>112650</v>
-      </c>
-      <c r="H29" s="11">
-        <v>0</v>
-      </c>
-      <c r="I29" s="11">
-        <v>7</v>
-      </c>
-      <c r="J29" s="11">
-        <v>7</v>
-      </c>
-      <c r="K29" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B30" s="11">
-        <v>1</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>77</v>
-      </c>
       <c r="E30" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" s="11">
-        <f>G29</f>
         <v>112650</v>
       </c>
       <c r="G30" s="11">
         <v>112650</v>
       </c>
       <c r="H30" s="11">
-        <f>F30-G30</f>
         <v>0</v>
       </c>
       <c r="I30" s="11">
@@ -2679,15 +3125,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B31" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E31" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" s="11">
         <f>G30</f>
@@ -2697,6 +3143,7 @@
         <v>112650</v>
       </c>
       <c r="H31" s="11">
+        <f>F31-G31</f>
         <v>0</v>
       </c>
       <c r="I31" s="11">
@@ -2709,15 +3156,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E32" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" s="11">
         <f>G31</f>
@@ -2739,29 +3186,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D33" t="s">
-        <v>93</v>
-      </c>
       <c r="E33" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" s="11">
         <f>G32</f>
         <v>112650</v>
       </c>
       <c r="G33" s="11">
-        <v>98666</v>
+        <v>112650</v>
       </c>
       <c r="H33" s="11">
-        <f>F33-G33</f>
-        <v>13984</v>
+        <v>0</v>
       </c>
       <c r="I33" s="11">
         <v>7</v>
@@ -2773,125 +3216,133 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B34" s="11">
+        <v>4</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" t="s">
+        <v>93</v>
+      </c>
       <c r="E34" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" s="11">
         <f>G33</f>
+        <v>112650</v>
+      </c>
+      <c r="G34" s="11">
         <v>98666</v>
       </c>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-    </row>
-    <row r="38" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="C38" s="13" t="s">
+      <c r="H34" s="11">
+        <f>F34-G34</f>
+        <v>13984</v>
+      </c>
+      <c r="I34" s="11">
+        <v>7</v>
+      </c>
+      <c r="J34" s="11">
+        <v>7</v>
+      </c>
+      <c r="K34" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B35" s="19">
+        <v>5</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="D35" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" s="11">
+        <v>5</v>
+      </c>
+      <c r="F35" s="11">
+        <f>G34</f>
+        <v>98666</v>
+      </c>
+      <c r="G35" s="11">
+        <v>98666</v>
+      </c>
+      <c r="H35" s="11">
+        <v>0</v>
+      </c>
+      <c r="I35" s="11">
+        <v>7</v>
+      </c>
+      <c r="J35" s="11">
+        <v>6</v>
+      </c>
+      <c r="K35" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
+    </row>
+    <row r="39" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="C39" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B39" s="6" t="s">
+    <row r="41" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B41" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C41" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E41" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F41" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="G41" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H39" s="9" t="s">
+      <c r="H41" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I39" s="10" t="s">
+      <c r="I41" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="J39" s="10" t="s">
+      <c r="J41" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="K39" s="10" t="s">
+      <c r="K41" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B40" s="11">
-        <v>0</v>
-      </c>
-      <c r="C40" s="11" t="s">
+    <row r="42" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B42" s="11">
+        <v>0</v>
+      </c>
+      <c r="C42" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E40" s="11">
-        <v>0</v>
-      </c>
-      <c r="F40" s="11">
-        <v>103886</v>
-      </c>
-      <c r="G40" s="11">
-        <v>103886</v>
-      </c>
-      <c r="H40" s="11">
-        <v>0</v>
-      </c>
-      <c r="I40" s="11">
-        <v>5</v>
-      </c>
-      <c r="J40" s="11">
-        <v>5</v>
-      </c>
-      <c r="K40" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B41" s="11">
-        <v>1</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E41" s="11">
-        <v>1</v>
-      </c>
-      <c r="F41" s="11">
-        <f>G40</f>
-        <v>103886</v>
-      </c>
-      <c r="G41" s="11">
-        <v>103886</v>
-      </c>
-      <c r="H41" s="11">
-        <v>0</v>
-      </c>
-      <c r="I41" s="11">
-        <v>5</v>
-      </c>
-      <c r="J41" s="11">
-        <v>5</v>
-      </c>
-      <c r="K41" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B42" s="11">
-        <v>2</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>78</v>
-      </c>
       <c r="E42" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F42" s="11">
-        <f>G41</f>
         <v>103886</v>
       </c>
       <c r="G42" s="11">
@@ -2910,15 +3361,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B43" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E43" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F43" s="11">
         <f>G42</f>
@@ -2940,712 +3391,921 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B44" s="11">
+        <v>2</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>78</v>
+      </c>
       <c r="E44" s="11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F44" s="11">
         <f>G43</f>
         <v>103886</v>
       </c>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="11"/>
-    </row>
-    <row r="48" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="C48" s="13" t="s">
+      <c r="G44" s="11">
+        <v>103886</v>
+      </c>
+      <c r="H44" s="11">
+        <v>0</v>
+      </c>
+      <c r="I44" s="11">
+        <v>5</v>
+      </c>
+      <c r="J44" s="11">
+        <v>5</v>
+      </c>
+      <c r="K44" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B45" s="11">
+        <v>3</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" s="11">
+        <v>3</v>
+      </c>
+      <c r="F45" s="11">
+        <f>G44</f>
+        <v>103886</v>
+      </c>
+      <c r="G45" s="11">
+        <v>103886</v>
+      </c>
+      <c r="H45" s="11">
+        <v>0</v>
+      </c>
+      <c r="I45" s="11">
+        <v>5</v>
+      </c>
+      <c r="J45" s="11">
+        <v>5</v>
+      </c>
+      <c r="K45" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B46" s="19">
+        <v>4</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="D46" t="s">
+        <v>109</v>
+      </c>
+      <c r="E46" s="11">
+        <v>4</v>
+      </c>
+      <c r="F46" s="11">
+        <f>G45</f>
+        <v>103886</v>
+      </c>
+      <c r="G46" s="11">
+        <v>103886</v>
+      </c>
+      <c r="H46" s="11">
+        <v>0</v>
+      </c>
+      <c r="I46" s="11">
+        <v>5</v>
+      </c>
+      <c r="J46" s="11">
+        <v>4</v>
+      </c>
+      <c r="K46" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="22"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
+      <c r="L48" s="22"/>
+      <c r="M48" s="22"/>
+    </row>
+    <row r="50" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="C50" s="23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B49" s="6" t="s">
+    <row r="52" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B52" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C52" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E52" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F52" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="G52" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H49" s="9" t="s">
+      <c r="H52" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I49" s="10" t="s">
+      <c r="I52" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="J49" s="10" t="s">
+      <c r="J52" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="K49" s="10" t="s">
+      <c r="K52" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B50" s="11">
-        <v>0</v>
-      </c>
-      <c r="C50" s="11" t="s">
+    <row r="53" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B53" s="11">
+        <v>0</v>
+      </c>
+      <c r="C53" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E50" s="11">
-        <v>0</v>
-      </c>
-      <c r="F50" s="11">
+      <c r="E53" s="11">
+        <v>0</v>
+      </c>
+      <c r="F53" s="11">
         <v>99329</v>
       </c>
-      <c r="G50" s="11">
+      <c r="G53" s="11">
         <v>99329</v>
       </c>
-      <c r="H50" s="11">
-        <v>0</v>
-      </c>
-      <c r="I50" s="11">
+      <c r="H53" s="11">
+        <v>0</v>
+      </c>
+      <c r="I53" s="11">
         <v>7</v>
       </c>
-      <c r="J50" s="11">
+      <c r="J53" s="11">
         <v>7</v>
       </c>
-      <c r="K50" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B51" s="11">
+      <c r="K53" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B54" s="11">
         <v>1</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C54" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E51" s="11">
+      <c r="E54" s="11">
         <v>1</v>
       </c>
-      <c r="F51" s="11">
-        <f t="shared" ref="F51:F56" si="1">G50</f>
+      <c r="F54" s="11">
+        <f t="shared" ref="F54:F59" si="1">G53</f>
         <v>99329</v>
       </c>
-      <c r="G51" s="11">
+      <c r="G54" s="11">
         <v>99327</v>
       </c>
-      <c r="H51" s="11">
-        <f>F51-G51</f>
+      <c r="H54" s="11">
+        <f>F54-G54</f>
         <v>2</v>
       </c>
-      <c r="I51" s="11">
+      <c r="I54" s="11">
         <v>7</v>
       </c>
-      <c r="J51" s="11">
+      <c r="J54" s="11">
         <v>7</v>
       </c>
-      <c r="K51" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B52" s="11">
+      <c r="K54" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B55" s="11">
         <v>2</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C55" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E52" s="11">
+      <c r="E55" s="11">
         <v>2</v>
       </c>
-      <c r="F52" s="11">
+      <c r="F55" s="11">
         <f t="shared" si="1"/>
         <v>99327</v>
       </c>
-      <c r="G52" s="11">
+      <c r="G55" s="11">
         <v>99268</v>
       </c>
-      <c r="H52" s="11">
-        <f>F52-G52</f>
+      <c r="H55" s="11">
+        <f>F55-G55</f>
         <v>59</v>
       </c>
-      <c r="I52" s="11">
+      <c r="I55" s="11">
         <v>7</v>
       </c>
-      <c r="J52" s="11">
+      <c r="J55" s="11">
         <v>7</v>
       </c>
-      <c r="K52" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B53" s="11">
+      <c r="K55" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B56" s="11">
         <v>3</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C56" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E53" s="11">
+      <c r="E56" s="11">
         <v>3</v>
       </c>
-      <c r="F53" s="11">
+      <c r="F56" s="11">
         <f t="shared" si="1"/>
         <v>99268</v>
       </c>
-      <c r="G53" s="11">
+      <c r="G56" s="11">
         <v>99268</v>
       </c>
-      <c r="H53" s="11">
-        <f>F53-G53</f>
-        <v>0</v>
-      </c>
-      <c r="I53" s="11">
+      <c r="H56" s="11">
+        <f>F56-G56</f>
+        <v>0</v>
+      </c>
+      <c r="I56" s="11">
         <v>7</v>
       </c>
-      <c r="J53" s="11">
+      <c r="J56" s="11">
         <v>7</v>
       </c>
-      <c r="K53" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B54" s="11">
+      <c r="K56" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B57" s="11">
         <v>4</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C57" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D57" t="s">
         <v>93</v>
       </c>
-      <c r="E54" s="11">
+      <c r="E57" s="11">
         <v>4</v>
       </c>
-      <c r="F54" s="11">
+      <c r="F57" s="11">
         <f t="shared" si="1"/>
         <v>99268</v>
       </c>
-      <c r="G54" s="11">
+      <c r="G57" s="11">
         <v>99223</v>
       </c>
-      <c r="H54" s="11">
-        <f>F54-G54</f>
+      <c r="H57" s="11">
+        <f>F57-G57</f>
         <v>45</v>
       </c>
-      <c r="I54" s="11">
+      <c r="I57" s="11">
         <v>7</v>
       </c>
-      <c r="J54" s="11">
+      <c r="J57" s="11">
         <v>7</v>
       </c>
-      <c r="K54" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B55" s="11">
-        <v>5</v>
-      </c>
-      <c r="C55" s="11" t="s">
+      <c r="K57" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B58" s="11">
+        <v>5</v>
+      </c>
+      <c r="C58" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D58" t="s">
         <v>126</v>
       </c>
-      <c r="E55" s="11">
-        <v>5</v>
-      </c>
-      <c r="F55" s="11">
+      <c r="E58" s="11">
+        <v>5</v>
+      </c>
+      <c r="F58" s="11">
         <f t="shared" si="1"/>
         <v>99223</v>
       </c>
-      <c r="G55" s="11">
+      <c r="G58" s="11">
         <v>99221</v>
       </c>
-      <c r="H55" s="11">
-        <f>F55-G55</f>
+      <c r="H58" s="11">
+        <f>F58-G58</f>
         <v>2</v>
       </c>
-      <c r="I55" s="11">
+      <c r="I58" s="11">
         <v>7</v>
       </c>
-      <c r="J55" s="11">
+      <c r="J58" s="11">
         <v>7</v>
       </c>
-      <c r="K55" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E56" s="11">
+      <c r="K58" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B59" s="19">
         <v>6</v>
       </c>
-      <c r="F56" s="11">
+      <c r="C59" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="D59" t="s">
+        <v>124</v>
+      </c>
+      <c r="E59" s="11">
+        <v>6</v>
+      </c>
+      <c r="F59" s="11">
         <f t="shared" si="1"/>
         <v>99221</v>
       </c>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11"/>
-      <c r="K56" s="11"/>
-    </row>
-    <row r="61" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="C61" s="13" t="s">
+      <c r="G59" s="11">
+        <v>99221</v>
+      </c>
+      <c r="H59" s="11">
+        <f>F59-G59</f>
+        <v>0</v>
+      </c>
+      <c r="I59" s="11">
+        <v>7</v>
+      </c>
+      <c r="J59" s="11">
+        <v>6</v>
+      </c>
+      <c r="K59" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B60" s="19">
+        <v>7</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="D60" t="s">
+        <v>122</v>
+      </c>
+      <c r="E60" s="19">
+        <v>7</v>
+      </c>
+      <c r="F60" s="19">
+        <f>G59</f>
+        <v>99221</v>
+      </c>
+      <c r="G60" s="19">
+        <v>99221</v>
+      </c>
+      <c r="H60" s="19">
+        <f>F60-G60</f>
+        <v>0</v>
+      </c>
+      <c r="I60" s="19">
+        <v>6</v>
+      </c>
+      <c r="J60" s="19">
+        <v>5</v>
+      </c>
+      <c r="K60" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B61" s="19">
+        <v>8</v>
+      </c>
+      <c r="C61" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="D61" t="s">
+        <v>128</v>
+      </c>
+      <c r="E61" s="19">
+        <v>8</v>
+      </c>
+      <c r="F61" s="19">
+        <f>G60</f>
+        <v>99221</v>
+      </c>
+      <c r="G61" s="19">
+        <v>99221</v>
+      </c>
+      <c r="H61" s="19">
+        <f>F61-G61</f>
+        <v>0</v>
+      </c>
+      <c r="I61" s="19">
+        <v>5</v>
+      </c>
+      <c r="J61" s="19">
+        <v>4</v>
+      </c>
+      <c r="K61" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A63" s="22"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="22"/>
+      <c r="I63" s="22"/>
+      <c r="J63" s="22"/>
+      <c r="K63" s="22"/>
+      <c r="L63" s="22"/>
+      <c r="M63" s="22"/>
+    </row>
+    <row r="65" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="C65" s="23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B62" s="6" t="s">
+    <row r="67" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B67" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C67" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="E67" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F62" s="9" t="s">
+      <c r="F67" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G62" s="9" t="s">
+      <c r="G67" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H62" s="9" t="s">
+      <c r="H67" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I62" s="10" t="s">
+      <c r="I67" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="J62" s="10" t="s">
+      <c r="J67" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="K62" s="10" t="s">
+      <c r="K67" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B63" s="11">
-        <v>0</v>
-      </c>
-      <c r="C63" s="11" t="s">
+    <row r="68" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B68" s="11">
+        <v>0</v>
+      </c>
+      <c r="C68" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E63" s="15">
-        <v>0</v>
-      </c>
-      <c r="F63" s="15">
+      <c r="E68" s="11">
+        <v>0</v>
+      </c>
+      <c r="F68" s="11">
         <v>99441</v>
       </c>
-      <c r="G63" s="15">
+      <c r="G68" s="11">
         <v>99441</v>
       </c>
-      <c r="H63" s="15">
-        <v>0</v>
-      </c>
-      <c r="I63" s="15">
+      <c r="H68" s="11">
+        <v>0</v>
+      </c>
+      <c r="I68" s="11">
         <v>8</v>
       </c>
-      <c r="J63" s="15">
+      <c r="J68" s="11">
         <v>8</v>
       </c>
-      <c r="K63" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B64" s="11">
+      <c r="K68" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B69" s="11">
         <v>1</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C69" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E64" s="15">
+      <c r="E69" s="11">
         <v>1</v>
       </c>
-      <c r="F64" s="15">
-        <f>G63</f>
+      <c r="F69" s="11">
+        <f>G68</f>
         <v>99441</v>
       </c>
-      <c r="G64" s="15">
+      <c r="G69" s="11">
         <v>99441</v>
       </c>
-      <c r="H64" s="15">
-        <v>0</v>
-      </c>
-      <c r="I64" s="15">
+      <c r="H69" s="11">
+        <v>0</v>
+      </c>
+      <c r="I69" s="11">
         <v>8</v>
       </c>
-      <c r="J64" s="15">
+      <c r="J69" s="11">
         <v>8</v>
       </c>
-      <c r="K64" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B65" s="11">
+      <c r="K69" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B70" s="11">
         <v>2</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C70" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E65" s="15">
+      <c r="E70" s="11">
         <v>2</v>
       </c>
-      <c r="F65" s="15">
-        <f>G64</f>
+      <c r="F70" s="11">
+        <f>G69</f>
         <v>99441</v>
       </c>
-      <c r="G65" s="15">
+      <c r="G70" s="11">
         <v>99441</v>
       </c>
-      <c r="H65" s="15">
-        <v>0</v>
-      </c>
-      <c r="I65" s="15">
+      <c r="H70" s="11">
+        <v>0</v>
+      </c>
+      <c r="I70" s="11">
         <v>8</v>
       </c>
-      <c r="J65" s="15">
+      <c r="J70" s="11">
         <v>8</v>
       </c>
-      <c r="K65" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B66" s="11">
+      <c r="K70" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B71" s="11">
         <v>3</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C71" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E66" s="15">
+      <c r="E71" s="11">
         <v>3</v>
       </c>
-      <c r="F66" s="15">
-        <f>G65</f>
+      <c r="F71" s="11">
+        <f>G70</f>
         <v>99441</v>
       </c>
-      <c r="G66" s="15">
+      <c r="G71" s="11">
         <v>99441</v>
       </c>
-      <c r="H66" s="15">
-        <v>0</v>
-      </c>
-      <c r="I66" s="15">
+      <c r="H71" s="11">
+        <v>0</v>
+      </c>
+      <c r="I71" s="11">
         <v>8</v>
       </c>
-      <c r="J66" s="15">
+      <c r="J71" s="11">
         <v>8</v>
       </c>
-      <c r="K66" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E67" s="15">
+      <c r="K71" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B72" s="19">
         <v>4</v>
       </c>
-      <c r="F67" s="15">
-        <f>G66</f>
+      <c r="C72" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="D72" t="s">
+        <v>139</v>
+      </c>
+      <c r="E72" s="11">
+        <v>4</v>
+      </c>
+      <c r="F72" s="11">
+        <f>G71</f>
         <v>99441</v>
       </c>
-      <c r="G67" s="15"/>
-      <c r="H67" s="15"/>
-      <c r="I67" s="15"/>
-      <c r="J67" s="15"/>
-      <c r="K67" s="15"/>
-    </row>
-    <row r="71" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="C71" s="13" t="s">
+      <c r="G72" s="11">
+        <v>99441</v>
+      </c>
+      <c r="H72" s="11">
+        <v>0</v>
+      </c>
+      <c r="I72" s="11">
+        <v>8</v>
+      </c>
+      <c r="J72" s="11">
+        <v>7</v>
+      </c>
+      <c r="K72" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B73" s="19">
+        <v>5</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="D73" t="s">
+        <v>141</v>
+      </c>
+      <c r="E73" s="19">
+        <v>5</v>
+      </c>
+      <c r="F73" s="19">
+        <f>G72</f>
+        <v>99441</v>
+      </c>
+      <c r="G73" s="19">
+        <v>99441</v>
+      </c>
+      <c r="H73" s="19">
+        <v>0</v>
+      </c>
+      <c r="I73" s="19">
+        <v>7</v>
+      </c>
+      <c r="J73" s="19">
+        <v>6</v>
+      </c>
+      <c r="K73" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B74" s="21"/>
+      <c r="C74" s="21"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="21"/>
+      <c r="H74" s="21"/>
+      <c r="I74" s="21"/>
+      <c r="J74" s="21"/>
+      <c r="K74" s="21"/>
+    </row>
+    <row r="75" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="22"/>
+      <c r="B75" s="24"/>
+      <c r="C75" s="24"/>
+      <c r="D75" s="22"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="24"/>
+      <c r="H75" s="24"/>
+      <c r="I75" s="24"/>
+      <c r="J75" s="24"/>
+      <c r="K75" s="24"/>
+      <c r="L75" s="22"/>
+      <c r="M75" s="22"/>
+    </row>
+    <row r="76" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B76" s="21"/>
+      <c r="C76" s="21"/>
+      <c r="E76" s="21"/>
+      <c r="F76" s="21"/>
+      <c r="G76" s="21"/>
+      <c r="H76" s="21"/>
+      <c r="I76" s="21"/>
+      <c r="J76" s="21"/>
+      <c r="K76" s="21"/>
+    </row>
+    <row r="77" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="C77" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B72" s="6" t="s">
+    <row r="79" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B79" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C79" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E72" s="8" t="s">
+      <c r="E79" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F72" s="9" t="s">
+      <c r="F79" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G72" s="9" t="s">
+      <c r="G79" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H72" s="9" t="s">
+      <c r="H79" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I72" s="10" t="s">
+      <c r="I79" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="J72" s="10" t="s">
+      <c r="J79" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="K72" s="10" t="s">
+      <c r="K79" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B73" s="11">
-        <v>0</v>
-      </c>
-      <c r="C73" s="11" t="s">
+    <row r="80" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B80" s="11">
+        <v>0</v>
+      </c>
+      <c r="C80" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E73" s="11">
-        <v>0</v>
-      </c>
-      <c r="F73" s="11">
+      <c r="E80" s="11">
+        <v>0</v>
+      </c>
+      <c r="F80" s="11">
         <v>32951</v>
       </c>
-      <c r="G73" s="11">
+      <c r="G80" s="11">
         <v>32951</v>
       </c>
-      <c r="H73" s="11">
-        <v>0</v>
-      </c>
-      <c r="I73" s="11">
+      <c r="H80" s="11">
+        <v>0</v>
+      </c>
+      <c r="I80" s="11">
         <v>6</v>
       </c>
-      <c r="J73" s="11">
+      <c r="J80" s="11">
         <v>6</v>
       </c>
-      <c r="K73" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B74" s="11">
+      <c r="K80" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B81" s="11">
         <v>1</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C81" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E74" s="11">
+      <c r="E81" s="11">
         <v>1</v>
       </c>
-      <c r="F74" s="11">
-        <f>G73</f>
+      <c r="F81" s="11">
+        <f t="shared" ref="F81:F86" si="2">G80</f>
         <v>32951</v>
       </c>
-      <c r="G74" s="11">
+      <c r="G81" s="11">
         <v>32951</v>
       </c>
-      <c r="H74" s="11">
-        <v>0</v>
-      </c>
-      <c r="I74" s="11">
+      <c r="H81" s="11">
+        <v>0</v>
+      </c>
+      <c r="I81" s="11">
         <v>6</v>
       </c>
-      <c r="J74" s="11">
+      <c r="J81" s="11">
         <v>6</v>
       </c>
-      <c r="K74" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B75" s="11">
+      <c r="K81" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B82" s="11">
         <v>2</v>
       </c>
-      <c r="C75" s="11" t="s">
+      <c r="C82" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E75" s="11">
+      <c r="E82" s="11">
         <v>2</v>
       </c>
-      <c r="F75" s="11">
-        <f>G74</f>
+      <c r="F82" s="11">
+        <f t="shared" si="2"/>
         <v>32951</v>
       </c>
-      <c r="G75" s="11">
+      <c r="G82" s="11">
         <v>32951</v>
       </c>
-      <c r="H75" s="11">
-        <v>0</v>
-      </c>
-      <c r="I75" s="11">
+      <c r="H82" s="11">
+        <v>0</v>
+      </c>
+      <c r="I82" s="11">
         <v>6</v>
       </c>
-      <c r="J75" s="11">
+      <c r="J82" s="11">
         <v>6</v>
       </c>
-      <c r="K75" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B76" s="11">
+      <c r="K82" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B83" s="11">
         <v>3</v>
       </c>
-      <c r="C76" s="11" t="s">
+      <c r="C83" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E76" s="11">
+      <c r="E83" s="11">
         <v>3</v>
       </c>
-      <c r="F76" s="11">
-        <f>G75</f>
+      <c r="F83" s="11">
+        <f t="shared" si="2"/>
         <v>32951</v>
       </c>
-      <c r="G76" s="11">
+      <c r="G83" s="11">
         <v>32951</v>
       </c>
-      <c r="H76" s="11">
-        <v>0</v>
-      </c>
-      <c r="I76" s="11">
+      <c r="H83" s="11">
+        <v>0</v>
+      </c>
+      <c r="I83" s="11">
         <v>6</v>
       </c>
-      <c r="J76" s="11">
+      <c r="J83" s="11">
         <v>6</v>
       </c>
-      <c r="K76" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B77" s="16">
+      <c r="K83" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B84" s="11">
         <v>4</v>
       </c>
-      <c r="C77" s="16" t="s">
+      <c r="C84" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D77" t="s">
-        <v>153</v>
-      </c>
-      <c r="E77" s="11">
+      <c r="D84" t="s">
+        <v>151</v>
+      </c>
+      <c r="E84" s="11">
         <v>4</v>
       </c>
-      <c r="F77" s="11">
-        <f>G76</f>
+      <c r="F84" s="11">
+        <f t="shared" si="2"/>
         <v>32951</v>
       </c>
-      <c r="G77" s="11">
+      <c r="G84" s="11">
         <v>32949</v>
       </c>
-      <c r="H77" s="11">
-        <f>F77-G77</f>
+      <c r="H84" s="11">
+        <f>F84-G84</f>
         <v>2</v>
       </c>
-      <c r="I77" s="11">
+      <c r="I84" s="11">
         <v>6</v>
       </c>
-      <c r="J77" s="11">
+      <c r="J84" s="11">
         <v>6</v>
       </c>
-      <c r="K77" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B78" s="16">
-        <v>5</v>
-      </c>
-      <c r="C78" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="D78" t="s">
-        <v>153</v>
-      </c>
-      <c r="E78" s="11">
-        <v>5</v>
-      </c>
-      <c r="F78" s="11">
-        <f>G77</f>
+      <c r="K84" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B85" s="11">
+        <v>5</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D85" t="s">
+        <v>151</v>
+      </c>
+      <c r="E85" s="11">
+        <v>5</v>
+      </c>
+      <c r="F85" s="11">
+        <f t="shared" si="2"/>
         <v>32949</v>
       </c>
-      <c r="G78" s="11">
+      <c r="G85" s="11">
         <v>32945</v>
       </c>
-      <c r="H78" s="11">
-        <f>F78-G78</f>
+      <c r="H85" s="11">
+        <f>F85-G85</f>
         <v>4</v>
-      </c>
-      <c r="I78" s="11">
-        <v>6</v>
-      </c>
-      <c r="J78" s="11">
-        <v>6</v>
-      </c>
-      <c r="K78" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E79" s="11">
-        <v>6</v>
-      </c>
-      <c r="F79" s="11">
-        <f>G78</f>
-        <v>32945</v>
-      </c>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
-      <c r="I79" s="11"/>
-      <c r="J79" s="11"/>
-      <c r="K79" s="11"/>
-    </row>
-    <row r="83" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="C83" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="84" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B84" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G84" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H84" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="I84" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="J84" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="K84" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="85" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B85" s="11">
-        <v>0</v>
-      </c>
-      <c r="C85" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E85" s="11">
-        <v>0</v>
-      </c>
-      <c r="F85" s="11">
-        <v>3095</v>
-      </c>
-      <c r="G85" s="11">
-        <v>3095</v>
-      </c>
-      <c r="H85" s="11">
-        <v>0</v>
       </c>
       <c r="I85" s="11">
         <v>6</v>
@@ -3657,109 +4317,221 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B86" s="11">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A87" s="22"/>
+      <c r="B87" s="22"/>
+      <c r="C87" s="22"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="22"/>
+      <c r="F87" s="22"/>
+      <c r="G87" s="22"/>
+      <c r="H87" s="22"/>
+      <c r="I87" s="22"/>
+      <c r="J87" s="22"/>
+      <c r="K87" s="22"/>
+      <c r="L87" s="22"/>
+      <c r="M87" s="22"/>
+    </row>
+    <row r="89" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="C89" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B91" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E91" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H91" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I91" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J91" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K91" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B92" s="11">
+        <v>0</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E92" s="11">
+        <v>0</v>
+      </c>
+      <c r="F92" s="11">
+        <v>3095</v>
+      </c>
+      <c r="G92" s="11">
+        <v>3095</v>
+      </c>
+      <c r="H92" s="11">
+        <v>0</v>
+      </c>
+      <c r="I92" s="11">
+        <v>6</v>
+      </c>
+      <c r="J92" s="11">
+        <v>6</v>
+      </c>
+      <c r="K92" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B93" s="11">
         <v>1</v>
       </c>
-      <c r="C86" s="11" t="s">
+      <c r="C93" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E86" s="11">
+      <c r="E93" s="11">
         <v>1</v>
       </c>
-      <c r="F86" s="11">
-        <f>G85</f>
+      <c r="F93" s="11">
+        <f>G92</f>
         <v>3095</v>
       </c>
-      <c r="G86" s="11">
+      <c r="G93" s="11">
         <v>3095</v>
       </c>
-      <c r="H86" s="11">
-        <v>0</v>
-      </c>
-      <c r="I86" s="11">
+      <c r="H93" s="11">
+        <v>0</v>
+      </c>
+      <c r="I93" s="11">
         <v>6</v>
       </c>
-      <c r="J86" s="11">
+      <c r="J93" s="11">
         <v>6</v>
       </c>
-      <c r="K86" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B87" s="11">
+      <c r="K93" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B94" s="11">
         <v>2</v>
       </c>
-      <c r="C87" s="11" t="s">
+      <c r="C94" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E87" s="11">
+      <c r="E94" s="11">
         <v>2</v>
       </c>
-      <c r="F87" s="11">
-        <f>G86</f>
+      <c r="F94" s="11">
+        <f>G93</f>
         <v>3095</v>
       </c>
-      <c r="G87" s="11">
+      <c r="G94" s="11">
         <v>3095</v>
       </c>
-      <c r="H87" s="11">
-        <v>0</v>
-      </c>
-      <c r="I87" s="11">
+      <c r="H94" s="11">
+        <v>0</v>
+      </c>
+      <c r="I94" s="11">
         <v>6</v>
       </c>
-      <c r="J87" s="11">
+      <c r="J94" s="11">
         <v>6</v>
       </c>
-      <c r="K87" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B88" s="11">
+      <c r="K94" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B95" s="11">
         <v>3</v>
       </c>
-      <c r="C88" s="11" t="s">
+      <c r="C95" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E88" s="11">
+      <c r="E95" s="11">
         <v>3</v>
       </c>
-      <c r="F88" s="11">
-        <f>G87</f>
+      <c r="F95" s="11">
+        <f>G94</f>
         <v>3095</v>
       </c>
-      <c r="G88" s="11">
+      <c r="G95" s="11">
         <v>3095</v>
       </c>
-      <c r="H88" s="11">
-        <v>0</v>
-      </c>
-      <c r="I88" s="11">
+      <c r="H95" s="11">
+        <v>0</v>
+      </c>
+      <c r="I95" s="11">
         <v>6</v>
       </c>
-      <c r="J88" s="11">
+      <c r="J95" s="11">
         <v>6</v>
       </c>
-      <c r="K88" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E89" s="11">
+      <c r="K95" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B96" s="19">
         <v>4</v>
       </c>
-      <c r="F89" s="11">
-        <f>G88</f>
+      <c r="C96" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="D96" t="s">
+        <v>167</v>
+      </c>
+      <c r="E96" s="11">
+        <v>4</v>
+      </c>
+      <c r="F96" s="11">
+        <f>G95</f>
         <v>3095</v>
       </c>
-      <c r="G89" s="11"/>
-      <c r="H89" s="11"/>
-      <c r="I89" s="11"/>
-      <c r="J89" s="11"/>
-      <c r="K89" s="11"/>
+      <c r="G96" s="11">
+        <v>3095</v>
+      </c>
+      <c r="H96" s="11">
+        <v>0</v>
+      </c>
+      <c r="I96" s="11">
+        <v>6</v>
+      </c>
+      <c r="J96" s="11">
+        <v>5</v>
+      </c>
+      <c r="K96" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A98" s="27"/>
+      <c r="B98" s="27"/>
+      <c r="C98" s="27"/>
+      <c r="D98" s="27"/>
+      <c r="E98" s="27"/>
+      <c r="F98" s="27"/>
+      <c r="G98" s="27"/>
+      <c r="H98" s="27"/>
+      <c r="I98" s="27"/>
+      <c r="J98" s="27"/>
+      <c r="K98" s="27"/>
+      <c r="L98" s="27"/>
+      <c r="M98" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3768,12 +4540,181 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7DB601-2E61-4816-8642-3B30D49A003A}">
-  <dimension ref="A1"/>
+  <dimension ref="C3:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:6" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="D3" s="26" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C5" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C6" s="11">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C7" s="11">
+        <v>2</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C8" s="11">
+        <v>3</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C9" s="11">
+        <v>4</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C10" s="11">
+        <v>5</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C11" s="11">
+        <v>6</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C12" s="11">
+        <v>7</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C13" s="11">
+        <v>8</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C14" s="11">
+        <v>9</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C15" s="11">
+        <v>10</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Start Working On Home Page & add Model View
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463A294E-6CBC-4477-BE4E-62EF66EB4AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8DE41B-BFE1-4781-99C4-68779353AD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="2" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
@@ -1467,7 +1467,7 @@
   <dimension ref="B3:H103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F91" sqref="F91"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Complete Basic Design of Report
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8DE41B-BFE1-4781-99C4-68779353AD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827EB7C9-3FA6-4FCE-BB4D-9F9E8E19A5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="2" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
@@ -809,7 +809,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -857,14 +857,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1466,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035EC863-7662-4F46-A1E6-DDC33702C1E8}">
   <dimension ref="B3:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2544,7 +2541,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="20" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2773,26 +2770,26 @@
       <c r="D11" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="11">
         <v>6</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="11">
         <f>G10</f>
         <v>99441</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="11">
         <v>99441</v>
       </c>
       <c r="H11" s="11">
         <v>0</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="11">
         <v>10</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="11">
         <v>9</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2806,54 +2803,54 @@
       <c r="D12" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="11">
         <v>7</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="11">
         <f>G11</f>
         <v>99441</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="11">
         <v>99441</v>
       </c>
       <c r="H12" s="11">
         <v>0</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="11">
         <v>9</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="11">
         <v>8</v>
       </c>
-      <c r="K12" s="19">
+      <c r="K12" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
     </row>
     <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="12"/>
@@ -2861,7 +2858,7 @@
     </row>
     <row r="16" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B16" s="12"/>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="20" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3047,22 +3044,22 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="20" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3251,10 +3248,10 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B35" s="19">
-        <v>5</v>
-      </c>
-      <c r="C35" s="19" t="s">
+      <c r="B35" s="11">
+        <v>5</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>201</v>
       </c>
       <c r="D35" t="s">
@@ -3284,22 +3281,22 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
+      <c r="A37" s="19"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
     </row>
     <row r="39" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="C39" s="23" t="s">
+      <c r="C39" s="20" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3452,10 +3449,10 @@
       </c>
     </row>
     <row r="46" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B46" s="19">
+      <c r="B46" s="11">
         <v>4</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C46" s="11" t="s">
         <v>201</v>
       </c>
       <c r="D46" t="s">
@@ -3485,22 +3482,22 @@
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A48" s="22"/>
-      <c r="B48" s="22"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="22"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="22"/>
-      <c r="J48" s="22"/>
-      <c r="K48" s="22"/>
-      <c r="L48" s="22"/>
-      <c r="M48" s="22"/>
+      <c r="A48" s="19"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="19"/>
+      <c r="L48" s="19"/>
+      <c r="M48" s="19"/>
     </row>
     <row r="50" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="C50" s="23" t="s">
+      <c r="C50" s="20" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3580,7 +3577,7 @@
         <v>99327</v>
       </c>
       <c r="H54" s="11">
-        <f>F54-G54</f>
+        <f t="shared" ref="H54:H61" si="2">F54-G54</f>
         <v>2</v>
       </c>
       <c r="I54" s="11">
@@ -3611,7 +3608,7 @@
         <v>99268</v>
       </c>
       <c r="H55" s="11">
-        <f>F55-G55</f>
+        <f t="shared" si="2"/>
         <v>59</v>
       </c>
       <c r="I55" s="11">
@@ -3642,7 +3639,7 @@
         <v>99268</v>
       </c>
       <c r="H56" s="11">
-        <f>F56-G56</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I56" s="11">
@@ -3676,7 +3673,7 @@
         <v>99223</v>
       </c>
       <c r="H57" s="11">
-        <f>F57-G57</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="I57" s="11">
@@ -3710,7 +3707,7 @@
         <v>99221</v>
       </c>
       <c r="H58" s="11">
-        <f>F58-G58</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I58" s="11">
@@ -3724,10 +3721,10 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B59" s="19">
+      <c r="B59" s="11">
         <v>6</v>
       </c>
-      <c r="C59" s="19" t="s">
+      <c r="C59" s="11" t="s">
         <v>201</v>
       </c>
       <c r="D59" t="s">
@@ -3744,7 +3741,7 @@
         <v>99221</v>
       </c>
       <c r="H59" s="11">
-        <f>F59-G59</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I59" s="11">
@@ -3758,90 +3755,90 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B60" s="19">
+      <c r="B60" s="11">
         <v>7</v>
       </c>
-      <c r="C60" s="19" t="s">
+      <c r="C60" s="11" t="s">
         <v>201</v>
       </c>
       <c r="D60" t="s">
         <v>122</v>
       </c>
-      <c r="E60" s="19">
+      <c r="E60" s="11">
         <v>7</v>
       </c>
-      <c r="F60" s="19">
+      <c r="F60" s="11">
         <f>G59</f>
         <v>99221</v>
       </c>
-      <c r="G60" s="19">
+      <c r="G60" s="11">
         <v>99221</v>
       </c>
-      <c r="H60" s="19">
-        <f>F60-G60</f>
-        <v>0</v>
-      </c>
-      <c r="I60" s="19">
+      <c r="H60" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I60" s="11">
         <v>6</v>
       </c>
-      <c r="J60" s="19">
-        <v>5</v>
-      </c>
-      <c r="K60" s="19">
+      <c r="J60" s="11">
+        <v>5</v>
+      </c>
+      <c r="K60" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B61" s="19">
+      <c r="B61" s="11">
         <v>8</v>
       </c>
-      <c r="C61" s="19" t="s">
+      <c r="C61" s="11" t="s">
         <v>201</v>
       </c>
       <c r="D61" t="s">
         <v>128</v>
       </c>
-      <c r="E61" s="19">
+      <c r="E61" s="11">
         <v>8</v>
       </c>
-      <c r="F61" s="19">
+      <c r="F61" s="11">
         <f>G60</f>
         <v>99221</v>
       </c>
-      <c r="G61" s="19">
+      <c r="G61" s="11">
         <v>99221</v>
       </c>
-      <c r="H61" s="19">
-        <f>F61-G61</f>
-        <v>0</v>
-      </c>
-      <c r="I61" s="19">
-        <v>5</v>
-      </c>
-      <c r="J61" s="19">
+      <c r="H61" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I61" s="11">
+        <v>5</v>
+      </c>
+      <c r="J61" s="11">
         <v>4</v>
       </c>
-      <c r="K61" s="19">
+      <c r="K61" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A63" s="22"/>
-      <c r="B63" s="22"/>
-      <c r="C63" s="22"/>
-      <c r="D63" s="22"/>
-      <c r="E63" s="22"/>
-      <c r="F63" s="22"/>
-      <c r="G63" s="22"/>
-      <c r="H63" s="22"/>
-      <c r="I63" s="22"/>
-      <c r="J63" s="22"/>
-      <c r="K63" s="22"/>
-      <c r="L63" s="22"/>
-      <c r="M63" s="22"/>
+      <c r="A63" s="19"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="19"/>
+      <c r="K63" s="19"/>
+      <c r="L63" s="19"/>
+      <c r="M63" s="19"/>
     </row>
     <row r="65" spans="1:13" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="C65" s="23" t="s">
+      <c r="C65" s="20" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3994,10 +3991,10 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B72" s="19">
+      <c r="B72" s="11">
         <v>4</v>
       </c>
-      <c r="C72" s="19" t="s">
+      <c r="C72" s="11" t="s">
         <v>201</v>
       </c>
       <c r="D72" t="s">
@@ -4027,74 +4024,74 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B73" s="19">
-        <v>5</v>
-      </c>
-      <c r="C73" s="19" t="s">
+      <c r="B73" s="11">
+        <v>5</v>
+      </c>
+      <c r="C73" s="11" t="s">
         <v>201</v>
       </c>
       <c r="D73" t="s">
         <v>141</v>
       </c>
-      <c r="E73" s="19">
-        <v>5</v>
-      </c>
-      <c r="F73" s="19">
+      <c r="E73" s="11">
+        <v>5</v>
+      </c>
+      <c r="F73" s="11">
         <f>G72</f>
         <v>99441</v>
       </c>
-      <c r="G73" s="19">
+      <c r="G73" s="11">
         <v>99441</v>
       </c>
-      <c r="H73" s="19">
-        <v>0</v>
-      </c>
-      <c r="I73" s="19">
+      <c r="H73" s="11">
+        <v>0</v>
+      </c>
+      <c r="I73" s="11">
         <v>7</v>
       </c>
-      <c r="J73" s="19">
+      <c r="J73" s="11">
         <v>6</v>
       </c>
-      <c r="K73" s="19">
+      <c r="K73" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B74" s="21"/>
-      <c r="C74" s="21"/>
-      <c r="E74" s="21"/>
-      <c r="F74" s="21"/>
-      <c r="G74" s="21"/>
-      <c r="H74" s="21"/>
-      <c r="I74" s="21"/>
-      <c r="J74" s="21"/>
-      <c r="K74" s="21"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="12"/>
+      <c r="J74" s="12"/>
+      <c r="K74" s="12"/>
     </row>
     <row r="75" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="22"/>
-      <c r="B75" s="24"/>
-      <c r="C75" s="24"/>
-      <c r="D75" s="22"/>
-      <c r="E75" s="24"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="24"/>
-      <c r="H75" s="24"/>
-      <c r="I75" s="24"/>
-      <c r="J75" s="24"/>
-      <c r="K75" s="24"/>
-      <c r="L75" s="22"/>
-      <c r="M75" s="22"/>
+      <c r="A75" s="19"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="21"/>
+      <c r="H75" s="21"/>
+      <c r="I75" s="21"/>
+      <c r="J75" s="21"/>
+      <c r="K75" s="21"/>
+      <c r="L75" s="19"/>
+      <c r="M75" s="19"/>
     </row>
     <row r="76" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B76" s="21"/>
-      <c r="C76" s="21"/>
-      <c r="E76" s="21"/>
-      <c r="F76" s="21"/>
-      <c r="G76" s="21"/>
-      <c r="H76" s="21"/>
-      <c r="I76" s="21"/>
-      <c r="J76" s="21"/>
-      <c r="K76" s="21"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="12"/>
     </row>
     <row r="77" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
       <c r="C77" s="13" t="s">
@@ -4170,7 +4167,7 @@
         <v>1</v>
       </c>
       <c r="F81" s="11">
-        <f t="shared" ref="F81:F86" si="2">G80</f>
+        <f t="shared" ref="F81:F85" si="3">G80</f>
         <v>32951</v>
       </c>
       <c r="G81" s="11">
@@ -4200,7 +4197,7 @@
         <v>2</v>
       </c>
       <c r="F82" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32951</v>
       </c>
       <c r="G82" s="11">
@@ -4230,7 +4227,7 @@
         <v>3</v>
       </c>
       <c r="F83" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32951</v>
       </c>
       <c r="G83" s="11">
@@ -4263,7 +4260,7 @@
         <v>4</v>
       </c>
       <c r="F84" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32951</v>
       </c>
       <c r="G84" s="11">
@@ -4297,7 +4294,7 @@
         <v>5</v>
       </c>
       <c r="F85" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32949</v>
       </c>
       <c r="G85" s="11">
@@ -4318,19 +4315,19 @@
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A87" s="22"/>
-      <c r="B87" s="22"/>
-      <c r="C87" s="22"/>
-      <c r="D87" s="22"/>
-      <c r="E87" s="22"/>
-      <c r="F87" s="22"/>
-      <c r="G87" s="22"/>
-      <c r="H87" s="22"/>
-      <c r="I87" s="22"/>
-      <c r="J87" s="22"/>
-      <c r="K87" s="22"/>
-      <c r="L87" s="22"/>
-      <c r="M87" s="22"/>
+      <c r="A87" s="19"/>
+      <c r="B87" s="19"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="19"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="19"/>
+      <c r="G87" s="19"/>
+      <c r="H87" s="19"/>
+      <c r="I87" s="19"/>
+      <c r="J87" s="19"/>
+      <c r="K87" s="19"/>
+      <c r="L87" s="19"/>
+      <c r="M87" s="19"/>
     </row>
     <row r="89" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
       <c r="C89" s="13" t="s">
@@ -4486,10 +4483,10 @@
       </c>
     </row>
     <row r="96" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B96" s="19">
+      <c r="B96" s="11">
         <v>4</v>
       </c>
-      <c r="C96" s="19" t="s">
+      <c r="C96" s="11" t="s">
         <v>202</v>
       </c>
       <c r="D96" t="s">
@@ -4519,19 +4516,19 @@
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A98" s="27"/>
-      <c r="B98" s="27"/>
-      <c r="C98" s="27"/>
-      <c r="D98" s="27"/>
-      <c r="E98" s="27"/>
-      <c r="F98" s="27"/>
-      <c r="G98" s="27"/>
-      <c r="H98" s="27"/>
-      <c r="I98" s="27"/>
-      <c r="J98" s="27"/>
-      <c r="K98" s="27"/>
-      <c r="L98" s="27"/>
-      <c r="M98" s="27"/>
+      <c r="A98" s="24"/>
+      <c r="B98" s="24"/>
+      <c r="C98" s="24"/>
+      <c r="D98" s="24"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="24"/>
+      <c r="G98" s="24"/>
+      <c r="H98" s="24"/>
+      <c r="I98" s="24"/>
+      <c r="J98" s="24"/>
+      <c r="K98" s="24"/>
+      <c r="L98" s="24"/>
+      <c r="M98" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4556,21 +4553,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:6" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="23" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="5" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="22" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Complete basic of Report pages like side bar buttons filters etc
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADAD70A-E0EA-4500-9021-8A4EA7A20ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8ADA191-5019-475B-80D5-2BF5B30B6AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="2" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="3" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
   <sheets>
     <sheet name="Data &amp; Purpose" sheetId="1" r:id="rId1"/>
@@ -846,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -904,29 +904,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1512,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05F3B95-CD15-4EA0-ACD4-4067EC5DC14D}">
   <dimension ref="A2:M105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E77" zoomScale="120" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85:K92"/>
+    <sheetView topLeftCell="A53" zoomScale="52" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2309,7 +2298,7 @@
       <c r="C37" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="D37" s="35" t="s">
+      <c r="D37" t="s">
         <v>205</v>
       </c>
       <c r="E37" s="11">
@@ -3753,29 +3742,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035EC863-7662-4F46-A1E6-DDC33702C1E8}">
-  <dimension ref="B3:H103"/>
+  <dimension ref="C3:H103"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScale="96" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56:H60"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="96" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:H102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" customWidth="1"/>
     <col min="3" max="3" width="28.109375" customWidth="1"/>
     <col min="4" max="4" width="26.6640625" customWidth="1"/>
     <col min="5" max="5" width="51" customWidth="1"/>
-    <col min="6" max="6" width="34.21875" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="F3" s="13" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
         <v>35</v>
       </c>
@@ -3792,7 +3781,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C5" s="5">
         <v>1</v>
       </c>
@@ -3809,7 +3798,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C6" s="5">
         <v>2</v>
       </c>
@@ -3826,7 +3815,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C7" s="5">
         <v>3</v>
       </c>
@@ -3843,7 +3832,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="5">
         <v>4</v>
       </c>
@@ -3860,7 +3849,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C9" s="5">
         <v>5</v>
       </c>
@@ -3877,7 +3866,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C10" s="5">
         <v>6</v>
       </c>
@@ -3894,7 +3883,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C11" s="5">
         <v>7</v>
       </c>
@@ -3911,7 +3900,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C12" s="5">
         <v>8</v>
       </c>
@@ -3928,7 +3917,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C13" s="5">
         <v>9</v>
       </c>
@@ -3938,14 +3927,14 @@
       <c r="E13" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="5">
         <v>9</v>
       </c>
-      <c r="H13" s="27" t="s">
+      <c r="H13" s="16" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C14" s="5">
         <v>10</v>
       </c>
@@ -3956,12 +3945,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B19" s="13" t="s">
+    <row r="19" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="F19" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
         <v>57</v>
       </c>
@@ -3978,7 +3967,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C21" s="5">
         <v>1</v>
       </c>
@@ -3995,7 +3984,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C22" s="5">
         <v>2</v>
       </c>
@@ -4012,7 +4001,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C23" s="5">
         <v>3</v>
       </c>
@@ -4029,7 +4018,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C24" s="5">
         <v>4</v>
       </c>
@@ -4046,7 +4035,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C25" s="5">
         <v>5</v>
       </c>
@@ -4063,12 +4052,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B30" s="13" t="s">
+    <row r="30" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="F30" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C31" s="3" t="s">
         <v>57</v>
       </c>
@@ -4085,7 +4074,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C32" s="5">
         <v>1</v>
       </c>
@@ -4095,14 +4084,14 @@
       <c r="E32" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G32" s="32">
-        <v>1</v>
-      </c>
-      <c r="H32" s="34" t="s">
+      <c r="G32" s="29">
+        <v>1</v>
+      </c>
+      <c r="H32" s="30" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C33" s="5">
         <v>2</v>
       </c>
@@ -4112,14 +4101,14 @@
       <c r="E33" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="G33" s="32">
+      <c r="G33" s="29">
         <v>2</v>
       </c>
-      <c r="H33" s="34" t="s">
+      <c r="H33" s="30" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C34" s="5">
         <v>3</v>
       </c>
@@ -4129,14 +4118,14 @@
       <c r="E34" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G34" s="32">
+      <c r="G34" s="29">
         <v>3</v>
       </c>
-      <c r="H34" s="34" t="s">
+      <c r="H34" s="30" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C35" s="5">
         <v>4</v>
       </c>
@@ -4146,14 +4135,14 @@
       <c r="E35" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G35" s="32">
+      <c r="G35" s="29">
         <v>4</v>
       </c>
-      <c r="H35" s="34" t="s">
+      <c r="H35" s="30" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C36" s="5">
         <v>5</v>
       </c>
@@ -4163,14 +4152,14 @@
       <c r="E36" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="G36" s="32">
-        <v>5</v>
-      </c>
-      <c r="H36" s="34" t="s">
+      <c r="G36" s="29">
+        <v>5</v>
+      </c>
+      <c r="H36" s="30" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C37" s="5">
         <v>6</v>
       </c>
@@ -4180,14 +4169,14 @@
       <c r="E37" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G37" s="32">
-        <v>6</v>
-      </c>
-      <c r="H37" s="34" t="s">
+      <c r="G37" s="29">
+        <v>6</v>
+      </c>
+      <c r="H37" s="30" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C38" s="5">
         <v>7</v>
       </c>
@@ -4197,19 +4186,19 @@
       <c r="E38" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="G38" s="33">
+      <c r="G38" s="29">
         <v>7</v>
       </c>
-      <c r="H38" s="34" t="s">
+      <c r="H38" s="30" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B43" s="13" t="s">
+    <row r="43" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="F43" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C44" s="3" t="s">
         <v>57</v>
       </c>
@@ -4226,7 +4215,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C45" s="5">
         <v>1</v>
       </c>
@@ -4243,7 +4232,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C46" s="5">
         <v>2</v>
       </c>
@@ -4260,7 +4249,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C47" s="5">
         <v>3</v>
       </c>
@@ -4277,7 +4266,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C48" s="5">
         <v>4</v>
       </c>
@@ -4294,7 +4283,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C49" s="5">
         <v>5</v>
       </c>
@@ -4304,19 +4293,19 @@
       <c r="E49" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G49" s="30">
+      <c r="G49" s="17">
         <v>5</v>
       </c>
       <c r="H49" s="18" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B54" s="13" t="s">
+    <row r="54" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="F54" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C55" s="3" t="s">
         <v>57</v>
       </c>
@@ -4333,7 +4322,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="56" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C56" s="5">
         <v>1</v>
       </c>
@@ -4350,7 +4339,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C57" s="5">
         <v>2</v>
       </c>
@@ -4367,7 +4356,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C58" s="5">
         <v>3</v>
       </c>
@@ -4384,7 +4373,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="59" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C59" s="5">
         <v>4</v>
       </c>
@@ -4401,7 +4390,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="60" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C60" s="5">
         <v>5</v>
       </c>
@@ -4411,14 +4400,14 @@
       <c r="E60" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="G60" s="30">
-        <v>5</v>
-      </c>
-      <c r="H60" s="31" t="s">
+      <c r="G60" s="17">
+        <v>5</v>
+      </c>
+      <c r="H60" s="28" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="61" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C61" s="5">
         <v>6</v>
       </c>
@@ -4429,7 +4418,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C62" s="5">
         <v>7</v>
       </c>
@@ -4440,12 +4429,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B67" s="13" t="s">
+    <row r="67" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="F67" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C68" s="3" t="s">
         <v>57</v>
       </c>
@@ -4462,7 +4451,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="69" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C69" s="14">
         <v>1</v>
       </c>
@@ -4479,7 +4468,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="70" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C70" s="14">
         <v>2</v>
       </c>
@@ -4496,7 +4485,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="71" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C71" s="14">
         <v>3</v>
       </c>
@@ -4513,7 +4502,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="72" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C72" s="14">
         <v>4</v>
       </c>
@@ -4530,7 +4519,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="73" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C73" s="14">
         <v>5</v>
       </c>
@@ -4547,7 +4536,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="74" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C74" s="14">
         <v>6</v>
       </c>
@@ -4564,7 +4553,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="75" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C75" s="14">
         <v>7</v>
       </c>
@@ -4575,7 +4564,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="76" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C76" s="14">
         <v>8</v>
       </c>
@@ -4586,12 +4575,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="82" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B82" s="13" t="s">
+    <row r="82" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="F82" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C83" s="3" t="s">
         <v>57</v>
       </c>
@@ -4608,7 +4597,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="84" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C84" s="14">
         <v>1</v>
       </c>
@@ -4625,7 +4614,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="85" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C85" s="14">
         <v>2</v>
       </c>
@@ -4642,7 +4631,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="86" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C86" s="14">
         <v>3</v>
       </c>
@@ -4659,7 +4648,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="87" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C87" s="14">
         <v>4</v>
       </c>
@@ -4676,7 +4665,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="88" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C88" s="14">
         <v>5</v>
       </c>
@@ -4693,7 +4682,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="89" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C89" s="14">
         <v>6</v>
       </c>
@@ -4710,8 +4699,8 @@
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B96" s="13" t="s">
+    <row r="96" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="F96" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5011,58 +5000,58 @@
       </c>
     </row>
     <row r="16" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C16" s="28">
+      <c r="C16" s="26">
         <v>11</v>
       </c>
       <c r="D16" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="26" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="17" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C17" s="28">
+      <c r="C17" s="26">
         <v>12</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="F17" s="26" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C18" s="28">
+      <c r="C18" s="26">
         <v>13</v>
       </c>
       <c r="D18" t="s">
         <v>206</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" s="26" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C19" s="28">
+      <c r="C19" s="26">
         <v>14</v>
       </c>
       <c r="D19" t="s">
         <v>207</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="26" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add & make blue print of chart and kpis for all pages
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8ADA191-5019-475B-80D5-2BF5B30B6AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBE6BFE-E276-4D24-964F-4A97DAD2C6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="3" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="5" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
   <sheets>
     <sheet name="Data &amp; Purpose" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="334">
   <si>
     <t>Table Name</t>
   </si>
@@ -672,13 +672,382 @@
   </si>
   <si>
     <t>Volume (cm³)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overview </t>
+  </si>
+  <si>
+    <t>KPI's</t>
+  </si>
+  <si>
+    <t>Total Order Completed</t>
+  </si>
+  <si>
+    <t>KPI Name</t>
+  </si>
+  <si>
+    <t>Insight</t>
+  </si>
+  <si>
+    <t>Top Selling Category</t>
+  </si>
+  <si>
+    <t>Top Seller</t>
+  </si>
+  <si>
+    <t>Active Customer (30 Days)</t>
+  </si>
+  <si>
+    <t>Total Revenue</t>
+  </si>
+  <si>
+    <t>Average Rating</t>
+  </si>
+  <si>
+    <t>Total completed orders indicate overall demand and marketplace performance over time.</t>
+  </si>
+  <si>
+    <t>Identifies the product category that contributes the highest number of orders, showing customer buying preference.</t>
+  </si>
+  <si>
+    <t>Highlights the seller generating the most revenue, revealing the strongest performer on the platform.</t>
+  </si>
+  <si>
+    <t>Shows how many unique customers placed an order in the last 30 days, measuring customer engagement and retention.</t>
+  </si>
+  <si>
+    <t>Represents total earnings from customer payments, reflecting the financial health of the business.</t>
+  </si>
+  <si>
+    <t>Indicates overall customer satisfaction based on the average review scores received.</t>
+  </si>
+  <si>
+    <t>Charts</t>
+  </si>
+  <si>
+    <t>Chart Name</t>
+  </si>
+  <si>
+    <t>Used Column</t>
+  </si>
+  <si>
+    <t>Linr Chart</t>
+  </si>
+  <si>
+    <t>Order Date, Seller Revenue(KPI)</t>
+  </si>
+  <si>
+    <t>Order Date, COUNT(OrderID)</t>
+  </si>
+  <si>
+    <t>Order Date, Total Order Compelted(KPI)</t>
+  </si>
+  <si>
+    <t>Order Date, Active Customer (30 Days)(KPI)</t>
+  </si>
+  <si>
+    <t>Order Date, Total Revenue (KPI)</t>
+  </si>
+  <si>
+    <t>Review Date, Average Rating (KPI)</t>
+  </si>
+  <si>
+    <t>Shows how the number of successfully delivered orders changes over time, highlighting periods of high and low demand.</t>
+  </si>
+  <si>
+    <t>Displays the overall order volume trend, helping identify monthly spikes or drops in customer purchasing activity.</t>
+  </si>
+  <si>
+    <t>Tracks revenue contributed by sellers over time, revealing top-performing periods and sales growth patterns.</t>
+  </si>
+  <si>
+    <t>Shows how customer engagement varies monthly by measuring how many unique customers placed orders in recent periods.</t>
+  </si>
+  <si>
+    <t>Illustrates revenue trends over time, helping identify business growth, seasonal peaks, or declining sales periods.</t>
+  </si>
+  <si>
+    <t>Displays customer satisfaction trends by showing how average product ratings change over time.</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Di_Customer_List</t>
+  </si>
+  <si>
+    <t>Di_Geolocations</t>
+  </si>
+  <si>
+    <t>Di_Products</t>
+  </si>
+  <si>
+    <t>Di_Sellers_List</t>
+  </si>
+  <si>
+    <t>Total Customers</t>
+  </si>
+  <si>
+    <t>Total Sellers</t>
+  </si>
+  <si>
+    <t>On-Time Delivery %</t>
+  </si>
+  <si>
+    <t>Orders Trend (Line Chart)</t>
+  </si>
+  <si>
+    <t>X-axis: Order Date, Y-axis: Number of Orders</t>
+  </si>
+  <si>
+    <t>Revenue Trend (Area Chart)</t>
+  </si>
+  <si>
+    <t>X-axis: Order Date, Y-axis: Total Revenue</t>
+  </si>
+  <si>
+    <t>Top 10 Products by Revenue (Bar Chart)</t>
+  </si>
+  <si>
+    <t>Axis: Product, Value: SUM(Total Item Cost or Payment Amount)</t>
+  </si>
+  <si>
+    <t>Sellers Performance (Bar Chart)</t>
+  </si>
+  <si>
+    <t>Sellers vs Revenue / Orders</t>
+  </si>
+  <si>
+    <t>Customer Acquisition Trend (Line Chart)</t>
+  </si>
+  <si>
+    <t>X-axis: Subscription Date, Y-axis: New Customers</t>
+  </si>
+  <si>
+    <t>Map – Orders by Geolocation (Map)</t>
+  </si>
+  <si>
+    <t>Postal Code → Latitude/Longitude → Total Orders</t>
+  </si>
+  <si>
+    <t>Top Selling Product (By Quantity)</t>
+  </si>
+  <si>
+    <t>Top Revenue Product</t>
+  </si>
+  <si>
+    <t>Average Product Rating</t>
+  </si>
+  <si>
+    <t>Avg Shipping Cost Per Product</t>
+  </si>
+  <si>
+    <t>Total Products→ DISTINCTCOUNT(Product ID)</t>
+  </si>
+  <si>
+    <t>Category-wise Sales (Bar Chart)</t>
+  </si>
+  <si>
+    <t>Top 10 Best Selling Products (Horizontal Bar)</t>
+  </si>
+  <si>
+    <t>Product Weight vs Shipping Cost (Scatter Plot)</t>
+  </si>
+  <si>
+    <t>Product Dimension Distribution (Treemap)</t>
+  </si>
+  <si>
+    <t>Product Rating Distribution (Column Chart)</t>
+  </si>
+  <si>
+    <t>Top Seller by Revenue</t>
+  </si>
+  <si>
+    <t>Avg Seller Rating</t>
+  </si>
+  <si>
+    <t>Orders per Seller</t>
+  </si>
+  <si>
+    <t>On-Time Delivery by Seller (%)</t>
+  </si>
+  <si>
+    <t>Seller Revenue Ranking (Bar Chart)</t>
+  </si>
+  <si>
+    <t>Seller Fulfillment Performance (Cluster Bar)</t>
+  </si>
+  <si>
+    <t>Geo Distribution of Sellers (Map)</t>
+  </si>
+  <si>
+    <t>Seller Category Performance (Matrix/Table)</t>
+  </si>
+  <si>
+    <t>Seller Shipping Cost Trend (Line)</t>
+  </si>
+  <si>
+    <t>Seller vs Avg Shipping Cost</t>
+  </si>
+  <si>
+    <t>Seller → Product Category → Revenue</t>
+  </si>
+  <si>
+    <t>Postal Code → Sellers Count</t>
+  </si>
+  <si>
+    <t>On-time vs Late Deliveries by Seller</t>
+  </si>
+  <si>
+    <t>Sellers vs Revenue</t>
+  </si>
+  <si>
+    <t>Category vs Revenue</t>
+  </si>
+  <si>
+    <t>Total Quantity Sold</t>
+  </si>
+  <si>
+    <t>Weight (g) → Shipping Cost</t>
+  </si>
+  <si>
+    <t>Category → Product Count</t>
+  </si>
+  <si>
+    <t>Rating Category vs Count</t>
+  </si>
+  <si>
+    <t>New Customers (MTD / YTD)</t>
+  </si>
+  <si>
+    <t>Avg Age of Customers</t>
+  </si>
+  <si>
+    <t>Repeat Purchase Rate</t>
+  </si>
+  <si>
+    <t>Customer Lifetime Value (CLV)</t>
+  </si>
+  <si>
+    <t>Age Group Distribution (Column Chart)</t>
+  </si>
+  <si>
+    <t>Gender Split (Donut Chart)</t>
+  </si>
+  <si>
+    <t>Customer Location Map (Map)</t>
+  </si>
+  <si>
+    <t>Customer Cohort – Orders by Subscription Month (Matrix/Area)</t>
+  </si>
+  <si>
+    <t>Customer Order Frequency (Histogram)</t>
+  </si>
+  <si>
+    <t>Count of Orders per Customer</t>
+  </si>
+  <si>
+    <t>Subscription Month vs Orders</t>
+  </si>
+  <si>
+    <t>Latitude/Longitude</t>
+  </si>
+  <si>
+    <t>Male vs Female</t>
+  </si>
+  <si>
+    <t>Age Group vs Count</t>
+  </si>
+  <si>
+    <t>Avg Payment Amount</t>
+  </si>
+  <si>
+    <t>Installment Payments (%)</t>
+  </si>
+  <si>
+    <t>Revenue per Order</t>
+  </si>
+  <si>
+    <t>Payment Method Share</t>
+  </si>
+  <si>
+    <t>Revenue Trend Over Time (Line Chart)</t>
+  </si>
+  <si>
+    <t>Payment Method Split (Pie / Donut)</t>
+  </si>
+  <si>
+    <t>Installments vs Non-installments (Stacked Bar)</t>
+  </si>
+  <si>
+    <t>Top Revenue Cities (Bar Chart)</t>
+  </si>
+  <si>
+    <t>Order Value Distribution (Histogram)</t>
+  </si>
+  <si>
+    <t>Total Order Value bins</t>
+  </si>
+  <si>
+    <t>City vs Revenue</t>
+  </si>
+  <si>
+    <t>Counts</t>
+  </si>
+  <si>
+    <t>Credit Card, Debit Card, PayPal, etc.</t>
+  </si>
+  <si>
+    <t>Monthly Revenue</t>
+  </si>
+  <si>
+    <t>Total Reviews</t>
+  </si>
+  <si>
+    <t>% Positive Reviews (Rating 4–5)</t>
+  </si>
+  <si>
+    <t>% Negative Reviews (Rating 1–2)</t>
+  </si>
+  <si>
+    <t>Avg Review Delay (Order vs Review Date)</t>
+  </si>
+  <si>
+    <t>Rating Distribution (Column Chart)</t>
+  </si>
+  <si>
+    <t>Average Rating Over Time (Line Chart)</t>
+  </si>
+  <si>
+    <t>Product-wise Rating (Bar Chart)</t>
+  </si>
+  <si>
+    <t>Seller-wise Rating (Bar Chart)</t>
+  </si>
+  <si>
+    <t>Reviews Word Cloud (If text is available)</t>
+  </si>
+  <si>
+    <t>Text analytics</t>
+  </si>
+  <si>
+    <t>Seller vs Rating</t>
+  </si>
+  <si>
+    <t>Product vs Avg Rating</t>
+  </si>
+  <si>
+    <t>Monthly Rating Trend</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -728,6 +1097,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -846,7 +1231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -915,6 +1300,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1394,7 +1784,7 @@
   <dimension ref="B4:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D11"/>
+      <selection activeCell="C6" sqref="C6:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1501,7 +1891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05F3B95-CD15-4EA0-ACD4-4067EC5DC14D}">
   <dimension ref="A2:M105"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" zoomScale="52" workbookViewId="0">
+    <sheetView zoomScale="52" workbookViewId="0">
       <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
@@ -3744,7 +4134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035EC863-7662-4F46-A1E6-DDC33702C1E8}">
   <dimension ref="C3:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="96" workbookViewId="0">
+    <sheetView topLeftCell="A99" zoomScale="96" workbookViewId="0">
       <selection activeCell="F3" sqref="F3:H102"/>
     </sheetView>
   </sheetViews>
@@ -3761,7 +4151,7 @@
   <sheetData>
     <row r="3" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="F3" s="13" t="s">
-        <v>66</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -3947,7 +4337,7 @@
     </row>
     <row r="19" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="F19" s="13" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4577,7 +4967,7 @@
     </row>
     <row r="82" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="F82" s="13" t="s">
-        <v>3</v>
+        <v>247</v>
       </c>
     </row>
     <row r="83" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4701,7 +5091,7 @@
     </row>
     <row r="96" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="F96" s="13" t="s">
-        <v>6</v>
+        <v>248</v>
       </c>
     </row>
     <row r="97" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -5062,14 +5452,1101 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD85EE9-7333-4E1C-BE00-8EC167B0E968}">
-  <dimension ref="A1"/>
+  <dimension ref="A3:P80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="103.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="100.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="C3" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="1:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="D5" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="31" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="H6" s="24"/>
+      <c r="J6" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12">
+        <v>1</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="G7" t="s">
+        <v>221</v>
+      </c>
+      <c r="H7" s="24"/>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>230</v>
+      </c>
+      <c r="L7" t="s">
+        <v>233</v>
+      </c>
+      <c r="M7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>219</v>
+      </c>
+      <c r="H8" s="24"/>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8" t="s">
+        <v>252</v>
+      </c>
+      <c r="L8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E9" s="12">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>249</v>
+      </c>
+      <c r="H9" s="24"/>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9" t="s">
+        <v>254</v>
+      </c>
+      <c r="L9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>250</v>
+      </c>
+      <c r="H10" s="24"/>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10" t="s">
+        <v>256</v>
+      </c>
+      <c r="L10" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E11" s="12">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>220</v>
+      </c>
+      <c r="H11" s="24"/>
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="K11" t="s">
+        <v>258</v>
+      </c>
+      <c r="L11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>251</v>
+      </c>
+      <c r="H12" s="24"/>
+      <c r="J12">
+        <v>6</v>
+      </c>
+      <c r="K12" t="s">
+        <v>260</v>
+      </c>
+      <c r="L12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H13" s="24"/>
+      <c r="J13">
+        <v>7</v>
+      </c>
+      <c r="K13" t="s">
+        <v>262</v>
+      </c>
+      <c r="L13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H16" s="24"/>
+    </row>
+    <row r="17" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="C17" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="H17" s="24"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H18" s="24"/>
+    </row>
+    <row r="19" spans="1:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="D19" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="31" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D20" s="12"/>
+      <c r="E20" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="H20" s="24"/>
+      <c r="J20" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D21" s="12"/>
+      <c r="E21" s="12">
+        <v>1</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="G21" t="s">
+        <v>222</v>
+      </c>
+      <c r="H21" s="24"/>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21" t="s">
+        <v>230</v>
+      </c>
+      <c r="L21" t="s">
+        <v>232</v>
+      </c>
+      <c r="M21" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>268</v>
+      </c>
+      <c r="H22" s="24"/>
+      <c r="J22">
+        <v>2</v>
+      </c>
+      <c r="K22" t="s">
+        <v>269</v>
+      </c>
+      <c r="L22" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>264</v>
+      </c>
+      <c r="H23" s="24"/>
+      <c r="J23">
+        <v>3</v>
+      </c>
+      <c r="K23" t="s">
+        <v>270</v>
+      </c>
+      <c r="L23" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E24" s="12">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>265</v>
+      </c>
+      <c r="H24" s="24"/>
+      <c r="J24">
+        <v>4</v>
+      </c>
+      <c r="K24" t="s">
+        <v>271</v>
+      </c>
+      <c r="L24" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E25" s="12">
+        <v>5</v>
+      </c>
+      <c r="F25" t="s">
+        <v>266</v>
+      </c>
+      <c r="H25" s="24"/>
+      <c r="J25">
+        <v>5</v>
+      </c>
+      <c r="K25" t="s">
+        <v>272</v>
+      </c>
+      <c r="L25" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E26" s="12">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
+        <v>267</v>
+      </c>
+      <c r="H26" s="24"/>
+      <c r="J26">
+        <v>6</v>
+      </c>
+      <c r="K26" t="s">
+        <v>273</v>
+      </c>
+      <c r="L26" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H27" s="24"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H29" s="24"/>
+    </row>
+    <row r="30" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="C30" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="H30" s="24"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H31" s="24"/>
+    </row>
+    <row r="32" spans="1:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="D32" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="31" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D33" s="12"/>
+      <c r="E33" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="H33" s="24"/>
+      <c r="J33" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="L33" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="M33" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D34" s="12"/>
+      <c r="E34" s="12">
+        <v>1</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="G34" t="s">
+        <v>223</v>
+      </c>
+      <c r="H34" s="24"/>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34" t="s">
+        <v>230</v>
+      </c>
+      <c r="L34" t="s">
+        <v>231</v>
+      </c>
+      <c r="M34" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>250</v>
+      </c>
+      <c r="H35" s="24"/>
+      <c r="J35">
+        <v>2</v>
+      </c>
+      <c r="K35" t="s">
+        <v>278</v>
+      </c>
+      <c r="L35" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>274</v>
+      </c>
+      <c r="H36" s="24"/>
+      <c r="J36">
+        <v>3</v>
+      </c>
+      <c r="K36" t="s">
+        <v>279</v>
+      </c>
+      <c r="L36" s="33" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E37" s="12">
+        <v>3</v>
+      </c>
+      <c r="F37" t="s">
+        <v>275</v>
+      </c>
+      <c r="H37" s="24"/>
+      <c r="J37">
+        <v>4</v>
+      </c>
+      <c r="K37" t="s">
+        <v>280</v>
+      </c>
+      <c r="L37" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E38" s="12">
+        <v>4</v>
+      </c>
+      <c r="F38" t="s">
+        <v>276</v>
+      </c>
+      <c r="H38" s="24"/>
+      <c r="J38">
+        <v>5</v>
+      </c>
+      <c r="K38" t="s">
+        <v>281</v>
+      </c>
+      <c r="L38" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E39" s="12">
+        <v>5</v>
+      </c>
+      <c r="F39" t="s">
+        <v>277</v>
+      </c>
+      <c r="H39" s="24"/>
+      <c r="J39">
+        <v>6</v>
+      </c>
+      <c r="K39" t="s">
+        <v>282</v>
+      </c>
+      <c r="L39" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H40" s="24"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A41" s="24"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="24"/>
+      <c r="N41" s="24"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H42" s="24"/>
+    </row>
+    <row r="43" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="C43" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="H43" s="24"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H44" s="24"/>
+    </row>
+    <row r="45" spans="1:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="D45" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="31" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D46" s="12"/>
+      <c r="E46" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="H46" s="24"/>
+      <c r="J46" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="K46" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="L46" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="M46" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D47" s="12"/>
+      <c r="E47" s="12">
+        <v>1</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="G47" t="s">
+        <v>224</v>
+      </c>
+      <c r="H47" s="24"/>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47" t="s">
+        <v>230</v>
+      </c>
+      <c r="L47" t="s">
+        <v>234</v>
+      </c>
+      <c r="M47" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>249</v>
+      </c>
+      <c r="H48" s="24"/>
+      <c r="K48" t="s">
+        <v>297</v>
+      </c>
+      <c r="L48" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="F49" t="s">
+        <v>293</v>
+      </c>
+      <c r="H49" s="24"/>
+      <c r="K49" t="s">
+        <v>298</v>
+      </c>
+      <c r="L49" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E50" s="12">
+        <v>4</v>
+      </c>
+      <c r="F50" t="s">
+        <v>294</v>
+      </c>
+      <c r="H50" s="24"/>
+      <c r="K50" t="s">
+        <v>299</v>
+      </c>
+      <c r="L50" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E51" s="12">
+        <v>5</v>
+      </c>
+      <c r="F51" t="s">
+        <v>295</v>
+      </c>
+      <c r="H51" s="24"/>
+      <c r="K51" t="s">
+        <v>300</v>
+      </c>
+      <c r="L51" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E52" s="12">
+        <v>6</v>
+      </c>
+      <c r="F52" t="s">
+        <v>296</v>
+      </c>
+      <c r="H52" s="24"/>
+      <c r="K52" t="s">
+        <v>301</v>
+      </c>
+      <c r="L52" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H53" s="24"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A54" s="24"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="24"/>
+      <c r="J54" s="24"/>
+      <c r="K54" s="24"/>
+      <c r="L54" s="24"/>
+      <c r="M54" s="24"/>
+      <c r="N54" s="24"/>
+      <c r="O54" s="24"/>
+      <c r="P54" s="24"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H55" s="24"/>
+    </row>
+    <row r="56" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="C56" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="H56" s="24"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H57" s="24"/>
+    </row>
+    <row r="58" spans="1:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="D58" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="31" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D59" s="12"/>
+      <c r="E59" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="H59" s="24"/>
+      <c r="J59" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="K59" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="L59" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="M59" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D60" s="12"/>
+      <c r="E60" s="12">
+        <v>1</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="G60" t="s">
+        <v>225</v>
+      </c>
+      <c r="H60" s="24"/>
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="K60" t="s">
+        <v>230</v>
+      </c>
+      <c r="L60" t="s">
+        <v>235</v>
+      </c>
+      <c r="M60" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61" t="s">
+        <v>307</v>
+      </c>
+      <c r="H61" s="24"/>
+      <c r="J61">
+        <v>2</v>
+      </c>
+      <c r="K61" t="s">
+        <v>311</v>
+      </c>
+      <c r="L61" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="F62" t="s">
+        <v>308</v>
+      </c>
+      <c r="H62" s="24"/>
+      <c r="J62">
+        <v>3</v>
+      </c>
+      <c r="K62" t="s">
+        <v>312</v>
+      </c>
+      <c r="L62" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E63" s="12">
+        <v>4</v>
+      </c>
+      <c r="F63" t="s">
+        <v>309</v>
+      </c>
+      <c r="H63" s="24"/>
+      <c r="J63">
+        <v>4</v>
+      </c>
+      <c r="K63" t="s">
+        <v>313</v>
+      </c>
+      <c r="L63" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E64" s="12">
+        <v>5</v>
+      </c>
+      <c r="F64" t="s">
+        <v>310</v>
+      </c>
+      <c r="H64" s="24"/>
+      <c r="J64">
+        <v>5</v>
+      </c>
+      <c r="K64" t="s">
+        <v>314</v>
+      </c>
+      <c r="L64" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H65" s="24"/>
+      <c r="J65">
+        <v>6</v>
+      </c>
+      <c r="K65" t="s">
+        <v>315</v>
+      </c>
+      <c r="L65" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H66" s="24"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A67" s="24"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="24"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="24"/>
+      <c r="H67" s="24"/>
+      <c r="I67" s="24"/>
+      <c r="J67" s="24"/>
+      <c r="K67" s="24"/>
+      <c r="L67" s="24"/>
+      <c r="M67" s="24"/>
+      <c r="N67" s="24"/>
+      <c r="O67" s="24"/>
+      <c r="P67" s="24"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H68" s="24"/>
+    </row>
+    <row r="69" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="C69" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="H69" s="24"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H70" s="24"/>
+    </row>
+    <row r="71" spans="1:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="D71" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="24"/>
+      <c r="I71" s="31" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D72" s="12"/>
+      <c r="E72" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F72" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G72" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="H72" s="24"/>
+      <c r="J72" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="K72" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="L72" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="M72" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D73" s="12"/>
+      <c r="E73" s="12">
+        <v>1</v>
+      </c>
+      <c r="F73" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="G73" t="s">
+        <v>226</v>
+      </c>
+      <c r="H73" s="24"/>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73" t="s">
+        <v>230</v>
+      </c>
+      <c r="L73" t="s">
+        <v>236</v>
+      </c>
+      <c r="M73" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E74">
+        <v>2</v>
+      </c>
+      <c r="F74" t="s">
+        <v>321</v>
+      </c>
+      <c r="H74" s="24"/>
+      <c r="K74" t="s">
+        <v>325</v>
+      </c>
+      <c r="L74" s="33" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E75">
+        <v>3</v>
+      </c>
+      <c r="F75" t="s">
+        <v>322</v>
+      </c>
+      <c r="H75" s="24"/>
+      <c r="K75" t="s">
+        <v>326</v>
+      </c>
+      <c r="L75" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E76" s="12">
+        <v>4</v>
+      </c>
+      <c r="F76" t="s">
+        <v>323</v>
+      </c>
+      <c r="H76" s="24"/>
+      <c r="K76" t="s">
+        <v>327</v>
+      </c>
+      <c r="L76" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E77" s="12">
+        <v>5</v>
+      </c>
+      <c r="F77" t="s">
+        <v>324</v>
+      </c>
+      <c r="H77" s="24"/>
+      <c r="K77" t="s">
+        <v>328</v>
+      </c>
+      <c r="L77" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H78" s="24"/>
+      <c r="K78" t="s">
+        <v>329</v>
+      </c>
+      <c r="L78" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H79" s="24"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A80" s="24"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="24"/>
+      <c r="D80" s="24"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="24"/>
+      <c r="H80" s="24"/>
+      <c r="I80" s="24"/>
+      <c r="J80" s="24"/>
+      <c r="K80" s="24"/>
+      <c r="L80" s="24"/>
+      <c r="M80" s="24"/>
+      <c r="N80" s="24"/>
+      <c r="O80" s="24"/>
+      <c r="P80" s="24"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Complete Overview page final touch
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B271A3-4BFB-4D54-A696-EEA093C91C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B1E7DD-4251-452B-8A4B-98FA61499197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="5" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="339">
   <si>
     <t>Table Name</t>
   </si>
@@ -737,9 +737,6 @@
     <t>Order Date, COUNT(OrderID)</t>
   </si>
   <si>
-    <t>Order Date, Total Order Compelted(KPI)</t>
-  </si>
-  <si>
     <t>Order Date, Active Customer (30 Days)(KPI)</t>
   </si>
   <si>
@@ -749,9 +746,6 @@
     <t>Review Date, Average Rating (KPI)</t>
   </si>
   <si>
-    <t>Shows how the number of successfully delivered orders changes over time, highlighting periods of high and low demand.</t>
-  </si>
-  <si>
     <t>Displays the overall order volume trend, helping identify monthly spikes or drops in customer purchasing activity.</t>
   </si>
   <si>
@@ -794,42 +788,9 @@
     <t>On-Time Delivery %</t>
   </si>
   <si>
-    <t>Orders Trend (Line Chart)</t>
-  </si>
-  <si>
-    <t>X-axis: Order Date, Y-axis: Number of Orders</t>
-  </si>
-  <si>
-    <t>Revenue Trend (Area Chart)</t>
-  </si>
-  <si>
-    <t>X-axis: Order Date, Y-axis: Total Revenue</t>
-  </si>
-  <si>
     <t>Top 10 Products by Revenue (Bar Chart)</t>
   </si>
   <si>
-    <t>Axis: Product, Value: SUM(Total Item Cost or Payment Amount)</t>
-  </si>
-  <si>
-    <t>Sellers Performance (Bar Chart)</t>
-  </si>
-  <si>
-    <t>Sellers vs Revenue / Orders</t>
-  </si>
-  <si>
-    <t>Customer Acquisition Trend (Line Chart)</t>
-  </si>
-  <si>
-    <t>X-axis: Subscription Date, Y-axis: New Customers</t>
-  </si>
-  <si>
-    <t>Map – Orders by Geolocation (Map)</t>
-  </si>
-  <si>
-    <t>Postal Code → Latitude/Longitude → Total Orders</t>
-  </si>
-  <si>
     <t>Top Selling Product (By Quantity)</t>
   </si>
   <si>
@@ -1059,6 +1020,94 @@
   </si>
   <si>
     <t>Shows how many orders were delivered on or before the estimated delivery date. A higher percentage indicates efficient logistics and better customer experience.</t>
+  </si>
+  <si>
+    <t>Used Columns / Measures</t>
+  </si>
+  <si>
+    <t>Monthly Completed Orders Trend (Line Chart)</t>
+  </si>
+  <si>
+    <t>Shows how successfully delivered orders change month by month, helping identify high-demand and low-demand periods.</t>
+  </si>
+  <si>
+    <t>Highlights the highest revenue-generating product categories and helps identify top-selling items.</t>
+  </si>
+  <si>
+    <t>Total Customers by Gender (Pie Chart)</t>
+  </si>
+  <si>
+    <t>Displays customer distribution based on gender, providing insight into the dominant customer segment.</t>
+  </si>
+  <si>
+    <t>Total Revenue by Quarter (Column Chart / Line Chart)</t>
+  </si>
+  <si>
+    <t>Shows quarterly revenue performance, helping identify seasonal patterns, growth cycles, and business health across quarters.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Order Date, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Total Orders Completed (KPI)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Category, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Total Revenue</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gender, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Total Customers</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Order Date, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Total Revenue</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1137,7 +1186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1210,6 +1259,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1249,7 +1304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1328,6 +1383,9 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4174,7 +4232,7 @@
   <sheetData>
     <row r="3" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="F3" s="13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4360,7 +4418,7 @@
     </row>
     <row r="19" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="F19" s="13" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4990,7 +5048,7 @@
     </row>
     <row r="82" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="F82" s="13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="83" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -5114,7 +5172,7 @@
     </row>
     <row r="96" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="F96" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="97" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -5477,8 +5535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD85EE9-7333-4E1C-BE00-8EC167B0E968}">
   <dimension ref="A3:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="G4" activeCellId="1" sqref="F12 G4"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5489,7 +5547,7 @@
     <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="54" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="61.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="100.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="116.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
@@ -5522,19 +5580,19 @@
         <v>214</v>
       </c>
       <c r="G6" s="36" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="J6" s="22" t="s">
+      <c r="J6" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="K6" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="L6" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="M6" s="22" t="s">
+      <c r="L6" s="36" t="s">
+        <v>327</v>
+      </c>
+      <c r="M6" s="36" t="s">
         <v>215</v>
       </c>
     </row>
@@ -5543,148 +5601,124 @@
       <c r="E7" s="14">
         <v>1</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="37" t="s">
         <v>213</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="J7" s="11">
+      <c r="J7" s="14">
         <v>1</v>
       </c>
-      <c r="K7" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>236</v>
+      <c r="K7" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
       <c r="E8" s="14">
         <v>2</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="37" t="s">
         <v>219</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="J8" s="11">
+      <c r="J8" s="14">
         <v>2</v>
       </c>
-      <c r="K8" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="M8" s="11"/>
+      <c r="K8" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="9" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
       <c r="E9" s="14">
         <v>3</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>248</v>
+      <c r="F9" s="37" t="s">
+        <v>246</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="H9" s="24"/>
-      <c r="J9" s="11">
+      <c r="J9" s="14">
         <v>3</v>
       </c>
-      <c r="K9" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="M9" s="11"/>
+      <c r="K9" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="10" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
       <c r="E10" s="14">
         <v>4</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>249</v>
+      <c r="F10" s="37" t="s">
+        <v>247</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="H10" s="24"/>
-      <c r="J10" s="11">
+      <c r="J10" s="14">
         <v>4</v>
       </c>
-      <c r="K10" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="M10" s="11"/>
+      <c r="K10" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="11" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
       <c r="E11" s="14">
         <v>5</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="37" t="s">
         <v>220</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="H11" s="24"/>
-      <c r="J11" s="11">
-        <v>5</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="M11" s="11"/>
     </row>
     <row r="12" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
       <c r="E12" s="14">
         <v>6</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>250</v>
+      <c r="F12" s="37" t="s">
+        <v>248</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="H12" s="24"/>
-      <c r="J12" s="11">
-        <v>6</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="L12" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="M12" s="11"/>
-    </row>
-    <row r="13" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H13" s="24"/>
-      <c r="J13" s="11">
-        <v>7</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="M13" s="11"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H14" s="24"/>
@@ -5712,7 +5746,7 @@
     </row>
     <row r="17" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
       <c r="C17" s="32" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H17" s="24"/>
     </row>
@@ -5778,7 +5812,7 @@
         <v>231</v>
       </c>
       <c r="M21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
@@ -5786,17 +5820,17 @@
         <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="H22" s="24"/>
       <c r="J22">
         <v>2</v>
       </c>
       <c r="K22" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="L22" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
@@ -5804,17 +5838,17 @@
         <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="H23" s="24"/>
       <c r="J23">
         <v>3</v>
       </c>
       <c r="K23" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="L23" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -5822,17 +5856,17 @@
         <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="H24" s="24"/>
       <c r="J24">
         <v>4</v>
       </c>
       <c r="K24" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="L24" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -5840,17 +5874,17 @@
         <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="H25" s="24"/>
       <c r="J25">
         <v>5</v>
       </c>
       <c r="K25" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="L25" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -5858,17 +5892,17 @@
         <v>6</v>
       </c>
       <c r="F26" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="H26" s="24"/>
       <c r="J26">
         <v>6</v>
       </c>
       <c r="K26" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="L26" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
@@ -5897,7 +5931,7 @@
     </row>
     <row r="30" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
       <c r="C30" s="32" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H30" s="24"/>
     </row>
@@ -5963,7 +5997,7 @@
         <v>230</v>
       </c>
       <c r="M34" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
@@ -5971,17 +6005,17 @@
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H35" s="24"/>
       <c r="J35">
         <v>2</v>
       </c>
       <c r="K35" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="L35" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
@@ -5989,17 +6023,17 @@
         <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="H36" s="24"/>
       <c r="J36">
         <v>3</v>
       </c>
       <c r="K36" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="L36" s="33" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6007,17 +6041,17 @@
         <v>3</v>
       </c>
       <c r="F37" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="H37" s="24"/>
       <c r="J37">
         <v>4</v>
       </c>
       <c r="K37" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="L37" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6025,17 +6059,17 @@
         <v>4</v>
       </c>
       <c r="F38" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="H38" s="24"/>
       <c r="J38">
         <v>5</v>
       </c>
       <c r="K38" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="L38" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6043,17 +6077,17 @@
         <v>5</v>
       </c>
       <c r="F39" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="H39" s="24"/>
       <c r="J39">
         <v>6</v>
       </c>
       <c r="K39" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="L39" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
@@ -6145,10 +6179,10 @@
         <v>229</v>
       </c>
       <c r="L47" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M47" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -6156,14 +6190,14 @@
         <v>2</v>
       </c>
       <c r="F48" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H48" s="24"/>
       <c r="K48" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="L48" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
@@ -6171,14 +6205,14 @@
         <v>3</v>
       </c>
       <c r="F49" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="H49" s="24"/>
       <c r="K49" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="L49" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6186,14 +6220,14 @@
         <v>4</v>
       </c>
       <c r="F50" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="H50" s="24"/>
       <c r="K50" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="L50" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6201,14 +6235,14 @@
         <v>5</v>
       </c>
       <c r="F51" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="H51" s="24"/>
       <c r="K51" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="L51" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6216,14 +6250,14 @@
         <v>6</v>
       </c>
       <c r="F52" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="H52" s="24"/>
       <c r="K52" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="L52" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.3">
@@ -6315,10 +6349,10 @@
         <v>229</v>
       </c>
       <c r="L60" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M60" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
@@ -6326,17 +6360,17 @@
         <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="H61" s="24"/>
       <c r="J61">
         <v>2</v>
       </c>
       <c r="K61" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="L61" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.3">
@@ -6344,17 +6378,17 @@
         <v>3</v>
       </c>
       <c r="F62" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="H62" s="24"/>
       <c r="J62">
         <v>3</v>
       </c>
       <c r="K62" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="L62" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6362,17 +6396,17 @@
         <v>4</v>
       </c>
       <c r="F63" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="H63" s="24"/>
       <c r="J63">
         <v>4</v>
       </c>
       <c r="K63" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="L63" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
     </row>
     <row r="64" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -6380,17 +6414,17 @@
         <v>5</v>
       </c>
       <c r="F64" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="H64" s="24"/>
       <c r="J64">
         <v>5</v>
       </c>
       <c r="K64" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="L64" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -6399,10 +6433,10 @@
         <v>6</v>
       </c>
       <c r="K65" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="L65" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -6494,10 +6528,10 @@
         <v>229</v>
       </c>
       <c r="L73" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M73" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.3">
@@ -6505,14 +6539,14 @@
         <v>2</v>
       </c>
       <c r="F74" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="H74" s="24"/>
       <c r="K74" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="L74" s="33" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.3">
@@ -6520,14 +6554,14 @@
         <v>3</v>
       </c>
       <c r="F75" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="H75" s="24"/>
       <c r="K75" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="L75" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
     </row>
     <row r="76" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6535,14 +6569,14 @@
         <v>4</v>
       </c>
       <c r="F76" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="H76" s="24"/>
       <c r="K76" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="L76" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
     </row>
     <row r="77" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6550,23 +6584,23 @@
         <v>5</v>
       </c>
       <c r="F77" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="H77" s="24"/>
       <c r="K77" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="L77" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H78" s="24"/>
       <c r="K78" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="L78" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Give final touch to Overview page
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B1E7DD-4251-452B-8A4B-98FA61499197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED463BA8-A1DB-48E4-B05A-023597A960D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="5" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
@@ -5535,8 +5535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD85EE9-7333-4E1C-BE00-8EC167B0E968}">
   <dimension ref="A3:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Work on product page and 70% done
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED463BA8-A1DB-48E4-B05A-023597A960D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC02C5E0-FA54-4527-B921-4C40AECFEAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="5" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="339">
   <si>
     <t>Table Name</t>
   </si>
@@ -689,9 +689,6 @@
     <t>Insight</t>
   </si>
   <si>
-    <t>Top Selling Category</t>
-  </si>
-  <si>
     <t>Top Seller</t>
   </si>
   <si>
@@ -704,9 +701,6 @@
     <t>Average Rating</t>
   </si>
   <si>
-    <t>Identifies the product category that contributes the highest number of orders, showing customer buying preference.</t>
-  </si>
-  <si>
     <t>Highlights the seller generating the most revenue, revealing the strongest performer on the platform.</t>
   </si>
   <si>
@@ -791,36 +785,6 @@
     <t>Top 10 Products by Revenue (Bar Chart)</t>
   </si>
   <si>
-    <t>Top Selling Product (By Quantity)</t>
-  </si>
-  <si>
-    <t>Top Revenue Product</t>
-  </si>
-  <si>
-    <t>Average Product Rating</t>
-  </si>
-  <si>
-    <t>Avg Shipping Cost Per Product</t>
-  </si>
-  <si>
-    <t>Total Products→ DISTINCTCOUNT(Product ID)</t>
-  </si>
-  <si>
-    <t>Category-wise Sales (Bar Chart)</t>
-  </si>
-  <si>
-    <t>Top 10 Best Selling Products (Horizontal Bar)</t>
-  </si>
-  <si>
-    <t>Product Weight vs Shipping Cost (Scatter Plot)</t>
-  </si>
-  <si>
-    <t>Product Dimension Distribution (Treemap)</t>
-  </si>
-  <si>
-    <t>Product Rating Distribution (Column Chart)</t>
-  </si>
-  <si>
     <t>Top Seller by Revenue</t>
   </si>
   <si>
@@ -861,18 +825,6 @@
   </si>
   <si>
     <t>Sellers vs Revenue</t>
-  </si>
-  <si>
-    <t>Category vs Revenue</t>
-  </si>
-  <si>
-    <t>Total Quantity Sold</t>
-  </si>
-  <si>
-    <t>Weight (g) → Shipping Cost</t>
-  </si>
-  <si>
-    <t>Category → Product Count</t>
   </si>
   <si>
     <t>Rating Category vs Count</t>
@@ -1108,6 +1060,54 @@
       </rPr>
       <t>Total Revenue</t>
     </r>
+  </si>
+  <si>
+    <t>Total Products</t>
+  </si>
+  <si>
+    <t>Active Products</t>
+  </si>
+  <si>
+    <t>Avg Shipping Cost</t>
+  </si>
+  <si>
+    <t>Avg Delivery Time</t>
+  </si>
+  <si>
+    <t>Insight (Easy, Professional)</t>
+  </si>
+  <si>
+    <t>Shows the total number of products in the catalog. Helps track catalog growth and overall marketplace inventory.</t>
+  </si>
+  <si>
+    <t>Indicates how many products have been ordered at least once. Helps identify products that are engaging customers.</t>
+  </si>
+  <si>
+    <t>Shows the average shipping cost per product. Helps monitor logistics expenses and manage delivery costs.</t>
+  </si>
+  <si>
+    <t>Displays the average delivery time per product. Helps evaluate delivery efficiency and customer satisfaction.</t>
+  </si>
+  <si>
+    <t>Monthly Order Trend (Linr Chart)</t>
+  </si>
+  <si>
+    <t>Top 5 Product by Volume</t>
+  </si>
+  <si>
+    <t>Category, Volume(cm2)</t>
+  </si>
+  <si>
+    <t>Top 5 Product by Quantity Sold (Orders)</t>
+  </si>
+  <si>
+    <t>Category, COUNT(OrderID)</t>
+  </si>
+  <si>
+    <t>Bottom 5 Product by Revenue</t>
+  </si>
+  <si>
+    <t>Category, Total Revenue</t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1265,6 +1265,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1304,7 +1310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1387,6 +1393,11 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4215,7 +4226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035EC863-7662-4F46-A1E6-DDC33702C1E8}">
   <dimension ref="C3:H103"/>
   <sheetViews>
-    <sheetView topLeftCell="A99" zoomScale="96" workbookViewId="0">
+    <sheetView topLeftCell="A78" zoomScale="96" workbookViewId="0">
       <selection activeCell="F3" sqref="F3:H102"/>
     </sheetView>
   </sheetViews>
@@ -4232,7 +4243,7 @@
   <sheetData>
     <row r="3" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="F3" s="13" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4418,7 +4429,7 @@
     </row>
     <row r="19" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="F19" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -5048,7 +5059,7 @@
     </row>
     <row r="82" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="F82" s="13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="83" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -5172,7 +5183,7 @@
     </row>
     <row r="96" spans="3:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="F96" s="13" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="97" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -5535,8 +5546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD85EE9-7333-4E1C-BE00-8EC167B0E968}">
   <dimension ref="A3:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:M10"/>
+    <sheetView tabSelected="1" topLeftCell="H10" zoomScale="88" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5568,7 +5579,7 @@
       <c r="G5" s="12"/>
       <c r="H5" s="24"/>
       <c r="I5" s="35" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -5580,17 +5591,17 @@
         <v>214</v>
       </c>
       <c r="G6" s="36" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="H6" s="24"/>
       <c r="J6" s="36" t="s">
         <v>57</v>
       </c>
       <c r="K6" s="36" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L6" s="36" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="M6" s="36" t="s">
         <v>215</v>
@@ -5605,20 +5616,20 @@
         <v>213</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="H7" s="24"/>
       <c r="J7" s="14">
         <v>1</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
@@ -5626,23 +5637,23 @@
         <v>2</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="H8" s="24"/>
       <c r="J8" s="14">
         <v>2</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
@@ -5650,23 +5661,23 @@
         <v>3</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="H9" s="24"/>
       <c r="J9" s="14">
         <v>3</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
@@ -5674,23 +5685,23 @@
         <v>4</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="H10" s="24"/>
       <c r="J10" s="14">
         <v>4</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
@@ -5698,10 +5709,10 @@
         <v>5</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="H11" s="24"/>
     </row>
@@ -5710,10 +5721,10 @@
         <v>6</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="H12" s="24"/>
     </row>
@@ -5745,8 +5756,8 @@
       <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="C17" s="32" t="s">
-        <v>240</v>
+      <c r="C17" s="38" t="s">
+        <v>238</v>
       </c>
       <c r="H17" s="24"/>
     </row>
@@ -5754,7 +5765,7 @@
       <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="40" t="s">
         <v>212</v>
       </c>
       <c r="E19" s="12"/>
@@ -5762,148 +5773,132 @@
       <c r="G19" s="12"/>
       <c r="H19" s="24"/>
       <c r="I19" s="31" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D20" s="12"/>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="39" t="s">
         <v>214</v>
       </c>
-      <c r="G20" s="12" t="s">
-        <v>215</v>
+      <c r="G20" s="39" t="s">
+        <v>327</v>
       </c>
       <c r="H20" s="24"/>
       <c r="J20" s="12" t="s">
         <v>57</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L20" s="12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M20" s="12" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
       <c r="D21" s="12"/>
-      <c r="E21" s="12">
+      <c r="E21" s="5">
         <v>1</v>
       </c>
-      <c r="F21" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="G21" t="s">
-        <v>221</v>
+      <c r="F21" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="H21" s="24"/>
       <c r="J21">
         <v>1</v>
       </c>
       <c r="K21" t="s">
+        <v>332</v>
+      </c>
+      <c r="L21" t="s">
         <v>229</v>
       </c>
-      <c r="L21" t="s">
-        <v>231</v>
-      </c>
       <c r="M21" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E22">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="E22" s="5">
         <v>2</v>
       </c>
-      <c r="F22" t="s">
-        <v>254</v>
+      <c r="F22" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>329</v>
       </c>
       <c r="H22" s="24"/>
       <c r="J22">
         <v>2</v>
       </c>
       <c r="K22" t="s">
-        <v>255</v>
+        <v>333</v>
       </c>
       <c r="L22" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E23">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="E23" s="5">
         <v>3</v>
       </c>
-      <c r="F23" t="s">
-        <v>250</v>
+      <c r="F23" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>330</v>
       </c>
       <c r="H23" s="24"/>
       <c r="J23">
         <v>3</v>
       </c>
       <c r="K23" t="s">
-        <v>256</v>
+        <v>335</v>
       </c>
       <c r="L23" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E24" s="12">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="E24" s="5">
         <v>4</v>
       </c>
-      <c r="F24" t="s">
-        <v>251</v>
+      <c r="F24" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>331</v>
       </c>
       <c r="H24" s="24"/>
       <c r="J24">
         <v>4</v>
       </c>
       <c r="K24" t="s">
-        <v>257</v>
+        <v>337</v>
       </c>
       <c r="L24" t="s">
-        <v>276</v>
+        <v>338</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E25" s="12">
-        <v>5</v>
-      </c>
-      <c r="F25" t="s">
-        <v>252</v>
-      </c>
+      <c r="E25" s="12"/>
       <c r="H25" s="24"/>
       <c r="J25">
         <v>5</v>
       </c>
-      <c r="K25" t="s">
-        <v>258</v>
-      </c>
-      <c r="L25" t="s">
-        <v>277</v>
-      </c>
     </row>
     <row r="26" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="E26" s="12">
-        <v>6</v>
-      </c>
-      <c r="F26" t="s">
-        <v>253</v>
-      </c>
+      <c r="E26" s="12"/>
       <c r="H26" s="24"/>
-      <c r="J26">
-        <v>6</v>
-      </c>
-      <c r="K26" t="s">
-        <v>259</v>
-      </c>
-      <c r="L26" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H27" s="24"/>
@@ -5931,7 +5926,7 @@
     </row>
     <row r="30" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
       <c r="C30" s="32" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H30" s="24"/>
     </row>
@@ -5947,7 +5942,7 @@
       <c r="G32" s="12"/>
       <c r="H32" s="24"/>
       <c r="I32" s="31" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -5966,10 +5961,10 @@
         <v>57</v>
       </c>
       <c r="K33" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L33" s="12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M33" s="12" t="s">
         <v>215</v>
@@ -5981,23 +5976,23 @@
         <v>1</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H34" s="24"/>
       <c r="J34">
         <v>1</v>
       </c>
       <c r="K34" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="L34" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M34" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
@@ -6005,17 +6000,17 @@
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H35" s="24"/>
       <c r="J35">
         <v>2</v>
       </c>
       <c r="K35" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="L35" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
@@ -6023,17 +6018,17 @@
         <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="H36" s="24"/>
       <c r="J36">
         <v>3</v>
       </c>
       <c r="K36" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="L36" s="33" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6041,17 +6036,17 @@
         <v>3</v>
       </c>
       <c r="F37" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="H37" s="24"/>
       <c r="J37">
         <v>4</v>
       </c>
       <c r="K37" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="L37" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6059,17 +6054,17 @@
         <v>4</v>
       </c>
       <c r="F38" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="H38" s="24"/>
       <c r="J38">
         <v>5</v>
       </c>
       <c r="K38" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="L38" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6077,17 +6072,17 @@
         <v>5</v>
       </c>
       <c r="F39" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="H39" s="24"/>
       <c r="J39">
         <v>6</v>
       </c>
       <c r="K39" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="L39" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
@@ -6132,7 +6127,7 @@
       <c r="G45" s="12"/>
       <c r="H45" s="24"/>
       <c r="I45" s="31" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6151,10 +6146,10 @@
         <v>57</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L46" s="12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M46" s="12" t="s">
         <v>215</v>
@@ -6166,23 +6161,23 @@
         <v>1</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G47" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H47" s="24"/>
       <c r="J47">
         <v>1</v>
       </c>
       <c r="K47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="L47" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M47" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -6190,14 +6185,14 @@
         <v>2</v>
       </c>
       <c r="F48" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H48" s="24"/>
       <c r="K48" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="L48" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
@@ -6205,14 +6200,14 @@
         <v>3</v>
       </c>
       <c r="F49" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="H49" s="24"/>
       <c r="K49" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="L49" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6220,14 +6215,14 @@
         <v>4</v>
       </c>
       <c r="F50" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="H50" s="24"/>
       <c r="K50" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="L50" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6235,14 +6230,14 @@
         <v>5</v>
       </c>
       <c r="F51" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="H51" s="24"/>
       <c r="K51" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="L51" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6250,14 +6245,14 @@
         <v>6</v>
       </c>
       <c r="F52" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="H52" s="24"/>
       <c r="K52" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="L52" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.3">
@@ -6302,7 +6297,7 @@
       <c r="G58" s="12"/>
       <c r="H58" s="24"/>
       <c r="I58" s="31" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="59" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6321,10 +6316,10 @@
         <v>57</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L59" s="12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M59" s="12" t="s">
         <v>215</v>
@@ -6336,23 +6331,23 @@
         <v>1</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G60" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H60" s="24"/>
       <c r="J60">
         <v>1</v>
       </c>
       <c r="K60" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="L60" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M60" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
@@ -6360,17 +6355,17 @@
         <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="H61" s="24"/>
       <c r="J61">
         <v>2</v>
       </c>
       <c r="K61" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="L61" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.3">
@@ -6378,17 +6373,17 @@
         <v>3</v>
       </c>
       <c r="F62" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="H62" s="24"/>
       <c r="J62">
         <v>3</v>
       </c>
       <c r="K62" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="L62" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6396,17 +6391,17 @@
         <v>4</v>
       </c>
       <c r="F63" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
       <c r="H63" s="24"/>
       <c r="J63">
         <v>4</v>
       </c>
       <c r="K63" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
       <c r="L63" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
     </row>
     <row r="64" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -6414,17 +6409,17 @@
         <v>5</v>
       </c>
       <c r="F64" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="H64" s="24"/>
       <c r="J64">
         <v>5</v>
       </c>
       <c r="K64" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
       <c r="L64" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -6433,10 +6428,10 @@
         <v>6</v>
       </c>
       <c r="K65" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
       <c r="L65" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -6481,7 +6476,7 @@
       <c r="G71" s="12"/>
       <c r="H71" s="24"/>
       <c r="I71" s="31" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="72" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6500,10 +6495,10 @@
         <v>57</v>
       </c>
       <c r="K72" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L72" s="12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M72" s="12" t="s">
         <v>215</v>
@@ -6515,23 +6510,23 @@
         <v>1</v>
       </c>
       <c r="F73" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G73" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H73" s="24"/>
       <c r="J73">
         <v>1</v>
       </c>
       <c r="K73" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="L73" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M73" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.3">
@@ -6539,14 +6534,14 @@
         <v>2</v>
       </c>
       <c r="F74" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="H74" s="24"/>
       <c r="K74" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="L74" s="33" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.3">
@@ -6554,14 +6549,14 @@
         <v>3</v>
       </c>
       <c r="F75" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="H75" s="24"/>
       <c r="K75" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="L75" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
     </row>
     <row r="76" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6569,14 +6564,14 @@
         <v>4</v>
       </c>
       <c r="F76" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="H76" s="24"/>
       <c r="K76" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="L76" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
     </row>
     <row r="77" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
@@ -6584,23 +6579,23 @@
         <v>5</v>
       </c>
       <c r="F77" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="H77" s="24"/>
       <c r="K77" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="L77" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H78" s="24"/>
       <c r="K78" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="L78" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Complete Vendor Performance Page
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B7EFEA-578B-46C8-A2A4-A7694240175B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56EEE8C-C5CB-4723-97A1-93D2003EDBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="5" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="350">
   <si>
     <t>Table Name</t>
   </si>
@@ -701,9 +701,6 @@
     <t>Average Rating</t>
   </si>
   <si>
-    <t>Highlights the seller generating the most revenue, revealing the strongest performer on the platform.</t>
-  </si>
-  <si>
     <t>Shows how many unique customers placed an order in the last 30 days, measuring customer engagement and retention.</t>
   </si>
   <si>
@@ -725,9 +722,6 @@
     <t>Linr Chart</t>
   </si>
   <si>
-    <t>Order Date, Seller Revenue(KPI)</t>
-  </si>
-  <si>
     <t>Order Date, Active Customer (30 Days)(KPI)</t>
   </si>
   <si>
@@ -737,9 +731,6 @@
     <t>Review Date, Average Rating (KPI)</t>
   </si>
   <si>
-    <t>Tracks revenue contributed by sellers over time, revealing top-performing periods and sales growth patterns.</t>
-  </si>
-  <si>
     <t>Shows how customer engagement varies monthly by measuring how many unique customers placed orders in recent periods.</t>
   </si>
   <si>
@@ -779,46 +770,13 @@
     <t>Top 10 Products by Revenue (Bar Chart)</t>
   </si>
   <si>
-    <t>Top Seller by Revenue</t>
-  </si>
-  <si>
-    <t>Avg Seller Rating</t>
-  </si>
-  <si>
-    <t>Orders per Seller</t>
-  </si>
-  <si>
-    <t>On-Time Delivery by Seller (%)</t>
-  </si>
-  <si>
-    <t>Seller Revenue Ranking (Bar Chart)</t>
-  </si>
-  <si>
-    <t>Seller Fulfillment Performance (Cluster Bar)</t>
-  </si>
-  <si>
     <t>Geo Distribution of Sellers (Map)</t>
   </si>
   <si>
     <t>Seller Category Performance (Matrix/Table)</t>
   </si>
   <si>
-    <t>Seller Shipping Cost Trend (Line)</t>
-  </si>
-  <si>
-    <t>Seller vs Avg Shipping Cost</t>
-  </si>
-  <si>
     <t>Seller → Product Category → Revenue</t>
-  </si>
-  <si>
-    <t>Postal Code → Sellers Count</t>
-  </si>
-  <si>
-    <t>On-time vs Late Deliveries by Seller</t>
-  </si>
-  <si>
-    <t>Sellers vs Revenue</t>
   </si>
   <si>
     <t>Rating Category vs Count</t>
@@ -1156,6 +1114,63 @@
       </rPr>
       <t>COUNT(Orders[OrderID])</t>
     </r>
+  </si>
+  <si>
+    <t>Seller Revenue</t>
+  </si>
+  <si>
+    <t>Highlights the seller generating the highest total revenue, identifying the strongest performer.</t>
+  </si>
+  <si>
+    <t>Shows how many sellers are registered on the platform.</t>
+  </si>
+  <si>
+    <t>Active Sellers</t>
+  </si>
+  <si>
+    <t>Shows the number of sellers who made at least one sale during the selected period.</t>
+  </si>
+  <si>
+    <t>Displays total revenue generated by all sellers combined.</t>
+  </si>
+  <si>
+    <t>Seller ID, Seller Revenue</t>
+  </si>
+  <si>
+    <t>Used Column(s)</t>
+  </si>
+  <si>
+    <t>Monthly Seller Revenue Trend (Line Chart)</t>
+  </si>
+  <si>
+    <t>Order Date, Seller Revenue (KPI)</t>
+  </si>
+  <si>
+    <t>Tracks total seller revenue month-wise to identify growth patterns and high-performing periods.</t>
+  </si>
+  <si>
+    <t>Shows which sellers generate the highest revenue, helping identify top contributors.</t>
+  </si>
+  <si>
+    <t>Seller ID, COUNT(Order ID)</t>
+  </si>
+  <si>
+    <t>Identifies sellers with the highest order count, highlighting high-volume sellers.</t>
+  </si>
+  <si>
+    <t>Country, COUNT(Seller ID)</t>
+  </si>
+  <si>
+    <t>Shows seller presence by geography, useful for understanding market penetration.</t>
+  </si>
+  <si>
+    <t>Shows revenue breakdown by seller and product category, helping analyze which categories perform best for each seller.</t>
+  </si>
+  <si>
+    <t>Top 5 Sellers by Revenue (Bar Chart)</t>
+  </si>
+  <si>
+    <t>Top 5 Sellers by Sold Quantity (Column Chart)</t>
   </si>
 </sst>
 </file>
@@ -1239,7 +1254,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1324,6 +1339,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1363,7 +1384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1451,6 +1472,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4296,7 +4323,7 @@
   <sheetData>
     <row r="3" spans="3:8" ht="23.4">
       <c r="F3" s="13" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="3:8" ht="15.6">
@@ -4482,7 +4509,7 @@
     </row>
     <row r="19" spans="3:8" ht="23.4">
       <c r="F19" s="13" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="15.6">
@@ -5112,7 +5139,7 @@
     </row>
     <row r="82" spans="3:8" ht="23.4">
       <c r="F82" s="13" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="83" spans="3:8" ht="15.6">
@@ -5236,7 +5263,7 @@
     </row>
     <row r="96" spans="3:8" ht="23.4">
       <c r="F96" s="13" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="97" spans="3:8" ht="15.6">
@@ -5599,8 +5626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD85EE9-7333-4E1C-BE00-8EC167B0E968}">
   <dimension ref="A3:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="88" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5632,7 +5659,7 @@
       <c r="G5" s="12"/>
       <c r="H5" s="24"/>
       <c r="I5" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.6">
@@ -5644,17 +5671,17 @@
         <v>214</v>
       </c>
       <c r="G6" s="36" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="H6" s="24"/>
       <c r="J6" s="36" t="s">
         <v>57</v>
       </c>
       <c r="K6" s="36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L6" s="36" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="M6" s="36" t="s">
         <v>215</v>
@@ -5669,20 +5696,20 @@
         <v>213</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="H7" s="24"/>
       <c r="J7" s="14">
         <v>1</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="31.2">
@@ -5693,20 +5720,20 @@
         <v>218</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="H8" s="24"/>
       <c r="J8" s="14">
         <v>2</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="31.2">
@@ -5714,23 +5741,23 @@
         <v>3</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="H9" s="24"/>
       <c r="J9" s="14">
         <v>3</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="31.2">
@@ -5738,23 +5765,23 @@
         <v>4</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="H10" s="24"/>
       <c r="J10" s="14">
         <v>4</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="31.2">
@@ -5765,7 +5792,7 @@
         <v>219</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="H11" s="24"/>
     </row>
@@ -5774,10 +5801,10 @@
         <v>6</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="H12" s="24"/>
     </row>
@@ -5810,7 +5837,7 @@
     </row>
     <row r="17" spans="1:16" ht="25.8">
       <c r="C17" s="38" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H17" s="24"/>
     </row>
@@ -5826,7 +5853,7 @@
       <c r="G19" s="12"/>
       <c r="H19" s="24"/>
       <c r="I19" s="40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.6">
@@ -5838,20 +5865,20 @@
         <v>214</v>
       </c>
       <c r="G20" s="39" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="H20" s="24"/>
       <c r="J20" s="39" t="s">
         <v>57</v>
       </c>
       <c r="K20" s="39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L20" s="39" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="M20" s="39" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="31.2">
@@ -5860,23 +5887,23 @@
         <v>1</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="H21" s="24"/>
       <c r="J21" s="5">
         <v>1</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="31.2">
@@ -5884,23 +5911,23 @@
         <v>2</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="H22" s="24"/>
       <c r="J22" s="5">
         <v>2</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="31.2">
@@ -5908,23 +5935,23 @@
         <v>3</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="H23" s="24"/>
       <c r="J23" s="5">
         <v>3</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="31.2">
@@ -5932,23 +5959,23 @@
         <v>4</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="H24" s="24"/>
       <c r="J24" s="5">
         <v>4</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.6">
@@ -5958,13 +5985,13 @@
         <v>5</v>
       </c>
       <c r="K25" s="14" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.6">
@@ -5996,8 +6023,8 @@
       <c r="H29" s="24"/>
     </row>
     <row r="30" spans="1:16" ht="25.8">
-      <c r="C30" s="32" t="s">
-        <v>237</v>
+      <c r="C30" s="41" t="s">
+        <v>234</v>
       </c>
       <c r="H30" s="24"/>
     </row>
@@ -6005,156 +6032,158 @@
       <c r="H31" s="24"/>
     </row>
     <row r="32" spans="1:16" ht="21">
-      <c r="D32" s="31" t="s">
+      <c r="D32" s="42" t="s">
         <v>212</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
       <c r="H32" s="24"/>
-      <c r="I32" s="31" t="s">
-        <v>224</v>
+      <c r="I32" s="44" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.6">
       <c r="D33" s="12"/>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="F33" s="12" t="s">
+      <c r="F33" s="43" t="s">
         <v>214</v>
       </c>
-      <c r="G33" s="12" t="s">
+      <c r="G33" s="43" t="s">
         <v>215</v>
       </c>
       <c r="H33" s="24"/>
-      <c r="J33" s="12" t="s">
+      <c r="J33" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="K33" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="L33" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="M33" s="12" t="s">
+      <c r="K33" s="43" t="s">
+        <v>224</v>
+      </c>
+      <c r="L33" s="43" t="s">
+        <v>338</v>
+      </c>
+      <c r="M33" s="43" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="15.6">
+    <row r="34" spans="1:16" ht="31.2">
       <c r="D34" s="12"/>
-      <c r="E34" s="12">
+      <c r="E34" s="14">
         <v>1</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="G34" t="s">
-        <v>220</v>
+      <c r="G34" s="5" t="s">
+        <v>332</v>
       </c>
       <c r="H34" s="24"/>
-      <c r="J34">
+      <c r="J34" s="14">
         <v>1</v>
       </c>
-      <c r="K34" t="s">
-        <v>227</v>
-      </c>
-      <c r="L34" t="s">
-        <v>228</v>
-      </c>
-      <c r="M34" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16">
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="K34" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="M34" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="15.6">
+      <c r="E35" s="14">
+        <v>2</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="H35" s="24"/>
+      <c r="J35" s="14">
+        <v>2</v>
+      </c>
+      <c r="K35" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="15.6">
+      <c r="E36" s="14">
+        <v>3</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="H36" s="24"/>
+      <c r="J36" s="14">
+        <v>3</v>
+      </c>
+      <c r="K36" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="15.6">
+      <c r="E37" s="14">
+        <v>4</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="H37" s="24"/>
+      <c r="J37" s="14">
+        <v>4</v>
+      </c>
+      <c r="K37" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="H35" s="24"/>
-      <c r="J35">
-        <v>2</v>
-      </c>
-      <c r="K35" t="s">
-        <v>250</v>
-      </c>
-      <c r="L35" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16">
-      <c r="E36">
-        <v>2</v>
-      </c>
-      <c r="F36" t="s">
-        <v>246</v>
-      </c>
-      <c r="H36" s="24"/>
-      <c r="J36">
-        <v>3</v>
-      </c>
-      <c r="K36" t="s">
-        <v>251</v>
-      </c>
-      <c r="L36" s="33" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="15.6">
-      <c r="E37" s="12">
-        <v>3</v>
-      </c>
-      <c r="F37" t="s">
-        <v>247</v>
-      </c>
-      <c r="H37" s="24"/>
-      <c r="J37">
-        <v>4</v>
-      </c>
-      <c r="K37" t="s">
-        <v>252</v>
-      </c>
-      <c r="L37" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" ht="15.6">
-      <c r="E38" s="12">
-        <v>4</v>
-      </c>
-      <c r="F38" t="s">
-        <v>248</v>
-      </c>
+      <c r="L37" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="31.2">
+      <c r="E38" s="12"/>
       <c r="H38" s="24"/>
-      <c r="J38">
+      <c r="J38" s="14">
         <v>5</v>
       </c>
-      <c r="K38" t="s">
-        <v>253</v>
-      </c>
-      <c r="L38" t="s">
-        <v>256</v>
+      <c r="K38" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.6">
-      <c r="E39" s="12">
-        <v>5</v>
-      </c>
-      <c r="F39" t="s">
-        <v>249</v>
-      </c>
+      <c r="E39" s="12"/>
       <c r="H39" s="24"/>
-      <c r="J39">
-        <v>6</v>
-      </c>
-      <c r="K39" t="s">
-        <v>254</v>
-      </c>
-      <c r="L39" t="s">
-        <v>255</v>
-      </c>
     </row>
     <row r="40" spans="1:16">
       <c r="H40" s="24"/>
@@ -6198,7 +6227,7 @@
       <c r="G45" s="12"/>
       <c r="H45" s="24"/>
       <c r="I45" s="31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15.6">
@@ -6217,10 +6246,10 @@
         <v>57</v>
       </c>
       <c r="K46" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="L46" s="12" t="s">
         <v>225</v>
-      </c>
-      <c r="L46" s="12" t="s">
-        <v>226</v>
       </c>
       <c r="M46" s="12" t="s">
         <v>215</v>
@@ -6235,20 +6264,20 @@
         <v>217</v>
       </c>
       <c r="G47" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H47" s="24"/>
       <c r="J47">
         <v>1</v>
       </c>
       <c r="K47" t="s">
+        <v>226</v>
+      </c>
+      <c r="L47" t="s">
         <v>227</v>
       </c>
-      <c r="L47" t="s">
-        <v>229</v>
-      </c>
       <c r="M47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -6256,14 +6285,14 @@
         <v>2</v>
       </c>
       <c r="F48" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H48" s="24"/>
       <c r="K48" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="L48" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -6271,14 +6300,14 @@
         <v>3</v>
       </c>
       <c r="F49" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="H49" s="24"/>
       <c r="K49" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="L49" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="15.6">
@@ -6286,14 +6315,14 @@
         <v>4</v>
       </c>
       <c r="F50" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="H50" s="24"/>
       <c r="K50" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="L50" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="15.6">
@@ -6301,14 +6330,14 @@
         <v>5</v>
       </c>
       <c r="F51" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="H51" s="24"/>
       <c r="K51" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="L51" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="15.6">
@@ -6316,14 +6345,14 @@
         <v>6</v>
       </c>
       <c r="F52" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="H52" s="24"/>
       <c r="K52" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="L52" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
     </row>
     <row r="53" spans="1:16">
@@ -6368,7 +6397,7 @@
       <c r="G58" s="12"/>
       <c r="H58" s="24"/>
       <c r="I58" s="31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="59" spans="1:16" ht="15.6">
@@ -6387,10 +6416,10 @@
         <v>57</v>
       </c>
       <c r="K59" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="L59" s="12" t="s">
         <v>225</v>
-      </c>
-      <c r="L59" s="12" t="s">
-        <v>226</v>
       </c>
       <c r="M59" s="12" t="s">
         <v>215</v>
@@ -6405,20 +6434,20 @@
         <v>218</v>
       </c>
       <c r="G60" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H60" s="24"/>
       <c r="J60">
         <v>1</v>
       </c>
       <c r="K60" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L60" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M60" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="61" spans="1:16">
@@ -6426,17 +6455,17 @@
         <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="H61" s="24"/>
       <c r="J61">
         <v>2</v>
       </c>
       <c r="K61" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="L61" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
     </row>
     <row r="62" spans="1:16">
@@ -6444,17 +6473,17 @@
         <v>3</v>
       </c>
       <c r="F62" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="H62" s="24"/>
       <c r="J62">
         <v>3</v>
       </c>
       <c r="K62" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="L62" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="15.6">
@@ -6462,17 +6491,17 @@
         <v>4</v>
       </c>
       <c r="F63" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="H63" s="24"/>
       <c r="J63">
         <v>4</v>
       </c>
       <c r="K63" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="L63" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="64" spans="1:16" ht="15.6" customHeight="1">
@@ -6480,17 +6509,17 @@
         <v>5</v>
       </c>
       <c r="F64" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="H64" s="24"/>
       <c r="J64">
         <v>5</v>
       </c>
       <c r="K64" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="L64" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="15.6" customHeight="1">
@@ -6499,10 +6528,10 @@
         <v>6</v>
       </c>
       <c r="K65" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="L65" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="15.6" customHeight="1">
@@ -6547,7 +6576,7 @@
       <c r="G71" s="12"/>
       <c r="H71" s="24"/>
       <c r="I71" s="31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="72" spans="1:16" ht="15.6">
@@ -6566,10 +6595,10 @@
         <v>57</v>
       </c>
       <c r="K72" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="L72" s="12" t="s">
         <v>225</v>
-      </c>
-      <c r="L72" s="12" t="s">
-        <v>226</v>
       </c>
       <c r="M72" s="12" t="s">
         <v>215</v>
@@ -6584,20 +6613,20 @@
         <v>219</v>
       </c>
       <c r="G73" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H73" s="24"/>
       <c r="J73">
         <v>1</v>
       </c>
       <c r="K73" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L73" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="M73" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="74" spans="1:16">
@@ -6605,14 +6634,14 @@
         <v>2</v>
       </c>
       <c r="F74" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="H74" s="24"/>
       <c r="K74" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="L74" s="33" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
     </row>
     <row r="75" spans="1:16">
@@ -6620,14 +6649,14 @@
         <v>3</v>
       </c>
       <c r="F75" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="H75" s="24"/>
       <c r="K75" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="L75" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="76" spans="1:16" ht="15.6">
@@ -6635,14 +6664,14 @@
         <v>4</v>
       </c>
       <c r="F76" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="H76" s="24"/>
       <c r="K76" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="L76" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
     </row>
     <row r="77" spans="1:16" ht="15.6">
@@ -6650,23 +6679,23 @@
         <v>5</v>
       </c>
       <c r="F77" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="H77" s="24"/>
       <c r="K77" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="L77" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
     </row>
     <row r="78" spans="1:16">
       <c r="H78" s="24"/>
       <c r="K78" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="L78" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="79" spans="1:16">

</xml_diff>

<commit_message>
Complete 60% work on Customer Page
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56EEE8C-C5CB-4723-97A1-93D2003EDBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA493CD-4E7E-4691-BB53-7E96A190E148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="5" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="350">
   <si>
     <t>Table Name</t>
   </si>
@@ -692,18 +692,12 @@
     <t>Top Seller</t>
   </si>
   <si>
-    <t>Active Customer (30 Days)</t>
-  </si>
-  <si>
     <t>Total Revenue</t>
   </si>
   <si>
     <t>Average Rating</t>
   </si>
   <si>
-    <t>Shows how many unique customers placed an order in the last 30 days, measuring customer engagement and retention.</t>
-  </si>
-  <si>
     <t>Represents total earnings from customer payments, reflecting the financial health of the business.</t>
   </si>
   <si>
@@ -782,18 +776,9 @@
     <t>Rating Category vs Count</t>
   </si>
   <si>
-    <t>New Customers (MTD / YTD)</t>
-  </si>
-  <si>
     <t>Avg Age of Customers</t>
   </si>
   <si>
-    <t>Repeat Purchase Rate</t>
-  </si>
-  <si>
-    <t>Customer Lifetime Value (CLV)</t>
-  </si>
-  <si>
     <t>Age Group Distribution (Column Chart)</t>
   </si>
   <si>
@@ -903,9 +888,6 @@
   </si>
   <si>
     <t>Monthly Rating Trend</t>
-  </si>
-  <si>
-    <t>Insight (Easy, Professional Explanation)</t>
   </si>
   <si>
     <t>Shows how many orders were successfully delivered. A higher number means strong customer demand and good overall marketplace activity.</t>
@@ -1171,6 +1153,24 @@
   </si>
   <si>
     <t>Top 5 Sellers by Sold Quantity (Column Chart)</t>
+  </si>
+  <si>
+    <t>Active Customers (Last 30 Days)</t>
+  </si>
+  <si>
+    <t>Shows how many unique customers placed at least one order in the past 30 days. This helps measure customer engagement, activity level, and short-term retention.</t>
+  </si>
+  <si>
+    <t>Represents the overall number of unique registered customers. It reflects the size of the customer base and long-term acquisition success.</t>
+  </si>
+  <si>
+    <t>Displays the average age of all customers, helping identify the dominant age group and supporting customer segmentation analysis.</t>
+  </si>
+  <si>
+    <t>Avg Customer Rating</t>
+  </si>
+  <si>
+    <t>Shows the average product/service rating given by customers. A higher average rating means better service quality and customer satisfaction.</t>
   </si>
 </sst>
 </file>
@@ -1384,7 +1384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1478,6 +1478,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4323,7 +4326,7 @@
   <sheetData>
     <row r="3" spans="3:8" ht="23.4">
       <c r="F3" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="3:8" ht="15.6">
@@ -4509,7 +4512,7 @@
     </row>
     <row r="19" spans="3:8" ht="23.4">
       <c r="F19" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="15.6">
@@ -5139,7 +5142,7 @@
     </row>
     <row r="82" spans="3:8" ht="23.4">
       <c r="F82" s="13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="83" spans="3:8" ht="15.6">
@@ -5263,7 +5266,7 @@
     </row>
     <row r="96" spans="3:8" ht="23.4">
       <c r="F96" s="13" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="97" spans="3:8" ht="15.6">
@@ -5626,8 +5629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD85EE9-7333-4E1C-BE00-8EC167B0E968}">
   <dimension ref="A3:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="88" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" topLeftCell="H37" zoomScale="88" workbookViewId="0">
+      <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5659,7 +5662,7 @@
       <c r="G5" s="12"/>
       <c r="H5" s="24"/>
       <c r="I5" s="35" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.6">
@@ -5671,17 +5674,17 @@
         <v>214</v>
       </c>
       <c r="G6" s="36" t="s">
-        <v>288</v>
+        <v>215</v>
       </c>
       <c r="H6" s="24"/>
       <c r="J6" s="36" t="s">
         <v>57</v>
       </c>
       <c r="K6" s="36" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="L6" s="36" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="M6" s="36" t="s">
         <v>215</v>
@@ -5696,20 +5699,20 @@
         <v>213</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="H7" s="24"/>
       <c r="J7" s="14">
         <v>1</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="31.2">
@@ -5717,23 +5720,23 @@
         <v>2</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="H8" s="24"/>
       <c r="J8" s="14">
         <v>2</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="31.2">
@@ -5741,23 +5744,23 @@
         <v>3</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="H9" s="24"/>
       <c r="J9" s="14">
         <v>3</v>
       </c>
       <c r="K9" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>305</v>
-      </c>
       <c r="M9" s="5" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="31.2">
@@ -5765,23 +5768,23 @@
         <v>4</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="H10" s="24"/>
       <c r="J10" s="14">
         <v>4</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="31.2">
@@ -5789,10 +5792,10 @@
         <v>5</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="H11" s="24"/>
     </row>
@@ -5801,10 +5804,10 @@
         <v>6</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H12" s="24"/>
     </row>
@@ -5837,7 +5840,7 @@
     </row>
     <row r="17" spans="1:16" ht="25.8">
       <c r="C17" s="38" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H17" s="24"/>
     </row>
@@ -5853,7 +5856,7 @@
       <c r="G19" s="12"/>
       <c r="H19" s="24"/>
       <c r="I19" s="40" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.6">
@@ -5865,20 +5868,20 @@
         <v>214</v>
       </c>
       <c r="G20" s="39" t="s">
-        <v>311</v>
+        <v>215</v>
       </c>
       <c r="H20" s="24"/>
       <c r="J20" s="39" t="s">
         <v>57</v>
       </c>
       <c r="K20" s="39" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="L20" s="39" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="M20" s="39" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="31.2">
@@ -5887,23 +5890,23 @@
         <v>1</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="H21" s="24"/>
       <c r="J21" s="5">
         <v>1</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="31.2">
@@ -5911,23 +5914,23 @@
         <v>2</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="H22" s="24"/>
       <c r="J22" s="5">
         <v>2</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="31.2">
@@ -5935,23 +5938,23 @@
         <v>3</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="H23" s="24"/>
       <c r="J23" s="5">
         <v>3</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="31.2">
@@ -5959,23 +5962,23 @@
         <v>4</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="H24" s="24"/>
       <c r="J24" s="5">
         <v>4</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="L24" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="M24" s="5" t="s">
         <v>316</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.6">
@@ -5985,13 +5988,13 @@
         <v>5</v>
       </c>
       <c r="K25" s="14" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.6">
@@ -6024,7 +6027,7 @@
     </row>
     <row r="30" spans="1:16" ht="25.8">
       <c r="C30" s="41" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H30" s="24"/>
     </row>
@@ -6040,7 +6043,7 @@
       <c r="G32" s="12"/>
       <c r="H32" s="24"/>
       <c r="I32" s="44" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.6">
@@ -6059,10 +6062,10 @@
         <v>57</v>
       </c>
       <c r="K33" s="43" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="L33" s="43" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="M33" s="43" t="s">
         <v>215</v>
@@ -6077,20 +6080,20 @@
         <v>216</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="H34" s="24"/>
       <c r="J34" s="14">
         <v>1</v>
       </c>
       <c r="K34" s="14" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.6">
@@ -6098,23 +6101,23 @@
         <v>2</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="H35" s="24"/>
       <c r="J35" s="14">
         <v>2</v>
       </c>
       <c r="K35" s="14" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.6">
@@ -6122,23 +6125,23 @@
         <v>3</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="H36" s="24"/>
       <c r="J36" s="14">
         <v>3</v>
       </c>
       <c r="K36" s="14" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.6">
@@ -6146,39 +6149,39 @@
         <v>4</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="H37" s="24"/>
       <c r="J37" s="14">
         <v>4</v>
       </c>
       <c r="K37" s="14" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" ht="31.2">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="15.6">
       <c r="E38" s="12"/>
       <c r="H38" s="24"/>
       <c r="J38" s="14">
         <v>5</v>
       </c>
       <c r="K38" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.6">
@@ -6210,7 +6213,7 @@
       <c r="H42" s="24"/>
     </row>
     <row r="43" spans="1:16" ht="25.8">
-      <c r="C43" s="32" t="s">
+      <c r="C43" s="46" t="s">
         <v>199</v>
       </c>
       <c r="H43" s="24"/>
@@ -6219,7 +6222,7 @@
       <c r="H44" s="24"/>
     </row>
     <row r="45" spans="1:16" ht="21">
-      <c r="D45" s="31" t="s">
+      <c r="D45" s="45" t="s">
         <v>212</v>
       </c>
       <c r="E45" s="12"/>
@@ -6227,18 +6230,18 @@
       <c r="G45" s="12"/>
       <c r="H45" s="24"/>
       <c r="I45" s="31" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15.6">
       <c r="D46" s="12"/>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="F46" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="G46" s="12" t="s">
+      <c r="G46" s="15" t="s">
         <v>215</v>
       </c>
       <c r="H46" s="24"/>
@@ -6246,113 +6249,112 @@
         <v>57</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="L46" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="M46" s="12" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="15.6">
+    <row r="47" spans="1:16" ht="31.2">
       <c r="D47" s="12"/>
-      <c r="E47" s="12">
+      <c r="E47" s="14">
         <v>1</v>
       </c>
-      <c r="F47" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="G47" t="s">
-        <v>220</v>
+      <c r="F47" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>345</v>
       </c>
       <c r="H47" s="24"/>
       <c r="J47">
         <v>1</v>
       </c>
-      <c r="K47" t="s">
-        <v>226</v>
+      <c r="K47" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="L47" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M47" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16">
-      <c r="E48">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="31.2">
+      <c r="E48" s="14">
         <v>2</v>
       </c>
-      <c r="F48" t="s">
-        <v>239</v>
+      <c r="F48" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>346</v>
       </c>
       <c r="H48" s="24"/>
-      <c r="K48" t="s">
-        <v>251</v>
+      <c r="K48" s="47" t="s">
+        <v>246</v>
       </c>
       <c r="L48" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16">
-      <c r="E49">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="31.2">
+      <c r="E49" s="14">
         <v>3</v>
       </c>
-      <c r="F49" t="s">
-        <v>247</v>
+      <c r="F49" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>347</v>
       </c>
       <c r="H49" s="24"/>
       <c r="K49" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="L49" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" ht="15.6">
-      <c r="E50" s="12">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="31.2">
+      <c r="E50" s="14">
         <v>4</v>
       </c>
-      <c r="F50" t="s">
-        <v>248</v>
+      <c r="F50" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>349</v>
       </c>
       <c r="H50" s="24"/>
       <c r="K50" t="s">
+        <v>248</v>
+      </c>
+      <c r="L50" t="s">
         <v>253</v>
       </c>
-      <c r="L50" t="s">
-        <v>258</v>
-      </c>
     </row>
     <row r="51" spans="1:16" ht="15.6">
-      <c r="E51" s="12">
-        <v>5</v>
-      </c>
-      <c r="F51" t="s">
+      <c r="E51" s="12"/>
+      <c r="H51" s="24"/>
+      <c r="K51" s="47" t="s">
         <v>249</v>
       </c>
-      <c r="H51" s="24"/>
-      <c r="K51" t="s">
-        <v>254</v>
-      </c>
       <c r="L51" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="15.6">
-      <c r="E52" s="12">
-        <v>6</v>
-      </c>
-      <c r="F52" t="s">
-        <v>250</v>
-      </c>
+      <c r="E52" s="12"/>
       <c r="H52" s="24"/>
       <c r="K52" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="L52" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="53" spans="1:16">
@@ -6397,7 +6399,7 @@
       <c r="G58" s="12"/>
       <c r="H58" s="24"/>
       <c r="I58" s="31" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="1:16" ht="15.6">
@@ -6416,10 +6418,10 @@
         <v>57</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="L59" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="M59" s="12" t="s">
         <v>215</v>
@@ -6431,23 +6433,23 @@
         <v>1</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G60" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H60" s="24"/>
       <c r="J60">
         <v>1</v>
       </c>
       <c r="K60" t="s">
+        <v>224</v>
+      </c>
+      <c r="L60" t="s">
         <v>226</v>
       </c>
-      <c r="L60" t="s">
-        <v>228</v>
-      </c>
       <c r="M60" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="61" spans="1:16">
@@ -6455,17 +6457,17 @@
         <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="H61" s="24"/>
       <c r="J61">
         <v>2</v>
       </c>
       <c r="K61" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="L61" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="62" spans="1:16">
@@ -6473,17 +6475,17 @@
         <v>3</v>
       </c>
       <c r="F62" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="H62" s="24"/>
       <c r="J62">
         <v>3</v>
       </c>
       <c r="K62" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="L62" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="15.6">
@@ -6491,17 +6493,17 @@
         <v>4</v>
       </c>
       <c r="F63" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H63" s="24"/>
       <c r="J63">
         <v>4</v>
       </c>
       <c r="K63" t="s">
+        <v>262</v>
+      </c>
+      <c r="L63" t="s">
         <v>267</v>
-      </c>
-      <c r="L63" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="64" spans="1:16" ht="15.6" customHeight="1">
@@ -6509,17 +6511,17 @@
         <v>5</v>
       </c>
       <c r="F64" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="H64" s="24"/>
       <c r="J64">
         <v>5</v>
       </c>
       <c r="K64" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="L64" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="15.6" customHeight="1">
@@ -6528,10 +6530,10 @@
         <v>6</v>
       </c>
       <c r="K65" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="L65" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="15.6" customHeight="1">
@@ -6576,7 +6578,7 @@
       <c r="G71" s="12"/>
       <c r="H71" s="24"/>
       <c r="I71" s="31" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="72" spans="1:16" ht="15.6">
@@ -6595,10 +6597,10 @@
         <v>57</v>
       </c>
       <c r="K72" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="L72" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="M72" s="12" t="s">
         <v>215</v>
@@ -6610,23 +6612,23 @@
         <v>1</v>
       </c>
       <c r="F73" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G73" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H73" s="24"/>
       <c r="J73">
         <v>1</v>
       </c>
       <c r="K73" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="L73" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M73" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="74" spans="1:16">
@@ -6634,14 +6636,14 @@
         <v>2</v>
       </c>
       <c r="F74" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="H74" s="24"/>
       <c r="K74" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="L74" s="33" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="75" spans="1:16">
@@ -6649,14 +6651,14 @@
         <v>3</v>
       </c>
       <c r="F75" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="H75" s="24"/>
       <c r="K75" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="L75" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="76" spans="1:16" ht="15.6">
@@ -6664,14 +6666,14 @@
         <v>4</v>
       </c>
       <c r="F76" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="H76" s="24"/>
       <c r="K76" t="s">
+        <v>276</v>
+      </c>
+      <c r="L76" t="s">
         <v>281</v>
-      </c>
-      <c r="L76" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="77" spans="1:16" ht="15.6">
@@ -6679,23 +6681,23 @@
         <v>5</v>
       </c>
       <c r="F77" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="H77" s="24"/>
       <c r="K77" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="L77" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="78" spans="1:16">
       <c r="H78" s="24"/>
       <c r="K78" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="L78" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="79" spans="1:16">

</xml_diff>

<commit_message>
Workin gon Review Pgae
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E145EF6B-C689-44A1-8E5D-B94D57D58EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902C0B9D-D123-4FAE-B7F6-0B93E251A4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="5" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="356">
   <si>
     <t>Table Name</t>
   </si>
@@ -777,9 +777,6 @@
   </si>
   <si>
     <t>% Negative Reviews (Rating 1–2)</t>
-  </si>
-  <si>
-    <t>Avg Review Delay (Order vs Review Date)</t>
   </si>
   <si>
     <t>Rating Distribution (Column Chart)</t>
@@ -5764,8 +5761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD85EE9-7333-4E1C-BE00-8EC167B0E968}">
   <dimension ref="A3:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="88" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="H60" zoomScale="88" workbookViewId="0">
+      <selection activeCell="K76" sqref="K76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5819,7 +5816,7 @@
         <v>221</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M6" s="35" t="s">
         <v>215</v>
@@ -5834,20 +5831,20 @@
         <v>213</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H7" s="24"/>
       <c r="J7" s="14">
         <v>1</v>
       </c>
       <c r="K7" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="M7" s="5" t="s">
         <v>263</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="31.2">
@@ -5858,7 +5855,7 @@
         <v>217</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H8" s="24"/>
       <c r="J8" s="14">
@@ -5868,10 +5865,10 @@
         <v>235</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="31.2">
@@ -5882,20 +5879,20 @@
         <v>232</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H9" s="24"/>
       <c r="J9" s="14">
         <v>3</v>
       </c>
       <c r="K9" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="M9" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="31.2">
@@ -5906,20 +5903,20 @@
         <v>233</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H10" s="24"/>
       <c r="J10" s="14">
         <v>4</v>
       </c>
       <c r="K10" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="M10" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="31.2">
@@ -5930,7 +5927,7 @@
         <v>218</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H11" s="24"/>
     </row>
@@ -5942,7 +5939,7 @@
         <v>234</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H12" s="24"/>
     </row>
@@ -6013,10 +6010,10 @@
         <v>221</v>
       </c>
       <c r="L20" s="38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M20" s="38" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="31.2">
@@ -6025,23 +6022,23 @@
         <v>1</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H21" s="24"/>
       <c r="J21" s="5">
         <v>1</v>
       </c>
       <c r="K21" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="M21" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="M21" s="5" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="31.2">
@@ -6049,23 +6046,23 @@
         <v>2</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H22" s="24"/>
       <c r="J22" s="5">
         <v>2</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L22" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="M22" s="5" t="s">
         <v>286</v>
-      </c>
-      <c r="M22" s="5" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="31.2">
@@ -6073,23 +6070,23 @@
         <v>3</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H23" s="24"/>
       <c r="J23" s="5">
         <v>3</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="31.2">
@@ -6097,23 +6094,23 @@
         <v>4</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H24" s="24"/>
       <c r="J24" s="5">
         <v>4</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.6">
@@ -6123,13 +6120,13 @@
         <v>5</v>
       </c>
       <c r="K25" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.6">
@@ -6200,7 +6197,7 @@
         <v>221</v>
       </c>
       <c r="L33" s="42" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M33" s="42" t="s">
         <v>215</v>
@@ -6215,20 +6212,20 @@
         <v>216</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H34" s="24"/>
       <c r="J34" s="14">
         <v>1</v>
       </c>
       <c r="K34" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="L34" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>307</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.6">
@@ -6239,20 +6236,20 @@
         <v>233</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H35" s="24"/>
       <c r="J35" s="14">
         <v>2</v>
       </c>
       <c r="K35" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.6">
@@ -6260,23 +6257,23 @@
         <v>3</v>
       </c>
       <c r="F36" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="G36" s="5" t="s">
         <v>301</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>302</v>
       </c>
       <c r="H36" s="24"/>
       <c r="J36" s="14">
         <v>3</v>
       </c>
       <c r="K36" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L36" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="M36" s="5" t="s">
         <v>310</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.6">
@@ -6284,10 +6281,10 @@
         <v>4</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H37" s="24"/>
       <c r="J37" s="14">
@@ -6297,10 +6294,10 @@
         <v>236</v>
       </c>
       <c r="L37" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="M37" s="5" t="s">
         <v>312</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.6">
@@ -6316,7 +6313,7 @@
         <v>238</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.6">
@@ -6387,10 +6384,10 @@
         <v>221</v>
       </c>
       <c r="L46" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="M46" s="15" t="s">
         <v>324</v>
-      </c>
-      <c r="M46" s="15" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="31.2">
@@ -6399,23 +6396,23 @@
         <v>1</v>
       </c>
       <c r="F47" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>317</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>318</v>
       </c>
       <c r="H47" s="24"/>
       <c r="J47" s="14">
         <v>1</v>
       </c>
       <c r="K47" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="L47" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="M47" s="5" t="s">
         <v>326</v>
-      </c>
-      <c r="L47" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="M47" s="5" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="31.2">
@@ -6426,7 +6423,7 @@
         <v>232</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H48" s="24"/>
       <c r="J48" s="14">
@@ -6436,10 +6433,10 @@
         <v>241</v>
       </c>
       <c r="L48" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="M48" s="5" t="s">
         <v>328</v>
-      </c>
-      <c r="M48" s="5" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="31.2">
@@ -6450,20 +6447,20 @@
         <v>240</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H49" s="24"/>
       <c r="J49" s="14">
         <v>3</v>
       </c>
       <c r="K49" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="L49" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="M49" s="5" t="s">
         <v>330</v>
-      </c>
-      <c r="L49" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="M49" s="5" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="31.2">
@@ -6471,23 +6468,23 @@
         <v>4</v>
       </c>
       <c r="F50" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="G50" s="5" t="s">
         <v>321</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>322</v>
       </c>
       <c r="H50" s="24"/>
       <c r="J50" s="14">
         <v>4</v>
       </c>
       <c r="K50" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="L50" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="L50" s="5" t="s">
+      <c r="M50" s="5" t="s">
         <v>333</v>
-      </c>
-      <c r="M50" s="5" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="31.2">
@@ -6497,13 +6494,13 @@
         <v>5</v>
       </c>
       <c r="K51" s="14" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="L51" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="M51" s="5" t="s">
         <v>335</v>
-      </c>
-      <c r="M51" s="5" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="15.6">
@@ -6574,7 +6571,7 @@
         <v>221</v>
       </c>
       <c r="L59" s="46" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M59" s="46" t="s">
         <v>215</v>
@@ -6589,20 +6586,20 @@
         <v>217</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H60" s="24"/>
       <c r="J60" s="14">
         <v>1</v>
       </c>
       <c r="K60" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="L60" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="M60" s="5" t="s">
         <v>348</v>
-      </c>
-      <c r="L60" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="M60" s="5" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="61" spans="1:16" ht="31.2">
@@ -6610,23 +6607,23 @@
         <v>2</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H61" s="24"/>
       <c r="J61" s="14">
         <v>2</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L61" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M61" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="62" spans="1:16" ht="31.2">
@@ -6637,20 +6634,20 @@
         <v>242</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H62" s="24"/>
       <c r="J62" s="14">
         <v>3</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L62" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="M62" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="31.2">
@@ -6658,23 +6655,23 @@
         <v>4</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H63" s="24"/>
       <c r="J63" s="14">
         <v>4</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L63" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="M63" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="64" spans="1:16" ht="15.6" customHeight="1">
@@ -6788,7 +6785,7 @@
       </c>
       <c r="H74" s="24"/>
       <c r="K74" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L74" s="32" t="s">
         <v>239</v>
@@ -6803,10 +6800,10 @@
       </c>
       <c r="H75" s="24"/>
       <c r="K75" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L75" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="76" spans="1:16" ht="15.6">
@@ -6818,34 +6815,29 @@
       </c>
       <c r="H76" s="24"/>
       <c r="K76" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L76" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="77" spans="1:16" ht="15.6">
-      <c r="E77" s="12">
-        <v>5</v>
-      </c>
-      <c r="F77" t="s">
-        <v>246</v>
-      </c>
+      <c r="E77" s="12"/>
       <c r="H77" s="24"/>
       <c r="K77" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="78" spans="1:16">
       <c r="H78" s="24"/>
       <c r="K78" t="s">
+        <v>250</v>
+      </c>
+      <c r="L78" t="s">
         <v>251</v>
-      </c>
-      <c r="L78" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="79" spans="1:16">

</xml_diff>

<commit_message>
Complete Fecon Inc Report
</commit_message>
<xml_diff>
--- a/Report/Fecom Inc Report.xlsx
+++ b/Report/Fecom Inc Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Fecom Inc Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762848C1-AA94-451C-BA76-6E931D76562E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E233FF8D-D39D-4FA0-B2B5-85537C7EFFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="5" xr2:uid="{483C6ECF-6E74-49B9-821E-7C94F0DB9B14}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="357">
   <si>
     <t>Table Name</t>
   </si>
@@ -707,18 +707,9 @@
     <t>Chart Name</t>
   </si>
   <si>
-    <t>Used Column</t>
-  </si>
-  <si>
-    <t>Linr Chart</t>
-  </si>
-  <si>
     <t>Review Date, Average Rating (KPI)</t>
   </si>
   <si>
-    <t>Displays customer satisfaction trends by showing how average product ratings change over time.</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -758,9 +749,6 @@
     <t>Seller → Product Category → Revenue</t>
   </si>
   <si>
-    <t>Rating Category vs Count</t>
-  </si>
-  <si>
     <t>Avg Age of Customers</t>
   </si>
   <si>
@@ -777,33 +765,6 @@
   </si>
   <si>
     <t>% Negative Reviews (Rating 1–2)</t>
-  </si>
-  <si>
-    <t>Rating Distribution (Column Chart)</t>
-  </si>
-  <si>
-    <t>Average Rating Over Time (Line Chart)</t>
-  </si>
-  <si>
-    <t>Product-wise Rating (Bar Chart)</t>
-  </si>
-  <si>
-    <t>Seller-wise Rating (Bar Chart)</t>
-  </si>
-  <si>
-    <t>Reviews Word Cloud (If text is available)</t>
-  </si>
-  <si>
-    <t>Text analytics</t>
-  </si>
-  <si>
-    <t>Seller vs Rating</t>
-  </si>
-  <si>
-    <t>Product vs Avg Rating</t>
-  </si>
-  <si>
-    <t>Monthly Rating Trend</t>
   </si>
   <si>
     <t>Shows how many orders were successfully delivered. A higher number means strong customer demand and good overall marketplace activity.</t>
@@ -1264,6 +1225,48 @@
       </rPr>
       <t>Avg Revenue Per Order (KPI)</t>
     </r>
+  </si>
+  <si>
+    <t>Shows the total number of customer reviews submitted, helping understand engagement and feedback volume.</t>
+  </si>
+  <si>
+    <t>Represents the percentage of highly satisfied customers who rated the product or service positively.</t>
+  </si>
+  <si>
+    <t>Highlights the percentage of unhappy customers, helping identify issues in product quality, delivery, or service.</t>
+  </si>
+  <si>
+    <t>Rating Distribution (Donut Chart)</t>
+  </si>
+  <si>
+    <t>Monthly Avg Rating (Line Chart)</t>
+  </si>
+  <si>
+    <t>Shows how customer satisfaction changes month-by-month by tracking average rating trends over time.</t>
+  </si>
+  <si>
+    <t>Rating Category, COUNT(Review ID)</t>
+  </si>
+  <si>
+    <t>Displays how ratings are spread across categories (1–5), helping identify whether customers are mostly happy or unhappy.</t>
+  </si>
+  <si>
+    <t>Top 10 Categories by Rating</t>
+  </si>
+  <si>
+    <t>Category, COUNT(Review ID)</t>
+  </si>
+  <si>
+    <t>Highlights which product categories receive the most reviews, helping identify customers' most discussed items.</t>
+  </si>
+  <si>
+    <t>Feedback in Detail (Matrix/Table)</t>
+  </si>
+  <si>
+    <t>Customer ID, Category, Volume (cm³), Avg Rating, Revenue, Status</t>
+  </si>
+  <si>
+    <t>Provides a detailed view of each customer’s feedback along with product category, size, rating, and revenue data.</t>
   </si>
 </sst>
 </file>
@@ -1505,7 +1508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1576,11 +1579,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1608,6 +1607,9 @@
     <xf numFmtId="0" fontId="11" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4458,7 +4460,7 @@
   <sheetData>
     <row r="3" spans="3:8" ht="23.4">
       <c r="F3" s="13" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="3:8" ht="15.6">
@@ -4644,7 +4646,7 @@
     </row>
     <row r="19" spans="3:8" ht="23.4">
       <c r="F19" s="13" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="15.6">
@@ -5274,7 +5276,7 @@
     </row>
     <row r="82" spans="3:8" ht="23.4">
       <c r="F82" s="13" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="83" spans="3:8" ht="15.6">
@@ -5398,7 +5400,7 @@
     </row>
     <row r="96" spans="3:8" ht="23.4">
       <c r="F96" s="13" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="97" spans="3:8" ht="15.6">
@@ -5761,8 +5763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD85EE9-7333-4E1C-BE00-8EC167B0E968}">
   <dimension ref="A3:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H60" zoomScale="88" workbookViewId="0">
-      <selection activeCell="K78" sqref="K78:L78"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5786,39 +5788,39 @@
       <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:16" ht="21">
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="32" t="s">
         <v>212</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="24"/>
-      <c r="I5" s="34" t="s">
+      <c r="I5" s="32" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.6">
       <c r="D6" s="12"/>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="33" t="s">
         <v>215</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="J6" s="35" t="s">
+      <c r="J6" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="35" t="s">
+      <c r="K6" s="33" t="s">
         <v>221</v>
       </c>
-      <c r="L6" s="35" t="s">
-        <v>261</v>
-      </c>
-      <c r="M6" s="35" t="s">
+      <c r="L6" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="M6" s="33" t="s">
         <v>215</v>
       </c>
     </row>
@@ -5827,107 +5829,107 @@
       <c r="E7" s="14">
         <v>1</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="34" t="s">
         <v>213</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="H7" s="24"/>
       <c r="J7" s="14">
         <v>1</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="31.2">
       <c r="E8" s="14">
         <v>2</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="34" t="s">
         <v>217</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="H8" s="24"/>
       <c r="J8" s="14">
         <v>2</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="31.2">
       <c r="E9" s="14">
         <v>3</v>
       </c>
-      <c r="F9" s="36" t="s">
-        <v>232</v>
+      <c r="F9" s="34" t="s">
+        <v>229</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="H9" s="24"/>
       <c r="J9" s="14">
         <v>3</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="31.2">
       <c r="E10" s="14">
         <v>4</v>
       </c>
-      <c r="F10" s="36" t="s">
-        <v>233</v>
+      <c r="F10" s="34" t="s">
+        <v>230</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="H10" s="24"/>
       <c r="J10" s="14">
         <v>4</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="31.2">
       <c r="E11" s="14">
         <v>5</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="34" t="s">
         <v>218</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="H11" s="24"/>
     </row>
@@ -5935,11 +5937,11 @@
       <c r="E12" s="14">
         <v>6</v>
       </c>
-      <c r="F12" s="36" t="s">
-        <v>234</v>
+      <c r="F12" s="34" t="s">
+        <v>231</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="H12" s="24"/>
     </row>
@@ -5971,8 +5973,8 @@
       <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:16" ht="25.8">
-      <c r="C17" s="37" t="s">
-        <v>226</v>
+      <c r="C17" s="35" t="s">
+        <v>223</v>
       </c>
       <c r="H17" s="24"/>
     </row>
@@ -5980,40 +5982,40 @@
       <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:16" ht="21">
-      <c r="D19" s="39" t="s">
+      <c r="D19" s="37" t="s">
         <v>212</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="24"/>
-      <c r="I19" s="39" t="s">
+      <c r="I19" s="37" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.6">
       <c r="D20" s="12"/>
-      <c r="E20" s="38" t="s">
+      <c r="E20" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="38" t="s">
+      <c r="F20" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="G20" s="38" t="s">
+      <c r="G20" s="36" t="s">
         <v>215</v>
       </c>
       <c r="H20" s="24"/>
-      <c r="J20" s="38" t="s">
+      <c r="J20" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="K20" s="38" t="s">
+      <c r="K20" s="36" t="s">
         <v>221</v>
       </c>
-      <c r="L20" s="38" t="s">
-        <v>261</v>
-      </c>
-      <c r="M20" s="38" t="s">
-        <v>277</v>
+      <c r="L20" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="M20" s="36" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="31.2">
@@ -6022,23 +6024,23 @@
         <v>1</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="H21" s="24"/>
       <c r="J21" s="5">
         <v>1</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="31.2">
@@ -6046,23 +6048,23 @@
         <v>2</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="H22" s="24"/>
       <c r="J22" s="5">
         <v>2</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="31.2">
@@ -6070,23 +6072,23 @@
         <v>3</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="H23" s="24"/>
       <c r="J23" s="5">
         <v>3</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="31.2">
@@ -6094,23 +6096,23 @@
         <v>4</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="H24" s="24"/>
       <c r="J24" s="5">
         <v>4</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.6">
@@ -6120,13 +6122,13 @@
         <v>5</v>
       </c>
       <c r="K25" s="14" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.6">
@@ -6158,8 +6160,8 @@
       <c r="H29" s="24"/>
     </row>
     <row r="30" spans="1:16" ht="25.8">
-      <c r="C30" s="40" t="s">
-        <v>227</v>
+      <c r="C30" s="38" t="s">
+        <v>224</v>
       </c>
       <c r="H30" s="24"/>
     </row>
@@ -6167,39 +6169,39 @@
       <c r="H31" s="24"/>
     </row>
     <row r="32" spans="1:16" ht="21">
-      <c r="D32" s="41" t="s">
+      <c r="D32" s="39" t="s">
         <v>212</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
       <c r="H32" s="24"/>
-      <c r="I32" s="43" t="s">
+      <c r="I32" s="41" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.6">
       <c r="D33" s="12"/>
-      <c r="E33" s="42" t="s">
+      <c r="E33" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="F33" s="42" t="s">
+      <c r="F33" s="40" t="s">
         <v>214</v>
       </c>
-      <c r="G33" s="42" t="s">
+      <c r="G33" s="40" t="s">
         <v>215</v>
       </c>
       <c r="H33" s="24"/>
-      <c r="J33" s="42" t="s">
+      <c r="J33" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="K33" s="42" t="s">
+      <c r="K33" s="40" t="s">
         <v>221</v>
       </c>
-      <c r="L33" s="42" t="s">
-        <v>304</v>
-      </c>
-      <c r="M33" s="42" t="s">
+      <c r="L33" s="40" t="s">
+        <v>291</v>
+      </c>
+      <c r="M33" s="40" t="s">
         <v>215</v>
       </c>
     </row>
@@ -6212,20 +6214,20 @@
         <v>216</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="H34" s="24"/>
       <c r="J34" s="14">
         <v>1</v>
       </c>
       <c r="K34" s="14" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.6">
@@ -6233,23 +6235,23 @@
         <v>2</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="H35" s="24"/>
       <c r="J35" s="14">
         <v>2</v>
       </c>
       <c r="K35" s="14" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.6">
@@ -6257,23 +6259,23 @@
         <v>3</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="H36" s="24"/>
       <c r="J36" s="14">
         <v>3</v>
       </c>
       <c r="K36" s="14" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.6">
@@ -6281,23 +6283,23 @@
         <v>4</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="H37" s="24"/>
       <c r="J37" s="14">
         <v>4</v>
       </c>
       <c r="K37" s="14" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.6">
@@ -6307,13 +6309,13 @@
         <v>5</v>
       </c>
       <c r="K38" s="14" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.6">
@@ -6345,7 +6347,7 @@
       <c r="H42" s="24"/>
     </row>
     <row r="43" spans="1:16" ht="25.8">
-      <c r="C43" s="45" t="s">
+      <c r="C43" s="43" t="s">
         <v>199</v>
       </c>
       <c r="H43" s="24"/>
@@ -6354,14 +6356,14 @@
       <c r="H44" s="24"/>
     </row>
     <row r="45" spans="1:16" ht="21">
-      <c r="D45" s="44" t="s">
+      <c r="D45" s="42" t="s">
         <v>212</v>
       </c>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
       <c r="H45" s="24"/>
-      <c r="I45" s="44" t="s">
+      <c r="I45" s="42" t="s">
         <v>220</v>
       </c>
     </row>
@@ -6384,10 +6386,10 @@
         <v>221</v>
       </c>
       <c r="L46" s="15" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="M46" s="15" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="31.2">
@@ -6396,23 +6398,23 @@
         <v>1</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="H47" s="24"/>
       <c r="J47" s="14">
         <v>1</v>
       </c>
       <c r="K47" s="14" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="31.2">
@@ -6420,23 +6422,23 @@
         <v>2</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="H48" s="24"/>
       <c r="J48" s="14">
         <v>2</v>
       </c>
       <c r="K48" s="14" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="31.2">
@@ -6444,23 +6446,23 @@
         <v>3</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="H49" s="24"/>
       <c r="J49" s="14">
         <v>3</v>
       </c>
       <c r="K49" s="14" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="31.2">
@@ -6468,23 +6470,23 @@
         <v>4</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="H50" s="24"/>
       <c r="J50" s="14">
         <v>4</v>
       </c>
       <c r="K50" s="14" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="31.2">
@@ -6494,13 +6496,13 @@
         <v>5</v>
       </c>
       <c r="K51" s="14" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="15.6">
@@ -6532,7 +6534,7 @@
       <c r="H55" s="24"/>
     </row>
     <row r="56" spans="1:16" ht="25.8">
-      <c r="C56" s="49" t="s">
+      <c r="C56" s="47" t="s">
         <v>200</v>
       </c>
       <c r="H56" s="24"/>
@@ -6541,39 +6543,39 @@
       <c r="H57" s="24"/>
     </row>
     <row r="58" spans="1:16" ht="21">
-      <c r="D58" s="48" t="s">
+      <c r="D58" s="46" t="s">
         <v>212</v>
       </c>
       <c r="E58" s="12"/>
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
       <c r="H58" s="24"/>
-      <c r="I58" s="47" t="s">
+      <c r="I58" s="45" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="59" spans="1:16" ht="15.6">
       <c r="D59" s="12"/>
-      <c r="E59" s="46" t="s">
+      <c r="E59" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="F59" s="46" t="s">
+      <c r="F59" s="44" t="s">
         <v>214</v>
       </c>
-      <c r="G59" s="46" t="s">
+      <c r="G59" s="44" t="s">
         <v>215</v>
       </c>
       <c r="H59" s="24"/>
-      <c r="J59" s="46" t="s">
+      <c r="J59" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="K59" s="46" t="s">
+      <c r="K59" s="44" t="s">
         <v>221</v>
       </c>
-      <c r="L59" s="46" t="s">
-        <v>304</v>
-      </c>
-      <c r="M59" s="46" t="s">
+      <c r="L59" s="44" t="s">
+        <v>291</v>
+      </c>
+      <c r="M59" s="44" t="s">
         <v>215</v>
       </c>
     </row>
@@ -6586,20 +6588,20 @@
         <v>217</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="H60" s="24"/>
       <c r="J60" s="14">
         <v>1</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
       <c r="L60" s="5" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
       <c r="M60" s="5" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
     </row>
     <row r="61" spans="1:16" ht="31.2">
@@ -6607,23 +6609,23 @@
         <v>2</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="H61" s="24"/>
       <c r="J61" s="14">
         <v>2</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="L61" s="5" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="M61" s="5" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
     </row>
     <row r="62" spans="1:16" ht="31.2">
@@ -6631,23 +6633,23 @@
         <v>3</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="H62" s="24"/>
       <c r="J62" s="14">
         <v>3</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="L62" s="5" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="M62" s="5" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="31.2">
@@ -6655,23 +6657,23 @@
         <v>4</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="H63" s="24"/>
       <c r="J63" s="14">
         <v>4</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="L63" s="5" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="M63" s="5" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
     </row>
     <row r="64" spans="1:16" ht="15.6" customHeight="1">
@@ -6706,7 +6708,7 @@
       <c r="H68" s="24"/>
     </row>
     <row r="69" spans="1:16" ht="25.8">
-      <c r="C69" s="50" t="s">
+      <c r="C69" s="48" t="s">
         <v>197</v>
       </c>
       <c r="H69" s="24"/>
@@ -6715,130 +6717,145 @@
       <c r="H70" s="24"/>
     </row>
     <row r="71" spans="1:16" ht="21">
-      <c r="D71" s="51" t="s">
+      <c r="D71" s="49" t="s">
         <v>212</v>
       </c>
       <c r="E71" s="12"/>
       <c r="F71" s="12"/>
       <c r="G71" s="12"/>
       <c r="H71" s="24"/>
-      <c r="I71" s="51" t="s">
+      <c r="I71" s="49" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="72" spans="1:16" ht="15.6">
       <c r="D72" s="12"/>
-      <c r="E72" s="12" t="s">
+      <c r="E72" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="F72" s="12" t="s">
+      <c r="F72" s="50" t="s">
         <v>214</v>
       </c>
-      <c r="G72" s="12" t="s">
+      <c r="G72" s="50" t="s">
         <v>215</v>
       </c>
       <c r="H72" s="24"/>
-      <c r="J72" s="12" t="s">
+      <c r="J72" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="K72" s="12" t="s">
+      <c r="K72" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="L72" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="M72" s="12" t="s">
-        <v>215</v>
+      <c r="L72" s="50" t="s">
+        <v>248</v>
+      </c>
+      <c r="M72" s="50" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="73" spans="1:16" ht="15.6">
       <c r="D73" s="12"/>
-      <c r="E73" s="12">
+      <c r="E73" s="14">
         <v>1</v>
       </c>
-      <c r="F73" s="12" t="s">
+      <c r="F73" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="G73" t="s">
+      <c r="G73" s="5" t="s">
         <v>219</v>
       </c>
       <c r="H73" s="24"/>
-      <c r="J73">
+      <c r="J73" s="14">
         <v>1</v>
       </c>
-      <c r="K73" t="s">
-        <v>223</v>
-      </c>
-      <c r="L73" t="s">
-        <v>224</v>
-      </c>
-      <c r="M73" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16">
-      <c r="E74">
+      <c r="K73" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="L73" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="M73" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" ht="31.2">
+      <c r="E74" s="14">
         <v>2</v>
       </c>
-      <c r="F74" t="s">
-        <v>243</v>
+      <c r="F74" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>343</v>
       </c>
       <c r="H74" s="24"/>
-      <c r="K74" t="s">
-        <v>246</v>
-      </c>
-      <c r="L74" s="32" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16">
-      <c r="E75">
+      <c r="J74" s="14">
+        <v>2</v>
+      </c>
+      <c r="K74" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="L74" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="M74" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" ht="31.2">
+      <c r="E75" s="14">
         <v>3</v>
       </c>
-      <c r="F75" t="s">
-        <v>244</v>
+      <c r="F75" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>344</v>
       </c>
       <c r="H75" s="24"/>
-      <c r="K75" t="s">
-        <v>247</v>
-      </c>
-      <c r="L75" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" ht="15.6">
-      <c r="E76" s="12">
+      <c r="J75" s="14">
+        <v>3</v>
+      </c>
+      <c r="K75" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="L75" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="M75" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" ht="31.2">
+      <c r="E76" s="14">
         <v>4</v>
       </c>
-      <c r="F76" t="s">
-        <v>245</v>
+      <c r="F76" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>345</v>
       </c>
       <c r="H76" s="24"/>
-      <c r="K76" t="s">
-        <v>248</v>
-      </c>
-      <c r="L76" t="s">
-        <v>253</v>
+      <c r="J76" s="14">
+        <v>4</v>
+      </c>
+      <c r="K76" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="L76" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="M76" s="5" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="77" spans="1:16" ht="15.6">
       <c r="E77" s="12"/>
       <c r="H77" s="24"/>
-      <c r="K77" t="s">
-        <v>249</v>
-      </c>
-      <c r="L77" t="s">
-        <v>252</v>
-      </c>
     </row>
     <row r="78" spans="1:16">
       <c r="H78" s="24"/>
-      <c r="K78" t="s">
-        <v>250</v>
-      </c>
-      <c r="L78" t="s">
-        <v>251</v>
-      </c>
     </row>
     <row r="79" spans="1:16">
       <c r="H79" s="24"/>

</xml_diff>